<commit_message>
Updated Burnup With backlog and scrumboard
Updated Burnup With backlog and scrumboard
</commit_message>
<xml_diff>
--- a/bookkeeping/Sprint1 BurnUp.xlsx
+++ b/bookkeeping/Sprint1 BurnUp.xlsx
@@ -9,13 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8430" yWindow="0" windowWidth="16410" windowHeight="7815"/>
+    <workbookView xWindow="9450" yWindow="0" windowWidth="16410" windowHeight="7815" tabRatio="601" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks List" sheetId="1" r:id="rId1"/>
-    <sheet name="Chart - Burn Up" sheetId="3" r:id="rId2"/>
-    <sheet name="Names-Hours" sheetId="2" r:id="rId3"/>
-    <sheet name="ToDo" sheetId="4" r:id="rId4"/>
+    <sheet name="Backlog" sheetId="5" r:id="rId2"/>
+    <sheet name="Scrum Board" sheetId="6" r:id="rId3"/>
+    <sheet name="Chart - Burn Up" sheetId="3" r:id="rId4"/>
+    <sheet name="Names-Hours" sheetId="2" r:id="rId5"/>
+    <sheet name="ToDo" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="87">
   <si>
     <t>Sprint 1</t>
   </si>
@@ -121,13 +123,181 @@
   </si>
   <si>
     <t>Started Bookkeeping folder and files</t>
+  </si>
+  <si>
+    <t>Diagram Processes of OSRA's processing of a Diagram</t>
+  </si>
+  <si>
+    <t>Generate/Compile Call Tree</t>
+  </si>
+  <si>
+    <t>Review call tree, and map to higher level processes</t>
+  </si>
+  <si>
+    <t>Identify locations for code insertion of other user stories</t>
+  </si>
+  <si>
+    <t>Code review Higher level processes from Processing Diagram</t>
+  </si>
+  <si>
+    <t>Identify external dependencies</t>
+  </si>
+  <si>
+    <t>Review O-Chem Chapter</t>
+  </si>
+  <si>
+    <t>Review Notes</t>
+  </si>
+  <si>
+    <t>Generate Cheat/Reference sheet for diagrams</t>
+  </si>
+  <si>
+    <t>O-Chem - to - SMILES</t>
+  </si>
+  <si>
+    <t>Organize structure of repo</t>
+  </si>
+  <si>
+    <t>Designate naming convention for branchs and code submition</t>
+  </si>
+  <si>
+    <t>Create and enforce workflow for pulls/pushes/merges</t>
+  </si>
+  <si>
+    <t>Create template for bug submissions</t>
+  </si>
+  <si>
+    <t>Create build/test server in windows</t>
+  </si>
+  <si>
+    <t>Create initial test cases</t>
+  </si>
+  <si>
+    <t>Create location for consolidated documentation</t>
+  </si>
+  <si>
+    <t>Create template for indevidual's documentation</t>
+  </si>
+  <si>
+    <t>Review .SD File contents</t>
+  </si>
+  <si>
+    <t>Review SMILES notation documentations</t>
+  </si>
+  <si>
+    <t>Create DB Schema</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>As a Developer, I need an architectural overview of OSRA’s processing, so I can understand the code base.</t>
+  </si>
+  <si>
+    <t>Identify locations for code insertion of other user stories in Process Diagram</t>
+  </si>
+  <si>
+    <t>As a Developer, I need to review each aspect of OSRA’s architecture, so I can understand the code base.</t>
+  </si>
+  <si>
+    <t>As a Developer, I need to get a basic grasp of O-Chem, so I can better understand use cases.</t>
+  </si>
+  <si>
+    <t>As a Developer, I need workflow and processes for the github repo, so I can collaborate on c</t>
+  </si>
+  <si>
+    <t>As a Developer, I need a testing enviroment and test documentation, so I can better contribu</t>
+  </si>
+  <si>
+    <t>As a Developer, I need to have consolidated documentation from other developers, so I can be</t>
+  </si>
+  <si>
+    <t>As a Developer, I need to understand SMILES notation and .SD file structure, so I can desing</t>
+  </si>
+  <si>
+    <t>As a User, I want to have a data structure for encoding polymers in “Smile Notation”, so I c</t>
+  </si>
+  <si>
+    <t>Create Development Workflow</t>
+  </si>
+  <si>
+    <t>Design DB Access Layer</t>
+  </si>
+  <si>
+    <t>Design Object Model</t>
+  </si>
+  <si>
+    <t>Backlog</t>
+  </si>
+  <si>
+    <t>As a Developer, I need workflow and processes for the github repo, so I can collaborate on code</t>
+  </si>
+  <si>
+    <t>As a Developer, I need a testing enviroment and test documentation, so I can better contribute to the codebase</t>
+  </si>
+  <si>
+    <t>As a Developer, I need to have consolidated documentation from other developers, so I can better contribute to the codebase</t>
+  </si>
+  <si>
+    <t>As a Developer, I need to understand SMILES notation and .SD file structure, so I can desing the smile data structure.</t>
+  </si>
+  <si>
+    <t>As a User, I want to be able to detect Par. in Chemical Diagram, so I can work with polymers</t>
+  </si>
+  <si>
+    <t>As a User, I want to be able to detect Brackets in Chemical Diagrams, so I can work with polymers</t>
+  </si>
+  <si>
+    <t>As a User, I want to be able to detect subscripts for polymer diagrams, so I can work with polymers</t>
+  </si>
+  <si>
+    <t>As a User, I want to be able to detect “R-Notation”, so I can work with polymers</t>
+  </si>
+  <si>
+    <t>As a User, I want to have a data structure for encoding polymers in “Smile Notation”, so I can work with polymers</t>
+  </si>
+  <si>
+    <t>As a User, I need an .SD files from the diagram for each sub molecule in the diagram, so I can work with polymers</t>
+  </si>
+  <si>
+    <t>User Stories</t>
+  </si>
+  <si>
+    <t>Assigned Sprint</t>
+  </si>
+  <si>
+    <t>INF</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Not Started</t>
+  </si>
+  <si>
+    <t>In Progrers</t>
+  </si>
+  <si>
+    <t>Finished</t>
+  </si>
+  <si>
+    <t>MoSCoW</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>W</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -157,12 +327,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
@@ -177,8 +341,41 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12.1"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="13.2"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -201,8 +398,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="30">
+  <borders count="63">
     <border>
       <left/>
       <right/>
@@ -211,43 +414,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thick">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -304,12 +470,629 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
         <color indexed="64"/>
       </left>
       <right/>
       <top/>
-      <bottom style="thin">
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -321,7 +1104,9 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -329,11 +1114,22 @@
     </border>
     <border>
       <left/>
-      <right style="thick">
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="thick">
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -345,246 +1141,90 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thick">
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="thick">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thick">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="thick">
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thick">
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="thick">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thick">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thick">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thick">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thick">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thick">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thick">
-        <color indexed="64"/>
-      </right>
-      <top style="thick">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thick">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thick">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color indexed="64"/>
-      </left>
-      <right style="thick">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thick">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thick">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color indexed="64"/>
-      </left>
-      <right style="thick">
-        <color indexed="64"/>
-      </right>
-      <top style="thick">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
       <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thick">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -594,9 +1234,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="144">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
@@ -609,84 +1249,37 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="2" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="2" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="4" borderId="8" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="4" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="4" borderId="17" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="4" borderId="16" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="4" borderId="23" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="4" borderId="15" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -696,68 +1289,386 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="30" xfId="2" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="31" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="1" fillId="4" borderId="33" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="4" borderId="30" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="4" borderId="34" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="4" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="24" xfId="2" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="25" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="5" borderId="27" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="5" borderId="24" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="5" borderId="28" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="5" borderId="25" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="30" xfId="2" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="31" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="5" borderId="33" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="5" borderId="30" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="5" borderId="34" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="5" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="4" borderId="12" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="4" borderId="11" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="4" borderId="37" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="4" borderId="10" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="2" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="5" borderId="12" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="5" borderId="11" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="5" borderId="37" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="5" borderId="10" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="61" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -880,7 +1791,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Tasks List'!$E$15</c:f>
+              <c:f>'Tasks List'!$E$81</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -946,7 +1857,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Tasks List'!$E$12:$K$12</c:f>
+              <c:f>'Tasks List'!$E$78:$K$78</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -981,7 +1892,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Tasks List'!$F$15</c:f>
+              <c:f>'Tasks List'!$F$81</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1047,30 +1958,30 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Tasks List'!$E$13:$K$13</c:f>
+              <c:f>'Tasks List'!$E$79:$K$79</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>162.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>162.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>162.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>162.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>162.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>162.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>162.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1082,7 +1993,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Tasks List'!$G$15</c:f>
+              <c:f>'Tasks List'!$G$81</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1151,7 +2062,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Tasks List'!$E$14:$K$14</c:f>
+              <c:f>'Tasks List'!$E$80:$K$80</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1159,7 +2070,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>162.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1191,11 +2102,11 @@
         </c:dropLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="343819928"/>
-        <c:axId val="343813264"/>
+        <c:axId val="318329224"/>
+        <c:axId val="318330792"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="343819928"/>
+        <c:axId val="318329224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1238,14 +2149,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="343813264"/>
+        <c:crossAx val="318330792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="343813264"/>
+        <c:axId val="318330792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1282,7 +2193,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="343819928"/>
+        <c:crossAx val="318329224"/>
         <c:crossesAt val="41548"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="10"/>
@@ -1314,7 +2225,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.60560733754434537"/>
+          <c:x val="0.59095532289233077"/>
           <c:y val="5.025313590717953E-2"/>
           <c:w val="0.36546750886908369"/>
           <c:h val="4.9226138714506387E-2"/>
@@ -1963,7 +2874,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -2261,50 +3172,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T34"/>
+  <dimension ref="A1:T100"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="5" ySplit="8" topLeftCell="F9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="R34" sqref="R34"/>
+      <selection pane="bottomRight" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="37.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47.42578125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="76.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" style="2" customWidth="1"/>
     <col min="5" max="5" width="11.28515625" style="2" hidden="1" customWidth="1"/>
     <col min="6" max="11" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="36" t="s">
+    <row r="1" spans="1:12" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="J1" s="29" t="s">
+      <c r="J1" s="17" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="33"/>
-      <c r="B2" s="34"/>
-      <c r="D2" s="32" t="s">
+    <row r="2" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="21"/>
+      <c r="B2" s="22"/>
+      <c r="D2" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="44" t="s">
+      <c r="F2" s="94" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="45"/>
-    </row>
-    <row r="3" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="30" t="s">
+      <c r="G2" s="95"/>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="18" t="s">
         <v>26</v>
       </c>
       <c r="D3" s="6" t="str">
@@ -2312,28 +3223,28 @@
         <v>Nicholas</v>
       </c>
       <c r="F3" s="7" t="str">
-        <f>'Names-Hours'!D3-('Names-Hours'!H3) - (SUMIF(C9:C10,D3,D9:D10))&amp;+"/"&amp;+'Names-Hours'!D3</f>
-        <v>30/30</v>
+        <f>('Names-Hours'!H3) - (SUMIF(C9:C76,D3,D9:D76))&amp;+"/"&amp;+'Names-Hours'!D3</f>
+        <v>-9/30</v>
       </c>
       <c r="G3" s="6" t="str">
         <f>'Names-Hours'!B5</f>
         <v>Igor</v>
       </c>
       <c r="H3" s="7" t="str">
-        <f>'Names-Hours'!D5-('Names-Hours'!H5) -(SUMIF(C9:C10,G3,D9:D10)) &amp;+"/"&amp;+'Names-Hours'!D5</f>
-        <v>30/30</v>
+        <f>('Names-Hours'!H3) -(SUMIF(C9:C76,G3,D9:D76)) &amp;+"/"&amp;+'Names-Hours'!D5</f>
+        <v>-3.5/30</v>
       </c>
       <c r="I3" s="6" t="str">
         <f>'Names-Hours'!B7</f>
-        <v>Nicholas</v>
+        <v>David</v>
       </c>
       <c r="J3" s="7" t="str">
-        <f>'Names-Hours'!D7-('Names-Hours'!H7) -(SUMIF(C9:C10,I3,D9:D10)) &amp;+"/"&amp;+ 'Names-Hours'!D7</f>
-        <v>30/30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="31" t="s">
+        <f>('Names-Hours'!H4) -(SUMIF(C9:C76,I3,D9:D76)) &amp;+"/"&amp;+ 'Names-Hours'!D7</f>
+        <v>0.5/30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="19" t="s">
         <v>27</v>
       </c>
       <c r="B4" s="5"/>
@@ -2342,280 +3253,1570 @@
         <v>Konstantin</v>
       </c>
       <c r="F4" s="7" t="str">
-        <f>'Names-Hours'!D4-('Names-Hours'!H4) -(SUMIF(C9:C10,D4,D9:D10))&amp;+"/"&amp;+'Names-Hours'!D4</f>
-        <v>30/30</v>
+        <f>('Names-Hours'!H4) -(SUMIF(C9:C76,D4,D9:D76))&amp;+"/"&amp;+'Names-Hours'!D4</f>
+        <v>-3/30</v>
       </c>
       <c r="G4" s="6" t="str">
         <f>'Names-Hours'!B6</f>
         <v>Nathan</v>
       </c>
       <c r="H4" s="7" t="str">
-        <f>'Names-Hours'!D6-('Names-Hours'!H6) -(SUMIF(C9:C10,G4,D9:D10)) &amp;+"/"&amp;+'Names-Hours'!D6</f>
-        <v>30/30</v>
+        <f>('Names-Hours'!H4) -(SUMIF(C9:C76,G4,D9:D76)) &amp;+"/"&amp;+'Names-Hours'!D6</f>
+        <v>-6.5/30</v>
       </c>
       <c r="I4" s="6" t="str">
         <f>'Names-Hours'!B8</f>
         <v>Thomas</v>
       </c>
       <c r="J4" s="7" t="str">
-        <f>'Names-Hours'!D8-('Names-Hours'!H8) -(SUMIF(C9:C10,I4,D9:D10)) &amp;+"/"&amp;+ 'Names-Hours'!D8</f>
-        <v>30/30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <f>('Names-Hours'!H4) -(SUMIF(C9:C76,I4,D9:D76)) &amp;+"/"&amp;+ 'Names-Hours'!D8</f>
+        <v>0/30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="9"/>
-      <c r="D5" s="37" t="s">
+      <c r="D5" s="25" t="s">
         <v>21</v>
       </c>
       <c r="E5" s="8"/>
-      <c r="F5" s="38">
+      <c r="F5" s="26">
         <v>2</v>
       </c>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
     </row>
-    <row r="6" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:20" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="50" t="s">
+    <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:12" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="100" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="50" t="s">
+      <c r="B7" s="100" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="46" t="s">
+      <c r="C7" s="96" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="48" t="s">
+      <c r="D7" s="98" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="39"/>
-      <c r="F7" s="52" t="s">
+      <c r="E7" s="27"/>
+      <c r="F7" s="102" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="53"/>
-      <c r="H7" s="53"/>
-      <c r="I7" s="53"/>
-      <c r="J7" s="53"/>
-      <c r="K7" s="54"/>
-      <c r="L7" s="28"/>
-    </row>
-    <row r="8" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="51"/>
-      <c r="B8" s="51"/>
-      <c r="C8" s="47"/>
-      <c r="D8" s="49"/>
+      <c r="G7" s="103"/>
+      <c r="H7" s="103"/>
+      <c r="I7" s="103"/>
+      <c r="J7" s="103"/>
+      <c r="K7" s="104"/>
+      <c r="L7" s="16"/>
+    </row>
+    <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="101"/>
+      <c r="B8" s="101"/>
+      <c r="C8" s="97"/>
+      <c r="D8" s="99"/>
       <c r="E8" s="10">
         <v>41661</v>
       </c>
-      <c r="F8" s="40">
+      <c r="F8" s="28">
         <v>41663</v>
       </c>
-      <c r="G8" s="41">
+      <c r="G8" s="29">
         <v>41666</v>
       </c>
-      <c r="H8" s="41">
+      <c r="H8" s="29">
         <v>41668</v>
       </c>
-      <c r="I8" s="41">
+      <c r="I8" s="29">
         <v>41670</v>
       </c>
-      <c r="J8" s="41">
+      <c r="J8" s="29">
         <v>41673</v>
       </c>
-      <c r="K8" s="41">
+      <c r="K8" s="68">
         <v>41675</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="24.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="42"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="21"/>
-      <c r="K9" s="22"/>
-    </row>
-    <row r="10" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="43"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="26"/>
-      <c r="J10" s="26"/>
-      <c r="K10" s="27"/>
-    </row>
-    <row r="11" spans="1:20" ht="16.149999999999999" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D11" s="11">
-        <f>SUM(D9:D10)</f>
+    <row r="9" spans="1:12" ht="16.149999999999999" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="93" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="38">
+        <v>1.5</v>
+      </c>
+      <c r="E9" s="39"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="42"/>
+      <c r="J9" s="42"/>
+      <c r="K9" s="43"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="91"/>
+      <c r="B10" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="31">
+        <v>1.5</v>
+      </c>
+      <c r="E10" s="45"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="34"/>
+      <c r="J10" s="34"/>
+      <c r="K10" s="35"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="91"/>
+      <c r="B11" s="46" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="48">
+        <v>4</v>
+      </c>
+      <c r="E11" s="49"/>
+      <c r="F11" s="50"/>
+      <c r="G11" s="51"/>
+      <c r="H11" s="51"/>
+      <c r="I11" s="52"/>
+      <c r="J11" s="52"/>
+      <c r="K11" s="53"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="91"/>
+      <c r="B12" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="31">
+        <v>4</v>
+      </c>
+      <c r="E12" s="45"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="33"/>
+      <c r="I12" s="34"/>
+      <c r="J12" s="34"/>
+      <c r="K12" s="35"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="91"/>
+      <c r="B13" s="46" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="47" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="48">
+        <v>3</v>
+      </c>
+      <c r="E13" s="49"/>
+      <c r="F13" s="50"/>
+      <c r="G13" s="51"/>
+      <c r="H13" s="51"/>
+      <c r="I13" s="52"/>
+      <c r="J13" s="52"/>
+      <c r="K13" s="53"/>
+    </row>
+    <row r="14" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="92"/>
+      <c r="B14" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="15">
+        <v>5</v>
+      </c>
+      <c r="E14" s="55"/>
+      <c r="F14" s="56"/>
+      <c r="G14" s="57"/>
+      <c r="H14" s="57"/>
+      <c r="I14" s="58"/>
+      <c r="J14" s="58"/>
+      <c r="K14" s="59"/>
+    </row>
+    <row r="15" spans="1:12" ht="15.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="91" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" s="48">
+        <v>8</v>
+      </c>
+      <c r="E15" s="49"/>
+      <c r="F15" s="50"/>
+      <c r="G15" s="51"/>
+      <c r="H15" s="51"/>
+      <c r="I15" s="52"/>
+      <c r="J15" s="52"/>
+      <c r="K15" s="53"/>
+    </row>
+    <row r="16" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="91"/>
+      <c r="B16" s="44" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="31">
+        <v>8</v>
+      </c>
+      <c r="E16" s="45"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="34"/>
+      <c r="J16" s="34"/>
+      <c r="K16" s="35"/>
+    </row>
+    <row r="17" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="91"/>
+      <c r="B17" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="47" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" s="48">
+        <v>8</v>
+      </c>
+      <c r="E17" s="49"/>
+      <c r="F17" s="50"/>
+      <c r="G17" s="51"/>
+      <c r="H17" s="51"/>
+      <c r="I17" s="52"/>
+      <c r="J17" s="52"/>
+      <c r="K17" s="53"/>
+    </row>
+    <row r="18" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="91"/>
+      <c r="B18" s="44" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="31">
+        <v>8</v>
+      </c>
+      <c r="E18" s="45"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="34"/>
+      <c r="J18" s="34"/>
+      <c r="K18" s="35"/>
+    </row>
+    <row r="19" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="91"/>
+      <c r="B19" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="47" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" s="48">
+        <v>8</v>
+      </c>
+      <c r="E19" s="49"/>
+      <c r="F19" s="50"/>
+      <c r="G19" s="51"/>
+      <c r="H19" s="51"/>
+      <c r="I19" s="52"/>
+      <c r="J19" s="52"/>
+      <c r="K19" s="53"/>
+    </row>
+    <row r="20" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="91"/>
+      <c r="B20" s="44" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="31">
+        <v>8</v>
+      </c>
+      <c r="E20" s="45"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="33"/>
+      <c r="H20" s="33"/>
+      <c r="I20" s="34"/>
+      <c r="J20" s="34"/>
+      <c r="K20" s="35"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="91"/>
+      <c r="B21" s="46" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="48">
+        <v>6.5</v>
+      </c>
+      <c r="E21" s="49"/>
+      <c r="F21" s="50"/>
+      <c r="G21" s="51"/>
+      <c r="H21" s="51"/>
+      <c r="I21" s="52"/>
+      <c r="J21" s="52"/>
+      <c r="K21" s="53"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="91"/>
+      <c r="B22" s="44" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="31">
+        <v>6.5</v>
+      </c>
+      <c r="E22" s="45"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="33"/>
+      <c r="H22" s="33"/>
+      <c r="I22" s="34"/>
+      <c r="J22" s="34"/>
+      <c r="K22" s="35"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="91"/>
+      <c r="B23" s="46" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" s="48">
+        <v>3</v>
+      </c>
+      <c r="E23" s="49"/>
+      <c r="F23" s="50"/>
+      <c r="G23" s="51"/>
+      <c r="H23" s="51"/>
+      <c r="I23" s="52"/>
+      <c r="J23" s="52"/>
+      <c r="K23" s="53"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="91"/>
+      <c r="B24" s="44" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" s="31">
+        <v>3</v>
+      </c>
+      <c r="E24" s="45"/>
+      <c r="F24" s="32"/>
+      <c r="G24" s="33"/>
+      <c r="H24" s="33"/>
+      <c r="I24" s="34"/>
+      <c r="J24" s="34"/>
+      <c r="K24" s="35"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="91"/>
+      <c r="B25" s="46" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="47" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" s="48">
+        <v>3</v>
+      </c>
+      <c r="E25" s="49"/>
+      <c r="F25" s="50"/>
+      <c r="G25" s="51"/>
+      <c r="H25" s="51"/>
+      <c r="I25" s="52"/>
+      <c r="J25" s="52"/>
+      <c r="K25" s="53"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="91"/>
+      <c r="B26" s="44" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="D26" s="31">
+        <v>3</v>
+      </c>
+      <c r="E26" s="45"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="33"/>
+      <c r="H26" s="33"/>
+      <c r="I26" s="34"/>
+      <c r="J26" s="34"/>
+      <c r="K26" s="35"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="91"/>
+      <c r="B27" s="46" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" s="47" t="s">
+        <v>52</v>
+      </c>
+      <c r="D27" s="48">
+        <v>3</v>
+      </c>
+      <c r="E27" s="49"/>
+      <c r="F27" s="50"/>
+      <c r="G27" s="51"/>
+      <c r="H27" s="51"/>
+      <c r="I27" s="52"/>
+      <c r="J27" s="52"/>
+      <c r="K27" s="53"/>
+    </row>
+    <row r="28" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="92"/>
+      <c r="B28" s="54" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D28" s="15">
+        <v>3</v>
+      </c>
+      <c r="E28" s="55"/>
+      <c r="F28" s="56"/>
+      <c r="G28" s="57"/>
+      <c r="H28" s="57"/>
+      <c r="I28" s="58"/>
+      <c r="J28" s="58"/>
+      <c r="K28" s="59"/>
+    </row>
+    <row r="29" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="91" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" s="46" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="D29" s="48">
+        <v>3</v>
+      </c>
+      <c r="E29" s="49"/>
+      <c r="F29" s="50"/>
+      <c r="G29" s="51"/>
+      <c r="H29" s="51"/>
+      <c r="I29" s="52"/>
+      <c r="J29" s="52"/>
+      <c r="K29" s="53"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="91"/>
+      <c r="B30" s="44" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="D30" s="31">
+        <v>3</v>
+      </c>
+      <c r="E30" s="45"/>
+      <c r="F30" s="32"/>
+      <c r="G30" s="33"/>
+      <c r="H30" s="33"/>
+      <c r="I30" s="34"/>
+      <c r="J30" s="34"/>
+      <c r="K30" s="35"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="91"/>
+      <c r="B31" s="46" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" s="47" t="s">
+        <v>23</v>
+      </c>
+      <c r="D31" s="48">
+        <v>3</v>
+      </c>
+      <c r="E31" s="49"/>
+      <c r="F31" s="50"/>
+      <c r="G31" s="51"/>
+      <c r="H31" s="51"/>
+      <c r="I31" s="52"/>
+      <c r="J31" s="52"/>
+      <c r="K31" s="53"/>
+    </row>
+    <row r="32" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="91"/>
+      <c r="B32" s="44" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="D32" s="31">
+        <v>3</v>
+      </c>
+      <c r="E32" s="45"/>
+      <c r="F32" s="32"/>
+      <c r="G32" s="33"/>
+      <c r="H32" s="33"/>
+      <c r="I32" s="34"/>
+      <c r="J32" s="34"/>
+      <c r="K32" s="35"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="91"/>
+      <c r="B33" s="46" t="s">
+        <v>37</v>
+      </c>
+      <c r="C33" s="47" t="s">
+        <v>52</v>
+      </c>
+      <c r="D33" s="48">
+        <v>3</v>
+      </c>
+      <c r="E33" s="49"/>
+      <c r="F33" s="50"/>
+      <c r="G33" s="51"/>
+      <c r="H33" s="51"/>
+      <c r="I33" s="52"/>
+      <c r="J33" s="52"/>
+      <c r="K33" s="53"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="91"/>
+      <c r="B34" s="44" t="s">
+        <v>37</v>
+      </c>
+      <c r="C34" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="D34" s="31">
+        <v>3</v>
+      </c>
+      <c r="E34" s="45"/>
+      <c r="F34" s="32"/>
+      <c r="G34" s="33"/>
+      <c r="H34" s="33"/>
+      <c r="I34" s="34"/>
+      <c r="J34" s="34"/>
+      <c r="K34" s="35"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="91"/>
+      <c r="B35" s="46" t="s">
+        <v>38</v>
+      </c>
+      <c r="C35" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="D35" s="48">
+        <v>2</v>
+      </c>
+      <c r="E35" s="49"/>
+      <c r="F35" s="50"/>
+      <c r="G35" s="51"/>
+      <c r="H35" s="51"/>
+      <c r="I35" s="52"/>
+      <c r="J35" s="52"/>
+      <c r="K35" s="53"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="91"/>
+      <c r="B36" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="C36" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="D36" s="31">
+        <v>2</v>
+      </c>
+      <c r="E36" s="45"/>
+      <c r="F36" s="32"/>
+      <c r="G36" s="33"/>
+      <c r="H36" s="33"/>
+      <c r="I36" s="34"/>
+      <c r="J36" s="34"/>
+      <c r="K36" s="35"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="91"/>
+      <c r="B37" s="46" t="s">
+        <v>38</v>
+      </c>
+      <c r="C37" s="47" t="s">
+        <v>23</v>
+      </c>
+      <c r="D37" s="48">
+        <v>2</v>
+      </c>
+      <c r="E37" s="49"/>
+      <c r="F37" s="50"/>
+      <c r="G37" s="51"/>
+      <c r="H37" s="51"/>
+      <c r="I37" s="52"/>
+      <c r="J37" s="52"/>
+      <c r="K37" s="53"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="91"/>
+      <c r="B38" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="C38" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="D38" s="31">
+        <v>2</v>
+      </c>
+      <c r="E38" s="45"/>
+      <c r="F38" s="32"/>
+      <c r="G38" s="33"/>
+      <c r="H38" s="33"/>
+      <c r="I38" s="34"/>
+      <c r="J38" s="34"/>
+      <c r="K38" s="35"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="91"/>
+      <c r="B39" s="46" t="s">
+        <v>38</v>
+      </c>
+      <c r="C39" s="47" t="s">
+        <v>52</v>
+      </c>
+      <c r="D39" s="48">
+        <v>2</v>
+      </c>
+      <c r="E39" s="49"/>
+      <c r="F39" s="50"/>
+      <c r="G39" s="51"/>
+      <c r="H39" s="51"/>
+      <c r="I39" s="52"/>
+      <c r="J39" s="52"/>
+      <c r="K39" s="53"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="91"/>
+      <c r="B40" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="C40" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="D40" s="31">
+        <v>2</v>
+      </c>
+      <c r="E40" s="45"/>
+      <c r="F40" s="32"/>
+      <c r="G40" s="33"/>
+      <c r="H40" s="33"/>
+      <c r="I40" s="34"/>
+      <c r="J40" s="34"/>
+      <c r="K40" s="35"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="91"/>
+      <c r="B41" s="46" t="s">
+        <v>39</v>
+      </c>
+      <c r="C41" s="47" t="s">
+        <v>52</v>
+      </c>
+      <c r="D41" s="48">
+        <v>2.5</v>
+      </c>
+      <c r="E41" s="49"/>
+      <c r="F41" s="50"/>
+      <c r="G41" s="51"/>
+      <c r="H41" s="51"/>
+      <c r="I41" s="52"/>
+      <c r="J41" s="52"/>
+      <c r="K41" s="53"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="91"/>
+      <c r="B42" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="C42" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="D42" s="31">
+        <v>2.5</v>
+      </c>
+      <c r="E42" s="45"/>
+      <c r="F42" s="32"/>
+      <c r="G42" s="33"/>
+      <c r="H42" s="33"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="34"/>
+      <c r="K42" s="35"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="91"/>
+      <c r="B43" s="46" t="s">
+        <v>40</v>
+      </c>
+      <c r="C43" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="D43" s="48">
+        <v>0.5</v>
+      </c>
+      <c r="E43" s="49"/>
+      <c r="F43" s="50"/>
+      <c r="G43" s="51"/>
+      <c r="H43" s="51"/>
+      <c r="I43" s="52"/>
+      <c r="J43" s="52"/>
+      <c r="K43" s="53"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="91"/>
+      <c r="B44" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="C44" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="D44" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="E44" s="45"/>
+      <c r="F44" s="32"/>
+      <c r="G44" s="33"/>
+      <c r="H44" s="33"/>
+      <c r="I44" s="34"/>
+      <c r="J44" s="34"/>
+      <c r="K44" s="35"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="91"/>
+      <c r="B45" s="46" t="s">
+        <v>40</v>
+      </c>
+      <c r="C45" s="47" t="s">
+        <v>23</v>
+      </c>
+      <c r="D45" s="48">
+        <v>0.5</v>
+      </c>
+      <c r="E45" s="49"/>
+      <c r="F45" s="50"/>
+      <c r="G45" s="51"/>
+      <c r="H45" s="51"/>
+      <c r="I45" s="52"/>
+      <c r="J45" s="52"/>
+      <c r="K45" s="53"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="91"/>
+      <c r="B46" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="C46" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="D46" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="E46" s="45"/>
+      <c r="F46" s="32"/>
+      <c r="G46" s="33"/>
+      <c r="H46" s="33"/>
+      <c r="I46" s="34"/>
+      <c r="J46" s="34"/>
+      <c r="K46" s="35"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="91"/>
+      <c r="B47" s="46" t="s">
+        <v>40</v>
+      </c>
+      <c r="C47" s="47" t="s">
+        <v>52</v>
+      </c>
+      <c r="D47" s="48">
+        <v>0.5</v>
+      </c>
+      <c r="E47" s="49"/>
+      <c r="F47" s="50"/>
+      <c r="G47" s="51"/>
+      <c r="H47" s="51"/>
+      <c r="I47" s="52"/>
+      <c r="J47" s="52"/>
+      <c r="K47" s="53"/>
+    </row>
+    <row r="48" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="92"/>
+      <c r="B48" s="54" t="s">
+        <v>40</v>
+      </c>
+      <c r="C48" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D48" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="E48" s="55"/>
+      <c r="F48" s="56"/>
+      <c r="G48" s="57"/>
+      <c r="H48" s="57"/>
+      <c r="I48" s="58"/>
+      <c r="J48" s="58"/>
+      <c r="K48" s="59"/>
+    </row>
+    <row r="49" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="91" t="s">
+        <v>57</v>
+      </c>
+      <c r="B49" s="46" t="s">
+        <v>41</v>
+      </c>
+      <c r="C49" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="D49" s="48">
+        <v>0.5</v>
+      </c>
+      <c r="E49" s="49"/>
+      <c r="F49" s="50"/>
+      <c r="G49" s="51"/>
+      <c r="H49" s="51"/>
+      <c r="I49" s="52"/>
+      <c r="J49" s="52"/>
+      <c r="K49" s="53"/>
+    </row>
+    <row r="50" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="91"/>
+      <c r="B50" s="44" t="s">
+        <v>42</v>
+      </c>
+      <c r="C50" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="D50" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="E50" s="45"/>
+      <c r="F50" s="32"/>
+      <c r="G50" s="33"/>
+      <c r="H50" s="33"/>
+      <c r="I50" s="34"/>
+      <c r="J50" s="34"/>
+      <c r="K50" s="35"/>
+    </row>
+    <row r="51" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="92"/>
+      <c r="B51" s="60" t="s">
+        <v>43</v>
+      </c>
+      <c r="C51" s="61" t="s">
+        <v>22</v>
+      </c>
+      <c r="D51" s="62">
+        <v>0.5</v>
+      </c>
+      <c r="E51" s="63"/>
+      <c r="F51" s="64"/>
+      <c r="G51" s="65"/>
+      <c r="H51" s="65"/>
+      <c r="I51" s="66"/>
+      <c r="J51" s="66"/>
+      <c r="K51" s="67"/>
+    </row>
+    <row r="52" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="91" t="s">
+        <v>58</v>
+      </c>
+      <c r="B52" s="44" t="s">
+        <v>44</v>
+      </c>
+      <c r="C52" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="D52" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="E52" s="45"/>
+      <c r="F52" s="32"/>
+      <c r="G52" s="33"/>
+      <c r="H52" s="33"/>
+      <c r="I52" s="34"/>
+      <c r="J52" s="34"/>
+      <c r="K52" s="35"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53" s="91"/>
+      <c r="B53" s="46" t="s">
+        <v>45</v>
+      </c>
+      <c r="C53" s="47" t="s">
+        <v>23</v>
+      </c>
+      <c r="D53" s="48">
+        <v>5</v>
+      </c>
+      <c r="E53" s="49"/>
+      <c r="F53" s="50"/>
+      <c r="G53" s="51"/>
+      <c r="H53" s="51"/>
+      <c r="I53" s="52"/>
+      <c r="J53" s="52"/>
+      <c r="K53" s="53"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" s="91"/>
+      <c r="B54" s="44" t="s">
+        <v>46</v>
+      </c>
+      <c r="C54" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="D54" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="E54" s="45"/>
+      <c r="F54" s="32"/>
+      <c r="G54" s="33"/>
+      <c r="H54" s="33"/>
+      <c r="I54" s="34"/>
+      <c r="J54" s="34"/>
+      <c r="K54" s="35"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55" s="91"/>
+      <c r="B55" s="46" t="s">
+        <v>62</v>
+      </c>
+      <c r="C55" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="D55" s="48">
+        <v>1</v>
+      </c>
+      <c r="E55" s="49"/>
+      <c r="F55" s="50"/>
+      <c r="G55" s="51"/>
+      <c r="H55" s="51"/>
+      <c r="I55" s="52"/>
+      <c r="J55" s="52"/>
+      <c r="K55" s="53"/>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A56" s="91"/>
+      <c r="B56" s="44" t="s">
+        <v>62</v>
+      </c>
+      <c r="C56" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="D56" s="31">
+        <v>1</v>
+      </c>
+      <c r="E56" s="45"/>
+      <c r="F56" s="32"/>
+      <c r="G56" s="33"/>
+      <c r="H56" s="33"/>
+      <c r="I56" s="34"/>
+      <c r="J56" s="34"/>
+      <c r="K56" s="35"/>
+    </row>
+    <row r="57" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="92"/>
+      <c r="B57" s="60" t="s">
+        <v>62</v>
+      </c>
+      <c r="C57" s="61" t="s">
+        <v>23</v>
+      </c>
+      <c r="D57" s="62">
+        <v>1</v>
+      </c>
+      <c r="E57" s="63"/>
+      <c r="F57" s="64"/>
+      <c r="G57" s="65"/>
+      <c r="H57" s="65"/>
+      <c r="I57" s="66"/>
+      <c r="J57" s="66"/>
+      <c r="K57" s="67"/>
+    </row>
+    <row r="58" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="91" t="s">
+        <v>59</v>
+      </c>
+      <c r="B58" s="44" t="s">
+        <v>47</v>
+      </c>
+      <c r="C58" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="D58" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="E58" s="45"/>
+      <c r="F58" s="32"/>
+      <c r="G58" s="33"/>
+      <c r="H58" s="33"/>
+      <c r="I58" s="34"/>
+      <c r="J58" s="34"/>
+      <c r="K58" s="35"/>
+    </row>
+    <row r="59" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="92"/>
+      <c r="B59" s="60" t="s">
+        <v>48</v>
+      </c>
+      <c r="C59" s="61" t="s">
+        <v>24</v>
+      </c>
+      <c r="D59" s="62">
+        <v>0.5</v>
+      </c>
+      <c r="E59" s="63"/>
+      <c r="F59" s="64"/>
+      <c r="G59" s="65"/>
+      <c r="H59" s="65"/>
+      <c r="I59" s="66"/>
+      <c r="J59" s="66"/>
+      <c r="K59" s="67"/>
+    </row>
+    <row r="60" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="91" t="s">
+        <v>60</v>
+      </c>
+      <c r="B60" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="C60" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="D60" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="E60" s="45"/>
+      <c r="F60" s="32"/>
+      <c r="G60" s="33"/>
+      <c r="H60" s="33"/>
+      <c r="I60" s="34"/>
+      <c r="J60" s="34"/>
+      <c r="K60" s="35"/>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A61" s="91"/>
+      <c r="B61" s="46" t="s">
+        <v>49</v>
+      </c>
+      <c r="C61" s="47" t="s">
+        <v>25</v>
+      </c>
+      <c r="D61" s="48">
+        <v>0.5</v>
+      </c>
+      <c r="E61" s="49"/>
+      <c r="F61" s="50"/>
+      <c r="G61" s="51"/>
+      <c r="H61" s="51"/>
+      <c r="I61" s="52"/>
+      <c r="J61" s="52"/>
+      <c r="K61" s="53"/>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A62" s="91"/>
+      <c r="B62" s="44" t="s">
+        <v>50</v>
+      </c>
+      <c r="C62" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="D62" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="E62" s="45"/>
+      <c r="F62" s="32"/>
+      <c r="G62" s="33"/>
+      <c r="H62" s="33"/>
+      <c r="I62" s="34"/>
+      <c r="J62" s="34"/>
+      <c r="K62" s="35"/>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A63" s="91"/>
+      <c r="B63" s="46" t="s">
+        <v>50</v>
+      </c>
+      <c r="C63" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="D63" s="48">
+        <v>0.5</v>
+      </c>
+      <c r="E63" s="49"/>
+      <c r="F63" s="50"/>
+      <c r="G63" s="51"/>
+      <c r="H63" s="51"/>
+      <c r="I63" s="52"/>
+      <c r="J63" s="52"/>
+      <c r="K63" s="53"/>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A64" s="91"/>
+      <c r="B64" s="44" t="s">
+        <v>50</v>
+      </c>
+      <c r="C64" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="D64" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="E64" s="45"/>
+      <c r="F64" s="32"/>
+      <c r="G64" s="33"/>
+      <c r="H64" s="33"/>
+      <c r="I64" s="34"/>
+      <c r="J64" s="34"/>
+      <c r="K64" s="35"/>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A65" s="91"/>
+      <c r="B65" s="46" t="s">
+        <v>50</v>
+      </c>
+      <c r="C65" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="D65" s="48">
+        <v>0.5</v>
+      </c>
+      <c r="E65" s="49"/>
+      <c r="F65" s="50"/>
+      <c r="G65" s="51"/>
+      <c r="H65" s="51"/>
+      <c r="I65" s="52"/>
+      <c r="J65" s="52"/>
+      <c r="K65" s="53"/>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A66" s="91"/>
+      <c r="B66" s="44" t="s">
+        <v>50</v>
+      </c>
+      <c r="C66" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="D66" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="E66" s="45"/>
+      <c r="F66" s="32"/>
+      <c r="G66" s="33"/>
+      <c r="H66" s="33"/>
+      <c r="I66" s="34"/>
+      <c r="J66" s="34"/>
+      <c r="K66" s="35"/>
+    </row>
+    <row r="67" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="92"/>
+      <c r="B67" s="60" t="s">
+        <v>50</v>
+      </c>
+      <c r="C67" s="61" t="s">
+        <v>25</v>
+      </c>
+      <c r="D67" s="62">
+        <v>0.5</v>
+      </c>
+      <c r="E67" s="63"/>
+      <c r="F67" s="64"/>
+      <c r="G67" s="65"/>
+      <c r="H67" s="65"/>
+      <c r="I67" s="66"/>
+      <c r="J67" s="66"/>
+      <c r="K67" s="67"/>
+    </row>
+    <row r="68" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="91" t="s">
+        <v>61</v>
+      </c>
+      <c r="B68" s="44" t="s">
+        <v>51</v>
+      </c>
+      <c r="C68" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="D68" s="31">
+        <v>2</v>
+      </c>
+      <c r="E68" s="45"/>
+      <c r="F68" s="32"/>
+      <c r="G68" s="33"/>
+      <c r="H68" s="33"/>
+      <c r="I68" s="34"/>
+      <c r="J68" s="34"/>
+      <c r="K68" s="35"/>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A69" s="91"/>
+      <c r="B69" s="46" t="s">
+        <v>51</v>
+      </c>
+      <c r="C69" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="D69" s="48">
+        <v>2</v>
+      </c>
+      <c r="E69" s="49"/>
+      <c r="F69" s="50"/>
+      <c r="G69" s="51"/>
+      <c r="H69" s="51"/>
+      <c r="I69" s="52"/>
+      <c r="J69" s="52"/>
+      <c r="K69" s="53"/>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A70" s="91"/>
+      <c r="B70" s="44" t="s">
+        <v>51</v>
+      </c>
+      <c r="C70" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="D70" s="31">
+        <v>1</v>
+      </c>
+      <c r="E70" s="45"/>
+      <c r="F70" s="32"/>
+      <c r="G70" s="33"/>
+      <c r="H70" s="33"/>
+      <c r="I70" s="34"/>
+      <c r="J70" s="34"/>
+      <c r="K70" s="35"/>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A71" s="91"/>
+      <c r="B71" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="C71" s="47" t="s">
+        <v>25</v>
+      </c>
+      <c r="D71" s="48">
+        <v>1</v>
+      </c>
+      <c r="E71" s="49"/>
+      <c r="F71" s="50"/>
+      <c r="G71" s="51"/>
+      <c r="H71" s="51"/>
+      <c r="I71" s="52"/>
+      <c r="J71" s="52"/>
+      <c r="K71" s="53"/>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A72" s="91"/>
+      <c r="B72" s="44" t="s">
+        <v>63</v>
+      </c>
+      <c r="C72" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="D72" s="31">
+        <v>1</v>
+      </c>
+      <c r="E72" s="45"/>
+      <c r="F72" s="32"/>
+      <c r="G72" s="33"/>
+      <c r="H72" s="33"/>
+      <c r="I72" s="34"/>
+      <c r="J72" s="34"/>
+      <c r="K72" s="35"/>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A73" s="91"/>
+      <c r="B73" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="C73" s="47" t="s">
+        <v>23</v>
+      </c>
+      <c r="D73" s="48">
+        <v>1</v>
+      </c>
+      <c r="E73" s="49"/>
+      <c r="F73" s="50"/>
+      <c r="G73" s="51"/>
+      <c r="H73" s="51"/>
+      <c r="I73" s="52"/>
+      <c r="J73" s="52"/>
+      <c r="K73" s="53"/>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A74" s="91"/>
+      <c r="B74" s="44" t="s">
+        <v>64</v>
+      </c>
+      <c r="C74" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="D74" s="31">
+        <v>1</v>
+      </c>
+      <c r="E74" s="45"/>
+      <c r="F74" s="32"/>
+      <c r="G74" s="33"/>
+      <c r="H74" s="33"/>
+      <c r="I74" s="34"/>
+      <c r="J74" s="34"/>
+      <c r="K74" s="35"/>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A75" s="91"/>
+      <c r="B75" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="C75" s="47" t="s">
+        <v>23</v>
+      </c>
+      <c r="D75" s="48">
+        <v>1</v>
+      </c>
+      <c r="E75" s="49"/>
+      <c r="F75" s="50"/>
+      <c r="G75" s="51"/>
+      <c r="H75" s="51"/>
+      <c r="I75" s="52"/>
+      <c r="J75" s="52"/>
+      <c r="K75" s="53"/>
+    </row>
+    <row r="76" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="92"/>
+      <c r="B76" s="54" t="s">
+        <v>64</v>
+      </c>
+      <c r="C76" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D76" s="15">
+        <v>1</v>
+      </c>
+      <c r="E76" s="55"/>
+      <c r="F76" s="56"/>
+      <c r="G76" s="57"/>
+      <c r="H76" s="57"/>
+      <c r="I76" s="58"/>
+      <c r="J76" s="58"/>
+      <c r="K76" s="59"/>
+    </row>
+    <row r="77" spans="1:12" ht="16.149999999999999" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D77" s="11">
+        <f>SUM(D9:D76)</f>
+        <v>162.5</v>
+      </c>
+      <c r="E77" s="12" t="str">
+        <f>E78&amp;+ "/" &amp;+ $D$77</f>
+        <v>0/162.5</v>
+      </c>
+      <c r="F77" s="12" t="str">
+        <f>F78&amp;+ "/" &amp;+ $D$77</f>
+        <v>0/162.5</v>
+      </c>
+      <c r="G77" s="12" t="str">
+        <f t="shared" ref="G77:K77" si="0">G78&amp;+ "/" &amp;+ $D$77</f>
+        <v>0/162.5</v>
+      </c>
+      <c r="H77" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>0/162.5</v>
+      </c>
+      <c r="I77" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>0/162.5</v>
+      </c>
+      <c r="J77" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>0/162.5</v>
+      </c>
+      <c r="K77" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>0/162.5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" ht="15" hidden="1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="D78" s="1">
+        <f>SUM(D9:D76)</f>
+        <v>162.5</v>
+      </c>
+      <c r="E78" s="1">
+        <f>SUM(E9:E76)</f>
         <v>0</v>
       </c>
-      <c r="E11" s="12" t="str">
-        <f>E12&amp;+ "/" &amp;+ $D$11</f>
-        <v>0/0</v>
-      </c>
-      <c r="F11" s="12" t="str">
-        <f>F12&amp;+ "/" &amp;+ $D$11</f>
-        <v>0/0</v>
-      </c>
-      <c r="G11" s="12" t="str">
-        <f t="shared" ref="G11:K11" si="0">G12&amp;+ "/" &amp;+ $D$11</f>
-        <v>0/0</v>
-      </c>
-      <c r="H11" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v>0/0</v>
-      </c>
-      <c r="I11" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v>0/0</v>
-      </c>
-      <c r="J11" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v>0/0</v>
-      </c>
-      <c r="K11" s="13" t="str">
-        <f t="shared" si="0"/>
-        <v>0/0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" ht="15" hidden="1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="D12" s="1">
-        <f>SUM(D9:D10)</f>
+      <c r="F78" s="1">
+        <f>SUM(F9:F76)</f>
         <v>0</v>
       </c>
-      <c r="E12" s="1">
-        <f>SUM(E9:E10)</f>
+      <c r="G78" s="1">
+        <f>SUM(G9:G76)+F78</f>
         <v>0</v>
       </c>
-      <c r="F12" s="1">
-        <f>SUM(F9:F10)</f>
+      <c r="H78" s="1">
+        <f>SUM(H9:H76)+G78</f>
         <v>0</v>
       </c>
-      <c r="G12" s="1">
-        <f>SUM(G9:G10)+F12</f>
+      <c r="I78" s="1">
+        <f>SUM(I9:I76)+H78</f>
         <v>0</v>
       </c>
-      <c r="H12" s="1">
-        <f>SUM(H9:H10)+G12</f>
+      <c r="J78" s="1">
+        <f>SUM(J9:J76)+I78</f>
         <v>0</v>
       </c>
-      <c r="I12" s="1">
-        <f>SUM(I9:I10)+H12</f>
+      <c r="K78" s="1">
+        <f>SUM(K9:K76)+J78</f>
         <v>0</v>
       </c>
-      <c r="J12" s="1">
-        <f>SUM(J9:J10)+I12</f>
+      <c r="L78" s="1"/>
+    </row>
+    <row r="79" spans="1:12" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D79" s="1"/>
+      <c r="E79" s="1">
+        <f>D77</f>
+        <v>162.5</v>
+      </c>
+      <c r="F79" s="1">
+        <f>E79</f>
+        <v>162.5</v>
+      </c>
+      <c r="G79" s="1">
+        <f>F79</f>
+        <v>162.5</v>
+      </c>
+      <c r="H79" s="1">
+        <f t="shared" ref="H79:K79" si="1">G79</f>
+        <v>162.5</v>
+      </c>
+      <c r="I79" s="1">
+        <f t="shared" si="1"/>
+        <v>162.5</v>
+      </c>
+      <c r="J79" s="1">
+        <f t="shared" si="1"/>
+        <v>162.5</v>
+      </c>
+      <c r="K79" s="1">
+        <f t="shared" si="1"/>
+        <v>162.5</v>
+      </c>
+      <c r="L79" s="1"/>
+    </row>
+    <row r="80" spans="1:12" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D80" s="1"/>
+      <c r="E80" s="1">
         <v>0</v>
       </c>
-      <c r="K12" s="1">
-        <f>SUM(K9:K10)+J12</f>
-        <v>0</v>
-      </c>
-      <c r="L12" s="1"/>
-    </row>
-    <row r="13" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D13" s="1"/>
-      <c r="E13" s="1">
-        <f>D11</f>
-        <v>0</v>
-      </c>
-      <c r="F13" s="1">
-        <f>E13</f>
-        <v>0</v>
-      </c>
-      <c r="G13" s="1">
-        <f>F13</f>
-        <v>0</v>
-      </c>
-      <c r="H13" s="1">
-        <f t="shared" ref="H13:K13" si="1">G13</f>
-        <v>0</v>
-      </c>
-      <c r="I13" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J13" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K13" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L13" s="1"/>
-    </row>
-    <row r="14" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D14" s="1"/>
-      <c r="E14" s="1">
-        <v>0</v>
-      </c>
-      <c r="K14" s="2">
-        <f>K13</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
-      <c r="D15" s="1"/>
-      <c r="E15" s="5" t="s">
+      <c r="K80" s="2">
+        <f>K79</f>
+        <v>162.5</v>
+      </c>
+    </row>
+    <row r="81" spans="4:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D81" s="1"/>
+      <c r="E81" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="F81" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G15" s="5" t="s">
+      <c r="G81" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
-      <c r="O15" s="4"/>
-      <c r="P15" s="4"/>
-      <c r="Q15" s="4"/>
-      <c r="R15" s="4"/>
-      <c r="S15" s="4"/>
-      <c r="T15" s="4"/>
-    </row>
-    <row r="16" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-    </row>
-    <row r="34" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R34" s="2" t="s">
+      <c r="H81" s="5"/>
+      <c r="I81" s="5"/>
+      <c r="J81" s="4"/>
+      <c r="K81" s="4"/>
+      <c r="L81" s="4"/>
+      <c r="M81" s="4"/>
+      <c r="N81" s="4"/>
+      <c r="O81" s="4"/>
+      <c r="P81" s="4"/>
+      <c r="Q81" s="4"/>
+      <c r="R81" s="4"/>
+      <c r="S81" s="4"/>
+      <c r="T81" s="4"/>
+    </row>
+    <row r="82" spans="4:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="D82" s="1"/>
+      <c r="E82" s="1"/>
+      <c r="F82" s="1"/>
+      <c r="G82" s="1"/>
+      <c r="H82" s="1"/>
+      <c r="I82" s="1"/>
+    </row>
+    <row r="100" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R100" s="2" t="s">
         <v>30</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="14">
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="F7:K7"/>
     <mergeCell ref="B7:B8"/>
+    <mergeCell ref="A60:A67"/>
+    <mergeCell ref="A68:A76"/>
+    <mergeCell ref="A9:A14"/>
+    <mergeCell ref="A15:A28"/>
+    <mergeCell ref="A29:A48"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="A52:A57"/>
+    <mergeCell ref="A49:A51"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Number" error="Please Enter Only Numbers. You may use .5 increments. " sqref="D9:E10">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Number" error="Please Enter Only Numbers. You may use .5 increments. " sqref="D9:D76">
       <formula1>0</formula1>
       <formula2>100000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Numbers Only" error="Please Enter Only Numbers. You may use .5 increments. " sqref="F9:K10">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Numbers Only" error="Please Enter Only Numbers. You may use .5 increments. " sqref="F9:K76">
       <formula1>0</formula1>
       <formula2>10000</formula2>
     </dataValidation>
@@ -2629,7 +4830,7 @@
           <x14:formula1>
             <xm:f>'Names-Hours'!$B$3:$B$8</xm:f>
           </x14:formula1>
-          <xm:sqref>C9:C10</xm:sqref>
+          <xm:sqref>C9:C76</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2639,10 +4840,831 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="78" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="69" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="82" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" s="70" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" s="70" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="71" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="83" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" s="74">
+        <v>13</v>
+      </c>
+      <c r="D4" s="75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="72" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="83" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5" s="76">
+        <v>20</v>
+      </c>
+      <c r="D5" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="72" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="83" t="s">
+        <v>84</v>
+      </c>
+      <c r="C6" s="76">
+        <v>5</v>
+      </c>
+      <c r="D6" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="72" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" s="83" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" s="76">
+        <v>5</v>
+      </c>
+      <c r="D7" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="72" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" s="83" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8" s="76">
+        <v>20</v>
+      </c>
+      <c r="D8" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="72" t="s">
+        <v>68</v>
+      </c>
+      <c r="B9" s="83" t="s">
+        <v>84</v>
+      </c>
+      <c r="C9" s="76">
+        <v>13</v>
+      </c>
+      <c r="D9" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="72" t="s">
+        <v>69</v>
+      </c>
+      <c r="B10" s="83" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10" s="76">
+        <v>5</v>
+      </c>
+      <c r="D10" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="72" t="s">
+        <v>70</v>
+      </c>
+      <c r="B11" s="83" t="s">
+        <v>84</v>
+      </c>
+      <c r="C11" s="76">
+        <v>20</v>
+      </c>
+      <c r="D11" s="77">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="72" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" s="83" t="s">
+        <v>85</v>
+      </c>
+      <c r="C12" s="76">
+        <v>20</v>
+      </c>
+      <c r="D12" s="77">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="72" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" s="83" t="s">
+        <v>84</v>
+      </c>
+      <c r="C13" s="76">
+        <v>13</v>
+      </c>
+      <c r="D13" s="77">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="72" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" s="83" t="s">
+        <v>86</v>
+      </c>
+      <c r="C14" s="76" t="s">
+        <v>78</v>
+      </c>
+      <c r="D14" s="80" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="72" t="s">
+        <v>74</v>
+      </c>
+      <c r="B15" s="83" t="s">
+        <v>84</v>
+      </c>
+      <c r="C15" s="76">
+        <v>13</v>
+      </c>
+      <c r="D15" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="73" t="s">
+        <v>75</v>
+      </c>
+      <c r="B16" s="83" t="s">
+        <v>85</v>
+      </c>
+      <c r="C16" s="78">
+        <v>5</v>
+      </c>
+      <c r="D16" s="79">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K15" sqref="K15:L17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" customWidth="1"/>
+    <col min="5" max="6" width="20.7109375" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" customWidth="1"/>
+    <col min="8" max="9" width="20.7109375" customWidth="1"/>
+    <col min="10" max="10" width="8.7109375" customWidth="1"/>
+    <col min="11" max="12" width="20.7109375" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="29.25" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="137" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="138"/>
+      <c r="C1" s="139"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="137" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="138"/>
+      <c r="G1" s="138"/>
+      <c r="H1" s="138"/>
+      <c r="I1" s="138"/>
+      <c r="J1" s="138"/>
+      <c r="K1" s="138"/>
+      <c r="L1" s="138"/>
+      <c r="M1" s="139"/>
+    </row>
+    <row r="2" spans="1:13" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="140"/>
+      <c r="B2" s="141"/>
+      <c r="C2" s="142"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="140" t="s">
+        <v>80</v>
+      </c>
+      <c r="F2" s="141"/>
+      <c r="G2" s="142"/>
+      <c r="H2" s="141" t="s">
+        <v>81</v>
+      </c>
+      <c r="I2" s="141"/>
+      <c r="J2" s="142"/>
+      <c r="K2" s="141" t="s">
+        <v>82</v>
+      </c>
+      <c r="L2" s="141"/>
+      <c r="M2" s="142"/>
+    </row>
+    <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="129" t="str">
+        <f>Backlog!A11</f>
+        <v>As a User, I want to be able to detect Par. in Chemical Diagram, so I can work with polymers</v>
+      </c>
+      <c r="B3" s="130"/>
+      <c r="C3" s="87">
+        <f>Backlog!C11</f>
+        <v>20</v>
+      </c>
+      <c r="E3" s="111" t="str">
+        <f>Backlog!A4</f>
+        <v>As a Developer, I need an architectural overview of OSRA’s processing, so I can understand the code base.</v>
+      </c>
+      <c r="F3" s="112"/>
+      <c r="G3" s="87">
+        <f>Backlog!C4</f>
+        <v>13</v>
+      </c>
+      <c r="H3" s="105"/>
+      <c r="I3" s="106"/>
+      <c r="J3" s="86"/>
+      <c r="K3" s="105"/>
+      <c r="L3" s="106"/>
+      <c r="M3" s="86"/>
+    </row>
+    <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="131"/>
+      <c r="B4" s="132"/>
+      <c r="C4" s="88" t="str">
+        <f>Backlog!B11</f>
+        <v>M</v>
+      </c>
+      <c r="E4" s="113"/>
+      <c r="F4" s="114"/>
+      <c r="G4" s="88" t="str">
+        <f>Backlog!B4</f>
+        <v>M</v>
+      </c>
+      <c r="H4" s="107"/>
+      <c r="I4" s="108"/>
+      <c r="J4" s="84"/>
+      <c r="K4" s="107"/>
+      <c r="L4" s="108"/>
+      <c r="M4" s="84"/>
+    </row>
+    <row r="5" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="133"/>
+      <c r="B5" s="134"/>
+      <c r="C5" s="89"/>
+      <c r="E5" s="115"/>
+      <c r="F5" s="116"/>
+      <c r="G5" s="89"/>
+      <c r="H5" s="109"/>
+      <c r="I5" s="110"/>
+      <c r="J5" s="85"/>
+      <c r="K5" s="109"/>
+      <c r="L5" s="110"/>
+      <c r="M5" s="85"/>
+    </row>
+    <row r="6" spans="1:13" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="129" t="str">
+        <f>Backlog!A12</f>
+        <v>As a User, I want to be able to detect Brackets in Chemical Diagrams, so I can work with polymers</v>
+      </c>
+      <c r="B6" s="130"/>
+      <c r="C6" s="87">
+        <f>Backlog!C12</f>
+        <v>20</v>
+      </c>
+      <c r="E6" s="111" t="str">
+        <f>Backlog!A5</f>
+        <v>As a Developer, I need to review each aspect of OSRA’s architecture, so I can understand the code base.</v>
+      </c>
+      <c r="F6" s="112"/>
+      <c r="G6" s="87">
+        <f>Backlog!C5</f>
+        <v>20</v>
+      </c>
+      <c r="H6" s="105"/>
+      <c r="I6" s="106"/>
+      <c r="J6" s="86"/>
+      <c r="K6" s="105"/>
+      <c r="L6" s="106"/>
+      <c r="M6" s="86"/>
+    </row>
+    <row r="7" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="131"/>
+      <c r="B7" s="132"/>
+      <c r="C7" s="88" t="str">
+        <f>Backlog!B12</f>
+        <v>S</v>
+      </c>
+      <c r="E7" s="113"/>
+      <c r="F7" s="114"/>
+      <c r="G7" s="88" t="str">
+        <f>Backlog!B5</f>
+        <v>M</v>
+      </c>
+      <c r="H7" s="107"/>
+      <c r="I7" s="108"/>
+      <c r="J7" s="84"/>
+      <c r="K7" s="107"/>
+      <c r="L7" s="108"/>
+      <c r="M7" s="84"/>
+    </row>
+    <row r="8" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="133"/>
+      <c r="B8" s="134"/>
+      <c r="C8" s="89"/>
+      <c r="E8" s="115"/>
+      <c r="F8" s="116"/>
+      <c r="G8" s="89"/>
+      <c r="H8" s="109"/>
+      <c r="I8" s="110"/>
+      <c r="J8" s="85"/>
+      <c r="K8" s="109"/>
+      <c r="L8" s="110"/>
+      <c r="M8" s="85"/>
+    </row>
+    <row r="9" spans="1:13" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="129" t="str">
+        <f>Backlog!A13</f>
+        <v>As a User, I want to be able to detect subscripts for polymer diagrams, so I can work with polymers</v>
+      </c>
+      <c r="B9" s="130"/>
+      <c r="C9" s="87">
+        <f>Backlog!C13</f>
+        <v>13</v>
+      </c>
+      <c r="E9" s="111" t="str">
+        <f>Backlog!A6</f>
+        <v>As a Developer, I need to get a basic grasp of O-Chem, so I can better understand use cases.</v>
+      </c>
+      <c r="F9" s="112"/>
+      <c r="G9" s="87">
+        <f>Backlog!C6</f>
+        <v>5</v>
+      </c>
+      <c r="H9" s="105"/>
+      <c r="I9" s="106"/>
+      <c r="J9" s="86"/>
+      <c r="K9" s="105"/>
+      <c r="L9" s="106"/>
+      <c r="M9" s="86"/>
+    </row>
+    <row r="10" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="131"/>
+      <c r="B10" s="132"/>
+      <c r="C10" s="88" t="str">
+        <f>Backlog!B13</f>
+        <v>M</v>
+      </c>
+      <c r="E10" s="113"/>
+      <c r="F10" s="114"/>
+      <c r="G10" s="88" t="str">
+        <f>Backlog!B6</f>
+        <v>M</v>
+      </c>
+      <c r="H10" s="107"/>
+      <c r="I10" s="108"/>
+      <c r="J10" s="84"/>
+      <c r="K10" s="107"/>
+      <c r="L10" s="108"/>
+      <c r="M10" s="84"/>
+    </row>
+    <row r="11" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="133"/>
+      <c r="B11" s="134"/>
+      <c r="C11" s="89"/>
+      <c r="E11" s="115"/>
+      <c r="F11" s="116"/>
+      <c r="G11" s="89"/>
+      <c r="H11" s="109"/>
+      <c r="I11" s="110"/>
+      <c r="J11" s="85"/>
+      <c r="K11" s="109"/>
+      <c r="L11" s="110"/>
+      <c r="M11" s="85"/>
+    </row>
+    <row r="12" spans="1:13" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="129" t="str">
+        <f>Backlog!A14</f>
+        <v>As a User, I want to be able to detect “R-Notation”, so I can work with polymers</v>
+      </c>
+      <c r="B12" s="130"/>
+      <c r="C12" s="87" t="str">
+        <f>Backlog!C14</f>
+        <v>INF</v>
+      </c>
+      <c r="E12" s="111" t="str">
+        <f>Backlog!A7</f>
+        <v>As a Developer, I need workflow and processes for the github repo, so I can collaborate on code</v>
+      </c>
+      <c r="F12" s="112"/>
+      <c r="G12" s="87">
+        <f>Backlog!C7</f>
+        <v>5</v>
+      </c>
+      <c r="H12" s="105"/>
+      <c r="I12" s="106"/>
+      <c r="J12" s="86"/>
+      <c r="K12" s="105"/>
+      <c r="L12" s="106"/>
+      <c r="M12" s="86"/>
+    </row>
+    <row r="13" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="131"/>
+      <c r="B13" s="132"/>
+      <c r="C13" s="88" t="str">
+        <f>Backlog!B14</f>
+        <v>W</v>
+      </c>
+      <c r="E13" s="113"/>
+      <c r="F13" s="114"/>
+      <c r="G13" s="88" t="str">
+        <f>Backlog!B7</f>
+        <v>M</v>
+      </c>
+      <c r="H13" s="107"/>
+      <c r="I13" s="108"/>
+      <c r="J13" s="84"/>
+      <c r="K13" s="107"/>
+      <c r="L13" s="108"/>
+      <c r="M13" s="84"/>
+    </row>
+    <row r="14" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="135"/>
+      <c r="B14" s="136"/>
+      <c r="C14" s="90"/>
+      <c r="E14" s="115"/>
+      <c r="F14" s="116"/>
+      <c r="G14" s="89"/>
+      <c r="H14" s="109"/>
+      <c r="I14" s="110"/>
+      <c r="J14" s="85"/>
+      <c r="K14" s="109"/>
+      <c r="L14" s="110"/>
+      <c r="M14" s="85"/>
+    </row>
+    <row r="15" spans="1:13" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="123"/>
+      <c r="B15" s="124"/>
+      <c r="C15" s="87"/>
+      <c r="E15" s="111" t="str">
+        <f>Backlog!A8</f>
+        <v>As a Developer, I need a testing enviroment and test documentation, so I can better contribute to the codebase</v>
+      </c>
+      <c r="F15" s="112"/>
+      <c r="G15" s="87">
+        <f>Backlog!C8</f>
+        <v>20</v>
+      </c>
+      <c r="H15" s="105"/>
+      <c r="I15" s="106"/>
+      <c r="J15" s="86"/>
+      <c r="K15" s="105"/>
+      <c r="L15" s="106"/>
+      <c r="M15" s="86"/>
+    </row>
+    <row r="16" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="125"/>
+      <c r="B16" s="126"/>
+      <c r="C16" s="88"/>
+      <c r="E16" s="113"/>
+      <c r="F16" s="114"/>
+      <c r="G16" s="88" t="str">
+        <f>Backlog!B8</f>
+        <v>M</v>
+      </c>
+      <c r="H16" s="107"/>
+      <c r="I16" s="108"/>
+      <c r="J16" s="84"/>
+      <c r="K16" s="107"/>
+      <c r="L16" s="108"/>
+      <c r="M16" s="84"/>
+    </row>
+    <row r="17" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="127"/>
+      <c r="B17" s="128"/>
+      <c r="C17" s="89"/>
+      <c r="E17" s="115"/>
+      <c r="F17" s="116"/>
+      <c r="G17" s="89"/>
+      <c r="H17" s="109"/>
+      <c r="I17" s="110"/>
+      <c r="J17" s="85"/>
+      <c r="K17" s="109"/>
+      <c r="L17" s="110"/>
+      <c r="M17" s="85"/>
+    </row>
+    <row r="18" spans="1:13" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="123"/>
+      <c r="B18" s="124"/>
+      <c r="C18" s="87"/>
+      <c r="E18" s="111" t="str">
+        <f>Backlog!A9</f>
+        <v>As a Developer, I need to have consolidated documentation from other developers, so I can better contribute to the codebase</v>
+      </c>
+      <c r="F18" s="112"/>
+      <c r="G18" s="87">
+        <f>Backlog!C9</f>
+        <v>13</v>
+      </c>
+      <c r="H18" s="105"/>
+      <c r="I18" s="106"/>
+      <c r="J18" s="86"/>
+      <c r="K18" s="105"/>
+      <c r="L18" s="106"/>
+      <c r="M18" s="86"/>
+    </row>
+    <row r="19" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="125"/>
+      <c r="B19" s="126"/>
+      <c r="C19" s="88"/>
+      <c r="E19" s="113"/>
+      <c r="F19" s="114"/>
+      <c r="G19" s="88" t="str">
+        <f>Backlog!B9</f>
+        <v>M</v>
+      </c>
+      <c r="H19" s="107"/>
+      <c r="I19" s="108"/>
+      <c r="J19" s="84"/>
+      <c r="K19" s="107"/>
+      <c r="L19" s="108"/>
+      <c r="M19" s="84"/>
+    </row>
+    <row r="20" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="127"/>
+      <c r="B20" s="128"/>
+      <c r="C20" s="89"/>
+      <c r="E20" s="115"/>
+      <c r="F20" s="116"/>
+      <c r="G20" s="89"/>
+      <c r="H20" s="109"/>
+      <c r="I20" s="110"/>
+      <c r="J20" s="85"/>
+      <c r="K20" s="109"/>
+      <c r="L20" s="110"/>
+      <c r="M20" s="85"/>
+    </row>
+    <row r="21" spans="1:13" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="123"/>
+      <c r="B21" s="124"/>
+      <c r="C21" s="87"/>
+      <c r="E21" s="111" t="str">
+        <f>Backlog!A10</f>
+        <v>As a Developer, I need to understand SMILES notation and .SD file structure, so I can desing the smile data structure.</v>
+      </c>
+      <c r="F21" s="112"/>
+      <c r="G21" s="87">
+        <f>Backlog!C10</f>
+        <v>5</v>
+      </c>
+      <c r="H21" s="105"/>
+      <c r="I21" s="106"/>
+      <c r="J21" s="86"/>
+      <c r="K21" s="105"/>
+      <c r="L21" s="106"/>
+      <c r="M21" s="86"/>
+    </row>
+    <row r="22" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="125"/>
+      <c r="B22" s="126"/>
+      <c r="C22" s="88"/>
+      <c r="E22" s="113"/>
+      <c r="F22" s="114"/>
+      <c r="G22" s="88" t="str">
+        <f>Backlog!B10</f>
+        <v>M</v>
+      </c>
+      <c r="H22" s="107"/>
+      <c r="I22" s="108"/>
+      <c r="J22" s="84"/>
+      <c r="K22" s="107"/>
+      <c r="L22" s="108"/>
+      <c r="M22" s="84"/>
+    </row>
+    <row r="23" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="127"/>
+      <c r="B23" s="128"/>
+      <c r="C23" s="89"/>
+      <c r="E23" s="115"/>
+      <c r="F23" s="116"/>
+      <c r="G23" s="89"/>
+      <c r="H23" s="109"/>
+      <c r="I23" s="110"/>
+      <c r="J23" s="85"/>
+      <c r="K23" s="109"/>
+      <c r="L23" s="110"/>
+      <c r="M23" s="85"/>
+    </row>
+    <row r="24" spans="1:13" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="123"/>
+      <c r="B24" s="124"/>
+      <c r="C24" s="87"/>
+      <c r="E24" s="111" t="str">
+        <f>Backlog!A15</f>
+        <v>As a User, I want to have a data structure for encoding polymers in “Smile Notation”, so I can work with polymers</v>
+      </c>
+      <c r="F24" s="112"/>
+      <c r="G24" s="87">
+        <f>Backlog!C15</f>
+        <v>13</v>
+      </c>
+      <c r="H24" s="105"/>
+      <c r="I24" s="106"/>
+      <c r="J24" s="86"/>
+      <c r="K24" s="105"/>
+      <c r="L24" s="106"/>
+      <c r="M24" s="86"/>
+    </row>
+    <row r="25" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="125"/>
+      <c r="B25" s="126"/>
+      <c r="C25" s="88"/>
+      <c r="E25" s="113"/>
+      <c r="F25" s="114"/>
+      <c r="G25" s="88" t="str">
+        <f>Backlog!B15</f>
+        <v>M</v>
+      </c>
+      <c r="H25" s="107"/>
+      <c r="I25" s="108"/>
+      <c r="J25" s="84"/>
+      <c r="K25" s="107"/>
+      <c r="L25" s="108"/>
+      <c r="M25" s="84"/>
+    </row>
+    <row r="26" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="127"/>
+      <c r="B26" s="128"/>
+      <c r="C26" s="89"/>
+      <c r="E26" s="115"/>
+      <c r="F26" s="116"/>
+      <c r="G26" s="89"/>
+      <c r="H26" s="109"/>
+      <c r="I26" s="110"/>
+      <c r="J26" s="85"/>
+      <c r="K26" s="109"/>
+      <c r="L26" s="110"/>
+      <c r="M26" s="85"/>
+    </row>
+    <row r="27" spans="1:13" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="123"/>
+      <c r="B27" s="124"/>
+      <c r="C27" s="87"/>
+      <c r="E27" s="117"/>
+      <c r="F27" s="118"/>
+      <c r="G27" s="87"/>
+      <c r="H27" s="105"/>
+      <c r="I27" s="106"/>
+      <c r="J27" s="86"/>
+      <c r="K27" s="105"/>
+      <c r="L27" s="106"/>
+      <c r="M27" s="86"/>
+    </row>
+    <row r="28" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="125"/>
+      <c r="B28" s="126"/>
+      <c r="C28" s="88"/>
+      <c r="E28" s="119"/>
+      <c r="F28" s="120"/>
+      <c r="G28" s="88"/>
+      <c r="H28" s="107"/>
+      <c r="I28" s="108"/>
+      <c r="J28" s="84"/>
+      <c r="K28" s="107"/>
+      <c r="L28" s="108"/>
+      <c r="M28" s="84"/>
+    </row>
+    <row r="29" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="127"/>
+      <c r="B29" s="128"/>
+      <c r="C29" s="89"/>
+      <c r="E29" s="121"/>
+      <c r="F29" s="122"/>
+      <c r="G29" s="89"/>
+      <c r="H29" s="109"/>
+      <c r="I29" s="110"/>
+      <c r="J29" s="85"/>
+      <c r="K29" s="109"/>
+      <c r="L29" s="110"/>
+      <c r="M29" s="85"/>
+    </row>
+    <row r="30" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="41">
+    <mergeCell ref="E1:M1"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="A1:C2"/>
+    <mergeCell ref="A3:B5"/>
+    <mergeCell ref="A6:B8"/>
+    <mergeCell ref="A9:B11"/>
+    <mergeCell ref="A12:B14"/>
+    <mergeCell ref="A15:B17"/>
+    <mergeCell ref="E3:F5"/>
+    <mergeCell ref="E6:F8"/>
+    <mergeCell ref="E9:F11"/>
+    <mergeCell ref="E12:F14"/>
+    <mergeCell ref="E15:F17"/>
+    <mergeCell ref="E18:F20"/>
+    <mergeCell ref="E21:F23"/>
+    <mergeCell ref="E24:F26"/>
+    <mergeCell ref="E27:F29"/>
+    <mergeCell ref="A21:B23"/>
+    <mergeCell ref="A24:B26"/>
+    <mergeCell ref="A27:B29"/>
+    <mergeCell ref="A18:B20"/>
+    <mergeCell ref="H3:I5"/>
+    <mergeCell ref="H6:I8"/>
+    <mergeCell ref="H9:I11"/>
+    <mergeCell ref="H12:I14"/>
+    <mergeCell ref="H15:I17"/>
+    <mergeCell ref="K3:L5"/>
+    <mergeCell ref="K6:L8"/>
+    <mergeCell ref="K9:L11"/>
+    <mergeCell ref="K12:L14"/>
+    <mergeCell ref="K15:L17"/>
+    <mergeCell ref="K18:L20"/>
+    <mergeCell ref="K21:L23"/>
+    <mergeCell ref="K24:L26"/>
+    <mergeCell ref="K27:L29"/>
+    <mergeCell ref="H21:I23"/>
+    <mergeCell ref="H24:I26"/>
+    <mergeCell ref="H27:I29"/>
+    <mergeCell ref="H18:I20"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2694,14 +5716,14 @@
         <v>4</v>
       </c>
       <c r="F3" s="2">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="G3" s="2">
         <v>0</v>
       </c>
       <c r="H3" s="1">
-        <f>SUM(E3:G3)*'Tasks List'!B5</f>
-        <v>0</v>
+        <f>D3-SUM(E3:G3)</f>
+        <v>24.5</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
@@ -2719,14 +5741,14 @@
         <v>4</v>
       </c>
       <c r="F4" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G4" s="2">
         <v>0</v>
       </c>
       <c r="H4" s="1">
-        <f>SUM(E4:G4)*'Tasks List'!B5</f>
-        <v>0</v>
+        <f t="shared" ref="H4:H8" si="0">D4-SUM(E4:G4)</f>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -2744,14 +5766,14 @@
         <v>4</v>
       </c>
       <c r="F5" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G5" s="2">
         <v>0</v>
       </c>
       <c r="H5" s="1">
-        <f>SUM(E5:G5)*'Tasks List'!B5</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
@@ -2769,19 +5791,19 @@
         <v>4</v>
       </c>
       <c r="F6" s="2">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="G6" s="2">
         <v>0</v>
       </c>
       <c r="H6" s="1">
-        <f>SUM(E6:G6)*'Tasks List'!B5</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>24.5</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="C7" s="2">
         <v>15</v>
@@ -2794,14 +5816,14 @@
         <v>4</v>
       </c>
       <c r="F7" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G7" s="2">
         <v>0</v>
       </c>
       <c r="H7" s="1">
-        <f>SUM(E7:G7)*'Tasks List'!B5</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
@@ -2819,14 +5841,14 @@
         <v>4</v>
       </c>
       <c r="F8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8" s="2">
         <v>0</v>
       </c>
       <c r="H8" s="1">
-        <f>SUM(E8:G8)*'Tasks List'!B5</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -2834,7 +5856,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -2854,7 +5876,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="55">
+      <c r="A2" s="143">
         <v>41557</v>
       </c>
       <c r="B2" t="s">
@@ -2862,7 +5884,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="55"/>
+      <c r="A3" s="143"/>
       <c r="B3" t="s">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
Updated Tasks From Scrum Meeting 01/24/2014
</commit_message>
<xml_diff>
--- a/bookkeeping/Sprint1 BurnUp.xlsx
+++ b/bookkeeping/Sprint1 BurnUp.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9450" yWindow="0" windowWidth="16410" windowHeight="7815" tabRatio="601" activeTab="3"/>
+    <workbookView xWindow="11496" yWindow="0" windowWidth="16416" windowHeight="7812" tabRatio="601"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks List" sheetId="1" r:id="rId1"/>
@@ -1511,15 +1511,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1556,6 +1547,111 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1573,102 +1669,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1865,22 +1865,22 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2102,11 +2102,11 @@
         </c:dropLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="318329224"/>
-        <c:axId val="318330792"/>
+        <c:axId val="241513112"/>
+        <c:axId val="241508408"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="318329224"/>
+        <c:axId val="241513112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2149,14 +2149,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="318330792"/>
+        <c:crossAx val="241508408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="318330792"/>
+        <c:axId val="241508408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2193,7 +2193,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="318329224"/>
+        <c:crossAx val="241513112"/>
         <c:crossesAt val="41548"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="10"/>
@@ -2874,7 +2874,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -2886,7 +2886,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8667750" cy="6296025"/>
+    <xdr:ext cx="8656320" cy="6278880"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -3174,25 +3174,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T100"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="8" topLeftCell="F9" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" sqref="A1:B1"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60:A67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="47.42578125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="76.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" style="2" hidden="1" customWidth="1"/>
-    <col min="6" max="11" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="47.44140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="76.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" style="2" hidden="1" customWidth="1"/>
+    <col min="6" max="11" width="11.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
@@ -3203,18 +3200,18 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="21"/>
       <c r="B2" s="22"/>
       <c r="D2" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="94" t="s">
+      <c r="F2" s="91" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="95"/>
-    </row>
-    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G2" s="92"/>
+    </row>
+    <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="18" t="s">
         <v>26</v>
       </c>
@@ -3243,7 +3240,7 @@
         <v>0.5/30</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="19" t="s">
         <v>27</v>
       </c>
@@ -3273,7 +3270,7 @@
         <v>0/30</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="9"/>
       <c r="D5" s="25" t="s">
         <v>21</v>
@@ -3285,36 +3282,36 @@
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
     </row>
-    <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:12" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="100" t="s">
+    <row r="6" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="1:12" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="97" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="100" t="s">
+      <c r="B7" s="97" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="96" t="s">
+      <c r="C7" s="93" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="98" t="s">
+      <c r="D7" s="95" t="s">
         <v>9</v>
       </c>
       <c r="E7" s="27"/>
-      <c r="F7" s="102" t="s">
+      <c r="F7" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="103"/>
-      <c r="H7" s="103"/>
-      <c r="I7" s="103"/>
-      <c r="J7" s="103"/>
-      <c r="K7" s="104"/>
+      <c r="G7" s="100"/>
+      <c r="H7" s="100"/>
+      <c r="I7" s="100"/>
+      <c r="J7" s="100"/>
+      <c r="K7" s="101"/>
       <c r="L7" s="16"/>
     </row>
-    <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="101"/>
-      <c r="B8" s="101"/>
-      <c r="C8" s="97"/>
-      <c r="D8" s="99"/>
+    <row r="8" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="98"/>
+      <c r="B8" s="98"/>
+      <c r="C8" s="94"/>
+      <c r="D8" s="96"/>
       <c r="E8" s="10">
         <v>41661</v>
       </c>
@@ -3337,8 +3334,8 @@
         <v>41675</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="16.149999999999999" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="93" t="s">
+    <row r="9" spans="1:12" ht="16.2" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="104" t="s">
         <v>53</v>
       </c>
       <c r="B9" s="36" t="s">
@@ -3351,15 +3348,17 @@
         <v>1.5</v>
       </c>
       <c r="E9" s="39"/>
-      <c r="F9" s="40"/>
+      <c r="F9" s="40">
+        <v>0.5</v>
+      </c>
       <c r="G9" s="41"/>
       <c r="H9" s="41"/>
       <c r="I9" s="42"/>
       <c r="J9" s="42"/>
       <c r="K9" s="43"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="91"/>
+    <row r="10" spans="1:12" ht="15" x14ac:dyDescent="0.3">
+      <c r="A10" s="102"/>
       <c r="B10" s="44" t="s">
         <v>32</v>
       </c>
@@ -3370,15 +3369,17 @@
         <v>1.5</v>
       </c>
       <c r="E10" s="45"/>
-      <c r="F10" s="32"/>
+      <c r="F10" s="32">
+        <v>1</v>
+      </c>
       <c r="G10" s="33"/>
       <c r="H10" s="33"/>
       <c r="I10" s="34"/>
       <c r="J10" s="34"/>
       <c r="K10" s="35"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="91"/>
+    <row r="11" spans="1:12" ht="15" x14ac:dyDescent="0.3">
+      <c r="A11" s="102"/>
       <c r="B11" s="46" t="s">
         <v>33</v>
       </c>
@@ -3396,8 +3397,8 @@
       <c r="J11" s="52"/>
       <c r="K11" s="53"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="91"/>
+    <row r="12" spans="1:12" ht="15" x14ac:dyDescent="0.3">
+      <c r="A12" s="102"/>
       <c r="B12" s="44" t="s">
         <v>33</v>
       </c>
@@ -3415,8 +3416,8 @@
       <c r="J12" s="34"/>
       <c r="K12" s="35"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="91"/>
+    <row r="13" spans="1:12" ht="15" x14ac:dyDescent="0.3">
+      <c r="A13" s="102"/>
       <c r="B13" s="46" t="s">
         <v>31</v>
       </c>
@@ -3434,8 +3435,8 @@
       <c r="J13" s="52"/>
       <c r="K13" s="53"/>
     </row>
-    <row r="14" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="92"/>
+    <row r="14" spans="1:12" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="103"/>
       <c r="B14" s="54" t="s">
         <v>54</v>
       </c>
@@ -3446,15 +3447,17 @@
         <v>5</v>
       </c>
       <c r="E14" s="55"/>
-      <c r="F14" s="56"/>
+      <c r="F14" s="56">
+        <v>1</v>
+      </c>
       <c r="G14" s="57"/>
       <c r="H14" s="57"/>
       <c r="I14" s="58"/>
       <c r="J14" s="58"/>
       <c r="K14" s="59"/>
     </row>
-    <row r="15" spans="1:12" ht="15.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="91" t="s">
+    <row r="15" spans="1:12" ht="15.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="102" t="s">
         <v>55</v>
       </c>
       <c r="B15" s="46" t="s">
@@ -3474,8 +3477,8 @@
       <c r="J15" s="52"/>
       <c r="K15" s="53"/>
     </row>
-    <row r="16" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="91"/>
+    <row r="16" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="102"/>
       <c r="B16" s="44" t="s">
         <v>35</v>
       </c>
@@ -3493,8 +3496,8 @@
       <c r="J16" s="34"/>
       <c r="K16" s="35"/>
     </row>
-    <row r="17" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="91"/>
+    <row r="17" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="102"/>
       <c r="B17" s="46" t="s">
         <v>35</v>
       </c>
@@ -3505,15 +3508,17 @@
         <v>8</v>
       </c>
       <c r="E17" s="49"/>
-      <c r="F17" s="50"/>
+      <c r="F17" s="50">
+        <v>0.5</v>
+      </c>
       <c r="G17" s="51"/>
       <c r="H17" s="51"/>
       <c r="I17" s="52"/>
       <c r="J17" s="52"/>
       <c r="K17" s="53"/>
     </row>
-    <row r="18" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="91"/>
+    <row r="18" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="102"/>
       <c r="B18" s="44" t="s">
         <v>35</v>
       </c>
@@ -3524,15 +3529,17 @@
         <v>8</v>
       </c>
       <c r="E18" s="45"/>
-      <c r="F18" s="32"/>
+      <c r="F18" s="32">
+        <v>1</v>
+      </c>
       <c r="G18" s="33"/>
       <c r="H18" s="33"/>
       <c r="I18" s="34"/>
       <c r="J18" s="34"/>
       <c r="K18" s="35"/>
     </row>
-    <row r="19" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="91"/>
+    <row r="19" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="102"/>
       <c r="B19" s="46" t="s">
         <v>35</v>
       </c>
@@ -3543,15 +3550,17 @@
         <v>8</v>
       </c>
       <c r="E19" s="49"/>
-      <c r="F19" s="50"/>
+      <c r="F19" s="50">
+        <v>2</v>
+      </c>
       <c r="G19" s="51"/>
       <c r="H19" s="51"/>
       <c r="I19" s="52"/>
       <c r="J19" s="52"/>
       <c r="K19" s="53"/>
     </row>
-    <row r="20" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="91"/>
+    <row r="20" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="102"/>
       <c r="B20" s="44" t="s">
         <v>35</v>
       </c>
@@ -3569,8 +3578,8 @@
       <c r="J20" s="34"/>
       <c r="K20" s="35"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="91"/>
+    <row r="21" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A21" s="102"/>
       <c r="B21" s="46" t="s">
         <v>34</v>
       </c>
@@ -3588,8 +3597,8 @@
       <c r="J21" s="52"/>
       <c r="K21" s="53"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="91"/>
+    <row r="22" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A22" s="102"/>
       <c r="B22" s="44" t="s">
         <v>34</v>
       </c>
@@ -3607,8 +3616,8 @@
       <c r="J22" s="34"/>
       <c r="K22" s="35"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="91"/>
+    <row r="23" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A23" s="102"/>
       <c r="B23" s="46" t="s">
         <v>36</v>
       </c>
@@ -3626,8 +3635,8 @@
       <c r="J23" s="52"/>
       <c r="K23" s="53"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="91"/>
+    <row r="24" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A24" s="102"/>
       <c r="B24" s="44" t="s">
         <v>36</v>
       </c>
@@ -3645,8 +3654,8 @@
       <c r="J24" s="34"/>
       <c r="K24" s="35"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="91"/>
+    <row r="25" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A25" s="102"/>
       <c r="B25" s="46" t="s">
         <v>36</v>
       </c>
@@ -3664,8 +3673,8 @@
       <c r="J25" s="52"/>
       <c r="K25" s="53"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="91"/>
+    <row r="26" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A26" s="102"/>
       <c r="B26" s="44" t="s">
         <v>36</v>
       </c>
@@ -3683,8 +3692,8 @@
       <c r="J26" s="34"/>
       <c r="K26" s="35"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="91"/>
+    <row r="27" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A27" s="102"/>
       <c r="B27" s="46" t="s">
         <v>36</v>
       </c>
@@ -3702,8 +3711,8 @@
       <c r="J27" s="52"/>
       <c r="K27" s="53"/>
     </row>
-    <row r="28" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="92"/>
+    <row r="28" spans="1:11" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="103"/>
       <c r="B28" s="54" t="s">
         <v>36</v>
       </c>
@@ -3721,8 +3730,8 @@
       <c r="J28" s="58"/>
       <c r="K28" s="59"/>
     </row>
-    <row r="29" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="91" t="s">
+    <row r="29" spans="1:11" ht="15.6" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="102" t="s">
         <v>56</v>
       </c>
       <c r="B29" s="46" t="s">
@@ -3742,8 +3751,8 @@
       <c r="J29" s="52"/>
       <c r="K29" s="53"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="91"/>
+    <row r="30" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A30" s="102"/>
       <c r="B30" s="44" t="s">
         <v>37</v>
       </c>
@@ -3761,8 +3770,8 @@
       <c r="J30" s="34"/>
       <c r="K30" s="35"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="91"/>
+    <row r="31" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A31" s="102"/>
       <c r="B31" s="46" t="s">
         <v>37</v>
       </c>
@@ -3780,8 +3789,8 @@
       <c r="J31" s="52"/>
       <c r="K31" s="53"/>
     </row>
-    <row r="32" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="91"/>
+    <row r="32" spans="1:11" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="102"/>
       <c r="B32" s="44" t="s">
         <v>37</v>
       </c>
@@ -3799,8 +3808,8 @@
       <c r="J32" s="34"/>
       <c r="K32" s="35"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="91"/>
+    <row r="33" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A33" s="102"/>
       <c r="B33" s="46" t="s">
         <v>37</v>
       </c>
@@ -3818,8 +3827,8 @@
       <c r="J33" s="52"/>
       <c r="K33" s="53"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="91"/>
+    <row r="34" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A34" s="102"/>
       <c r="B34" s="44" t="s">
         <v>37</v>
       </c>
@@ -3837,8 +3846,8 @@
       <c r="J34" s="34"/>
       <c r="K34" s="35"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="91"/>
+    <row r="35" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A35" s="102"/>
       <c r="B35" s="46" t="s">
         <v>38</v>
       </c>
@@ -3856,8 +3865,8 @@
       <c r="J35" s="52"/>
       <c r="K35" s="53"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="91"/>
+    <row r="36" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A36" s="102"/>
       <c r="B36" s="44" t="s">
         <v>38</v>
       </c>
@@ -3875,8 +3884,8 @@
       <c r="J36" s="34"/>
       <c r="K36" s="35"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="91"/>
+    <row r="37" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A37" s="102"/>
       <c r="B37" s="46" t="s">
         <v>38</v>
       </c>
@@ -3894,8 +3903,8 @@
       <c r="J37" s="52"/>
       <c r="K37" s="53"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="91"/>
+    <row r="38" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A38" s="102"/>
       <c r="B38" s="44" t="s">
         <v>38</v>
       </c>
@@ -3913,8 +3922,8 @@
       <c r="J38" s="34"/>
       <c r="K38" s="35"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="91"/>
+    <row r="39" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A39" s="102"/>
       <c r="B39" s="46" t="s">
         <v>38</v>
       </c>
@@ -3932,8 +3941,8 @@
       <c r="J39" s="52"/>
       <c r="K39" s="53"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="91"/>
+    <row r="40" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A40" s="102"/>
       <c r="B40" s="44" t="s">
         <v>38</v>
       </c>
@@ -3951,8 +3960,8 @@
       <c r="J40" s="34"/>
       <c r="K40" s="35"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="91"/>
+    <row r="41" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A41" s="102"/>
       <c r="B41" s="46" t="s">
         <v>39</v>
       </c>
@@ -3970,8 +3979,8 @@
       <c r="J41" s="52"/>
       <c r="K41" s="53"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="91"/>
+    <row r="42" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A42" s="102"/>
       <c r="B42" s="44" t="s">
         <v>39</v>
       </c>
@@ -3989,8 +3998,8 @@
       <c r="J42" s="34"/>
       <c r="K42" s="35"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="91"/>
+    <row r="43" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A43" s="102"/>
       <c r="B43" s="46" t="s">
         <v>40</v>
       </c>
@@ -4008,8 +4017,8 @@
       <c r="J43" s="52"/>
       <c r="K43" s="53"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="91"/>
+    <row r="44" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A44" s="102"/>
       <c r="B44" s="44" t="s">
         <v>40</v>
       </c>
@@ -4027,8 +4036,8 @@
       <c r="J44" s="34"/>
       <c r="K44" s="35"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="91"/>
+    <row r="45" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A45" s="102"/>
       <c r="B45" s="46" t="s">
         <v>40</v>
       </c>
@@ -4046,8 +4055,8 @@
       <c r="J45" s="52"/>
       <c r="K45" s="53"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="91"/>
+    <row r="46" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A46" s="102"/>
       <c r="B46" s="44" t="s">
         <v>40</v>
       </c>
@@ -4065,8 +4074,8 @@
       <c r="J46" s="34"/>
       <c r="K46" s="35"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="91"/>
+    <row r="47" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A47" s="102"/>
       <c r="B47" s="46" t="s">
         <v>40</v>
       </c>
@@ -4084,8 +4093,8 @@
       <c r="J47" s="52"/>
       <c r="K47" s="53"/>
     </row>
-    <row r="48" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="92"/>
+    <row r="48" spans="1:11" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="103"/>
       <c r="B48" s="54" t="s">
         <v>40</v>
       </c>
@@ -4103,8 +4112,8 @@
       <c r="J48" s="58"/>
       <c r="K48" s="59"/>
     </row>
-    <row r="49" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="91" t="s">
+    <row r="49" spans="1:11" ht="15.6" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="102" t="s">
         <v>57</v>
       </c>
       <c r="B49" s="46" t="s">
@@ -4124,8 +4133,8 @@
       <c r="J49" s="52"/>
       <c r="K49" s="53"/>
     </row>
-    <row r="50" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="91"/>
+    <row r="50" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="102"/>
       <c r="B50" s="44" t="s">
         <v>42</v>
       </c>
@@ -4143,8 +4152,8 @@
       <c r="J50" s="34"/>
       <c r="K50" s="35"/>
     </row>
-    <row r="51" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="92"/>
+    <row r="51" spans="1:11" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="103"/>
       <c r="B51" s="60" t="s">
         <v>43</v>
       </c>
@@ -4162,8 +4171,8 @@
       <c r="J51" s="66"/>
       <c r="K51" s="67"/>
     </row>
-    <row r="52" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="91" t="s">
+    <row r="52" spans="1:11" ht="15.6" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="102" t="s">
         <v>58</v>
       </c>
       <c r="B52" s="44" t="s">
@@ -4183,8 +4192,8 @@
       <c r="J52" s="34"/>
       <c r="K52" s="35"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="91"/>
+    <row r="53" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A53" s="102"/>
       <c r="B53" s="46" t="s">
         <v>45</v>
       </c>
@@ -4202,8 +4211,8 @@
       <c r="J53" s="52"/>
       <c r="K53" s="53"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="91"/>
+    <row r="54" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A54" s="102"/>
       <c r="B54" s="44" t="s">
         <v>46</v>
       </c>
@@ -4221,8 +4230,8 @@
       <c r="J54" s="34"/>
       <c r="K54" s="35"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" s="91"/>
+    <row r="55" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A55" s="102"/>
       <c r="B55" s="46" t="s">
         <v>62</v>
       </c>
@@ -4240,8 +4249,8 @@
       <c r="J55" s="52"/>
       <c r="K55" s="53"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A56" s="91"/>
+    <row r="56" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A56" s="102"/>
       <c r="B56" s="44" t="s">
         <v>62</v>
       </c>
@@ -4259,8 +4268,8 @@
       <c r="J56" s="34"/>
       <c r="K56" s="35"/>
     </row>
-    <row r="57" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="92"/>
+    <row r="57" spans="1:11" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="103"/>
       <c r="B57" s="60" t="s">
         <v>62</v>
       </c>
@@ -4278,8 +4287,8 @@
       <c r="J57" s="66"/>
       <c r="K57" s="67"/>
     </row>
-    <row r="58" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="91" t="s">
+    <row r="58" spans="1:11" ht="15.6" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="102" t="s">
         <v>59</v>
       </c>
       <c r="B58" s="44" t="s">
@@ -4299,8 +4308,8 @@
       <c r="J58" s="34"/>
       <c r="K58" s="35"/>
     </row>
-    <row r="59" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="92"/>
+    <row r="59" spans="1:11" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="103"/>
       <c r="B59" s="60" t="s">
         <v>48</v>
       </c>
@@ -4318,8 +4327,8 @@
       <c r="J59" s="66"/>
       <c r="K59" s="67"/>
     </row>
-    <row r="60" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="91" t="s">
+    <row r="60" spans="1:11" ht="15.6" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="102" t="s">
         <v>60</v>
       </c>
       <c r="B60" s="44" t="s">
@@ -4339,8 +4348,8 @@
       <c r="J60" s="34"/>
       <c r="K60" s="35"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A61" s="91"/>
+    <row r="61" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A61" s="102"/>
       <c r="B61" s="46" t="s">
         <v>49</v>
       </c>
@@ -4358,8 +4367,8 @@
       <c r="J61" s="52"/>
       <c r="K61" s="53"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A62" s="91"/>
+    <row r="62" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A62" s="102"/>
       <c r="B62" s="44" t="s">
         <v>50</v>
       </c>
@@ -4377,8 +4386,8 @@
       <c r="J62" s="34"/>
       <c r="K62" s="35"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A63" s="91"/>
+    <row r="63" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A63" s="102"/>
       <c r="B63" s="46" t="s">
         <v>50</v>
       </c>
@@ -4396,8 +4405,8 @@
       <c r="J63" s="52"/>
       <c r="K63" s="53"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A64" s="91"/>
+    <row r="64" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A64" s="102"/>
       <c r="B64" s="44" t="s">
         <v>50</v>
       </c>
@@ -4415,8 +4424,8 @@
       <c r="J64" s="34"/>
       <c r="K64" s="35"/>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A65" s="91"/>
+    <row r="65" spans="1:12" ht="15" x14ac:dyDescent="0.3">
+      <c r="A65" s="102"/>
       <c r="B65" s="46" t="s">
         <v>50</v>
       </c>
@@ -4434,8 +4443,8 @@
       <c r="J65" s="52"/>
       <c r="K65" s="53"/>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A66" s="91"/>
+    <row r="66" spans="1:12" ht="15" x14ac:dyDescent="0.3">
+      <c r="A66" s="102"/>
       <c r="B66" s="44" t="s">
         <v>50</v>
       </c>
@@ -4453,8 +4462,8 @@
       <c r="J66" s="34"/>
       <c r="K66" s="35"/>
     </row>
-    <row r="67" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="92"/>
+    <row r="67" spans="1:12" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="103"/>
       <c r="B67" s="60" t="s">
         <v>50</v>
       </c>
@@ -4472,8 +4481,8 @@
       <c r="J67" s="66"/>
       <c r="K67" s="67"/>
     </row>
-    <row r="68" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="91" t="s">
+    <row r="68" spans="1:12" ht="15.6" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="102" t="s">
         <v>61</v>
       </c>
       <c r="B68" s="44" t="s">
@@ -4493,8 +4502,8 @@
       <c r="J68" s="34"/>
       <c r="K68" s="35"/>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A69" s="91"/>
+    <row r="69" spans="1:12" ht="15" x14ac:dyDescent="0.3">
+      <c r="A69" s="102"/>
       <c r="B69" s="46" t="s">
         <v>51</v>
       </c>
@@ -4512,8 +4521,8 @@
       <c r="J69" s="52"/>
       <c r="K69" s="53"/>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A70" s="91"/>
+    <row r="70" spans="1:12" ht="15" x14ac:dyDescent="0.3">
+      <c r="A70" s="102"/>
       <c r="B70" s="44" t="s">
         <v>51</v>
       </c>
@@ -4531,8 +4540,8 @@
       <c r="J70" s="34"/>
       <c r="K70" s="35"/>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A71" s="91"/>
+    <row r="71" spans="1:12" ht="15" x14ac:dyDescent="0.3">
+      <c r="A71" s="102"/>
       <c r="B71" s="46" t="s">
         <v>63</v>
       </c>
@@ -4550,8 +4559,8 @@
       <c r="J71" s="52"/>
       <c r="K71" s="53"/>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A72" s="91"/>
+    <row r="72" spans="1:12" ht="15" x14ac:dyDescent="0.3">
+      <c r="A72" s="102"/>
       <c r="B72" s="44" t="s">
         <v>63</v>
       </c>
@@ -4569,8 +4578,8 @@
       <c r="J72" s="34"/>
       <c r="K72" s="35"/>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A73" s="91"/>
+    <row r="73" spans="1:12" ht="15" x14ac:dyDescent="0.3">
+      <c r="A73" s="102"/>
       <c r="B73" s="46" t="s">
         <v>63</v>
       </c>
@@ -4588,8 +4597,8 @@
       <c r="J73" s="52"/>
       <c r="K73" s="53"/>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A74" s="91"/>
+    <row r="74" spans="1:12" ht="15" x14ac:dyDescent="0.3">
+      <c r="A74" s="102"/>
       <c r="B74" s="44" t="s">
         <v>64</v>
       </c>
@@ -4607,8 +4616,8 @@
       <c r="J74" s="34"/>
       <c r="K74" s="35"/>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A75" s="91"/>
+    <row r="75" spans="1:12" ht="15" x14ac:dyDescent="0.3">
+      <c r="A75" s="102"/>
       <c r="B75" s="46" t="s">
         <v>64</v>
       </c>
@@ -4626,8 +4635,8 @@
       <c r="J75" s="52"/>
       <c r="K75" s="53"/>
     </row>
-    <row r="76" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="92"/>
+    <row r="76" spans="1:12" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A76" s="103"/>
       <c r="B76" s="54" t="s">
         <v>64</v>
       </c>
@@ -4645,7 +4654,7 @@
       <c r="J76" s="58"/>
       <c r="K76" s="59"/>
     </row>
-    <row r="77" spans="1:12" ht="16.149999999999999" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:12" ht="16.2" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D77" s="11">
         <f>SUM(D9:D76)</f>
         <v>162.5</v>
@@ -4656,30 +4665,30 @@
       </c>
       <c r="F77" s="12" t="str">
         <f>F78&amp;+ "/" &amp;+ $D$77</f>
-        <v>0/162.5</v>
+        <v>6/162.5</v>
       </c>
       <c r="G77" s="12" t="str">
         <f t="shared" ref="G77:K77" si="0">G78&amp;+ "/" &amp;+ $D$77</f>
-        <v>0/162.5</v>
+        <v>6/162.5</v>
       </c>
       <c r="H77" s="12" t="str">
         <f t="shared" si="0"/>
-        <v>0/162.5</v>
+        <v>6/162.5</v>
       </c>
       <c r="I77" s="12" t="str">
         <f t="shared" si="0"/>
-        <v>0/162.5</v>
+        <v>6/162.5</v>
       </c>
       <c r="J77" s="12" t="str">
         <f t="shared" si="0"/>
-        <v>0/162.5</v>
+        <v>6/162.5</v>
       </c>
       <c r="K77" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>0/162.5</v>
-      </c>
-    </row>
-    <row r="78" spans="1:12" ht="15" hidden="1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+        <v>6/162.5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" ht="15" hidden="1" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="D78" s="1">
         <f>SUM(D9:D76)</f>
         <v>162.5</v>
@@ -4690,31 +4699,31 @@
       </c>
       <c r="F78" s="1">
         <f>SUM(F9:F76)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G78" s="1">
         <f>SUM(G9:G76)+F78</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H78" s="1">
         <f>SUM(H9:H76)+G78</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I78" s="1">
         <f>SUM(I9:I76)+H78</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J78" s="1">
         <f>SUM(J9:J76)+I78</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K78" s="1">
         <f>SUM(K9:K76)+J78</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="L78" s="1"/>
     </row>
-    <row r="79" spans="1:12" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D79" s="1"/>
       <c r="E79" s="1">
         <f>D77</f>
@@ -4746,7 +4755,7 @@
       </c>
       <c r="L79" s="1"/>
     </row>
-    <row r="80" spans="1:12" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D80" s="1"/>
       <c r="E80" s="1">
         <v>0</v>
@@ -4756,7 +4765,7 @@
         <v>162.5</v>
       </c>
     </row>
-    <row r="81" spans="4:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="4:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="D81" s="1"/>
       <c r="E81" s="5" t="s">
         <v>14</v>
@@ -4781,7 +4790,7 @@
       <c r="S81" s="4"/>
       <c r="T81" s="4"/>
     </row>
-    <row r="82" spans="4:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="4:20" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="D82" s="1"/>
       <c r="E82" s="1"/>
       <c r="F82" s="1"/>
@@ -4789,19 +4798,13 @@
       <c r="H82" s="1"/>
       <c r="I82" s="1"/>
     </row>
-    <row r="100" spans="18:18" x14ac:dyDescent="0.25">
+    <row r="100" spans="18:18" x14ac:dyDescent="0.3">
       <c r="R100" s="2" t="s">
         <v>30</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="F7:K7"/>
-    <mergeCell ref="B7:B8"/>
     <mergeCell ref="A60:A67"/>
     <mergeCell ref="A68:A76"/>
     <mergeCell ref="A9:A14"/>
@@ -4810,6 +4813,12 @@
     <mergeCell ref="A58:A59"/>
     <mergeCell ref="A52:A57"/>
     <mergeCell ref="A49:A51"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="F7:K7"/>
+    <mergeCell ref="B7:B8"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Number" error="Please Enter Only Numbers. You may use .5 increments. " sqref="D9:D76">
@@ -4846,15 +4855,15 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="78" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="23" t="s">
         <v>65</v>
       </c>
@@ -4862,8 +4871,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:4" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="69" t="s">
         <v>76</v>
       </c>
@@ -4877,7 +4886,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="71" t="s">
         <v>53</v>
       </c>
@@ -4891,7 +4900,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="72" t="s">
         <v>55</v>
       </c>
@@ -4905,7 +4914,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="72" t="s">
         <v>56</v>
       </c>
@@ -4919,7 +4928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="72" t="s">
         <v>66</v>
       </c>
@@ -4933,7 +4942,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="72" t="s">
         <v>67</v>
       </c>
@@ -4947,7 +4956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="72" t="s">
         <v>68</v>
       </c>
@@ -4961,7 +4970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="72" t="s">
         <v>69</v>
       </c>
@@ -4975,7 +4984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="72" t="s">
         <v>70</v>
       </c>
@@ -4989,7 +4998,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="72" t="s">
         <v>71</v>
       </c>
@@ -5003,7 +5012,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="72" t="s">
         <v>72</v>
       </c>
@@ -5017,7 +5026,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="72" t="s">
         <v>73</v>
       </c>
@@ -5031,7 +5040,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="72" t="s">
         <v>74</v>
       </c>
@@ -5045,7 +5054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="73" t="s">
         <v>75</v>
       </c>
@@ -5072,562 +5081,565 @@
       <selection activeCell="K15" sqref="K15:L17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="20.7109375" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" customWidth="1"/>
-    <col min="5" max="6" width="20.7109375" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" customWidth="1"/>
-    <col min="8" max="9" width="20.7109375" customWidth="1"/>
-    <col min="10" max="10" width="8.7109375" customWidth="1"/>
-    <col min="11" max="12" width="20.7109375" customWidth="1"/>
-    <col min="13" max="13" width="8.7109375" customWidth="1"/>
+    <col min="1" max="2" width="20.6640625" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" customWidth="1"/>
+    <col min="5" max="6" width="20.6640625" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" customWidth="1"/>
+    <col min="8" max="9" width="20.6640625" customWidth="1"/>
+    <col min="10" max="10" width="8.6640625" customWidth="1"/>
+    <col min="11" max="12" width="20.6640625" customWidth="1"/>
+    <col min="13" max="13" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="29.25" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="137" t="s">
+    <row r="1" spans="1:13" ht="29.4" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="105" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="138"/>
-      <c r="C1" s="139"/>
+      <c r="B1" s="106"/>
+      <c r="C1" s="107"/>
       <c r="D1" s="81"/>
-      <c r="E1" s="137" t="s">
+      <c r="E1" s="105" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="138"/>
-      <c r="G1" s="138"/>
-      <c r="H1" s="138"/>
-      <c r="I1" s="138"/>
-      <c r="J1" s="138"/>
-      <c r="K1" s="138"/>
-      <c r="L1" s="138"/>
-      <c r="M1" s="139"/>
-    </row>
-    <row r="2" spans="1:13" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="140"/>
-      <c r="B2" s="141"/>
-      <c r="C2" s="142"/>
+      <c r="F1" s="106"/>
+      <c r="G1" s="106"/>
+      <c r="H1" s="106"/>
+      <c r="I1" s="106"/>
+      <c r="J1" s="106"/>
+      <c r="K1" s="106"/>
+      <c r="L1" s="106"/>
+      <c r="M1" s="107"/>
+    </row>
+    <row r="2" spans="1:13" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="108"/>
+      <c r="B2" s="109"/>
+      <c r="C2" s="110"/>
       <c r="D2" s="81"/>
-      <c r="E2" s="140" t="s">
+      <c r="E2" s="108" t="s">
         <v>80</v>
       </c>
-      <c r="F2" s="141"/>
-      <c r="G2" s="142"/>
-      <c r="H2" s="141" t="s">
+      <c r="F2" s="109"/>
+      <c r="G2" s="110"/>
+      <c r="H2" s="109" t="s">
         <v>81</v>
       </c>
-      <c r="I2" s="141"/>
-      <c r="J2" s="142"/>
-      <c r="K2" s="141" t="s">
+      <c r="I2" s="109"/>
+      <c r="J2" s="110"/>
+      <c r="K2" s="109" t="s">
         <v>82</v>
       </c>
-      <c r="L2" s="141"/>
-      <c r="M2" s="142"/>
-    </row>
-    <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="129" t="str">
+      <c r="L2" s="109"/>
+      <c r="M2" s="110"/>
+    </row>
+    <row r="3" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="111" t="str">
         <f>Backlog!A11</f>
         <v>As a User, I want to be able to detect Par. in Chemical Diagram, so I can work with polymers</v>
       </c>
-      <c r="B3" s="130"/>
+      <c r="B3" s="112"/>
       <c r="C3" s="87">
         <f>Backlog!C11</f>
         <v>20</v>
       </c>
-      <c r="E3" s="111" t="str">
+      <c r="E3" s="125" t="str">
         <f>Backlog!A4</f>
         <v>As a Developer, I need an architectural overview of OSRA’s processing, so I can understand the code base.</v>
       </c>
-      <c r="F3" s="112"/>
+      <c r="F3" s="126"/>
       <c r="G3" s="87">
         <f>Backlog!C4</f>
         <v>13</v>
       </c>
-      <c r="H3" s="105"/>
-      <c r="I3" s="106"/>
+      <c r="H3" s="137"/>
+      <c r="I3" s="138"/>
       <c r="J3" s="86"/>
-      <c r="K3" s="105"/>
-      <c r="L3" s="106"/>
+      <c r="K3" s="137"/>
+      <c r="L3" s="138"/>
       <c r="M3" s="86"/>
     </row>
-    <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="131"/>
-      <c r="B4" s="132"/>
+    <row r="4" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="113"/>
+      <c r="B4" s="114"/>
       <c r="C4" s="88" t="str">
         <f>Backlog!B11</f>
         <v>M</v>
       </c>
-      <c r="E4" s="113"/>
-      <c r="F4" s="114"/>
+      <c r="E4" s="127"/>
+      <c r="F4" s="128"/>
       <c r="G4" s="88" t="str">
         <f>Backlog!B4</f>
         <v>M</v>
       </c>
-      <c r="H4" s="107"/>
-      <c r="I4" s="108"/>
+      <c r="H4" s="139"/>
+      <c r="I4" s="140"/>
       <c r="J4" s="84"/>
-      <c r="K4" s="107"/>
-      <c r="L4" s="108"/>
+      <c r="K4" s="139"/>
+      <c r="L4" s="140"/>
       <c r="M4" s="84"/>
     </row>
-    <row r="5" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="133"/>
-      <c r="B5" s="134"/>
+    <row r="5" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="115"/>
+      <c r="B5" s="116"/>
       <c r="C5" s="89"/>
-      <c r="E5" s="115"/>
-      <c r="F5" s="116"/>
+      <c r="E5" s="129"/>
+      <c r="F5" s="130"/>
       <c r="G5" s="89"/>
-      <c r="H5" s="109"/>
-      <c r="I5" s="110"/>
+      <c r="H5" s="141"/>
+      <c r="I5" s="142"/>
       <c r="J5" s="85"/>
-      <c r="K5" s="109"/>
-      <c r="L5" s="110"/>
+      <c r="K5" s="141"/>
+      <c r="L5" s="142"/>
       <c r="M5" s="85"/>
     </row>
-    <row r="6" spans="1:13" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="129" t="str">
+    <row r="6" spans="1:13" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="111" t="str">
         <f>Backlog!A12</f>
         <v>As a User, I want to be able to detect Brackets in Chemical Diagrams, so I can work with polymers</v>
       </c>
-      <c r="B6" s="130"/>
+      <c r="B6" s="112"/>
       <c r="C6" s="87">
         <f>Backlog!C12</f>
         <v>20</v>
       </c>
-      <c r="E6" s="111" t="str">
+      <c r="E6" s="125" t="str">
         <f>Backlog!A5</f>
         <v>As a Developer, I need to review each aspect of OSRA’s architecture, so I can understand the code base.</v>
       </c>
-      <c r="F6" s="112"/>
+      <c r="F6" s="126"/>
       <c r="G6" s="87">
         <f>Backlog!C5</f>
         <v>20</v>
       </c>
-      <c r="H6" s="105"/>
-      <c r="I6" s="106"/>
+      <c r="H6" s="137"/>
+      <c r="I6" s="138"/>
       <c r="J6" s="86"/>
-      <c r="K6" s="105"/>
-      <c r="L6" s="106"/>
+      <c r="K6" s="137"/>
+      <c r="L6" s="138"/>
       <c r="M6" s="86"/>
     </row>
-    <row r="7" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="131"/>
-      <c r="B7" s="132"/>
+    <row r="7" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="113"/>
+      <c r="B7" s="114"/>
       <c r="C7" s="88" t="str">
         <f>Backlog!B12</f>
         <v>S</v>
       </c>
-      <c r="E7" s="113"/>
-      <c r="F7" s="114"/>
+      <c r="E7" s="127"/>
+      <c r="F7" s="128"/>
       <c r="G7" s="88" t="str">
         <f>Backlog!B5</f>
         <v>M</v>
       </c>
-      <c r="H7" s="107"/>
-      <c r="I7" s="108"/>
+      <c r="H7" s="139"/>
+      <c r="I7" s="140"/>
       <c r="J7" s="84"/>
-      <c r="K7" s="107"/>
-      <c r="L7" s="108"/>
+      <c r="K7" s="139"/>
+      <c r="L7" s="140"/>
       <c r="M7" s="84"/>
     </row>
-    <row r="8" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="133"/>
-      <c r="B8" s="134"/>
+    <row r="8" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="115"/>
+      <c r="B8" s="116"/>
       <c r="C8" s="89"/>
-      <c r="E8" s="115"/>
-      <c r="F8" s="116"/>
+      <c r="E8" s="129"/>
+      <c r="F8" s="130"/>
       <c r="G8" s="89"/>
-      <c r="H8" s="109"/>
-      <c r="I8" s="110"/>
+      <c r="H8" s="141"/>
+      <c r="I8" s="142"/>
       <c r="J8" s="85"/>
-      <c r="K8" s="109"/>
-      <c r="L8" s="110"/>
+      <c r="K8" s="141"/>
+      <c r="L8" s="142"/>
       <c r="M8" s="85"/>
     </row>
-    <row r="9" spans="1:13" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="129" t="str">
+    <row r="9" spans="1:13" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="111" t="str">
         <f>Backlog!A13</f>
         <v>As a User, I want to be able to detect subscripts for polymer diagrams, so I can work with polymers</v>
       </c>
-      <c r="B9" s="130"/>
+      <c r="B9" s="112"/>
       <c r="C9" s="87">
         <f>Backlog!C13</f>
         <v>13</v>
       </c>
-      <c r="E9" s="111" t="str">
+      <c r="E9" s="125" t="str">
         <f>Backlog!A6</f>
         <v>As a Developer, I need to get a basic grasp of O-Chem, so I can better understand use cases.</v>
       </c>
-      <c r="F9" s="112"/>
+      <c r="F9" s="126"/>
       <c r="G9" s="87">
         <f>Backlog!C6</f>
         <v>5</v>
       </c>
-      <c r="H9" s="105"/>
-      <c r="I9" s="106"/>
+      <c r="H9" s="137"/>
+      <c r="I9" s="138"/>
       <c r="J9" s="86"/>
-      <c r="K9" s="105"/>
-      <c r="L9" s="106"/>
+      <c r="K9" s="137"/>
+      <c r="L9" s="138"/>
       <c r="M9" s="86"/>
     </row>
-    <row r="10" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="131"/>
-      <c r="B10" s="132"/>
+    <row r="10" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="113"/>
+      <c r="B10" s="114"/>
       <c r="C10" s="88" t="str">
         <f>Backlog!B13</f>
         <v>M</v>
       </c>
-      <c r="E10" s="113"/>
-      <c r="F10" s="114"/>
+      <c r="E10" s="127"/>
+      <c r="F10" s="128"/>
       <c r="G10" s="88" t="str">
         <f>Backlog!B6</f>
         <v>M</v>
       </c>
-      <c r="H10" s="107"/>
-      <c r="I10" s="108"/>
+      <c r="H10" s="139"/>
+      <c r="I10" s="140"/>
       <c r="J10" s="84"/>
-      <c r="K10" s="107"/>
-      <c r="L10" s="108"/>
+      <c r="K10" s="139"/>
+      <c r="L10" s="140"/>
       <c r="M10" s="84"/>
     </row>
-    <row r="11" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="133"/>
-      <c r="B11" s="134"/>
+    <row r="11" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="115"/>
+      <c r="B11" s="116"/>
       <c r="C11" s="89"/>
-      <c r="E11" s="115"/>
-      <c r="F11" s="116"/>
+      <c r="E11" s="129"/>
+      <c r="F11" s="130"/>
       <c r="G11" s="89"/>
-      <c r="H11" s="109"/>
-      <c r="I11" s="110"/>
+      <c r="H11" s="141"/>
+      <c r="I11" s="142"/>
       <c r="J11" s="85"/>
-      <c r="K11" s="109"/>
-      <c r="L11" s="110"/>
+      <c r="K11" s="141"/>
+      <c r="L11" s="142"/>
       <c r="M11" s="85"/>
     </row>
-    <row r="12" spans="1:13" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="129" t="str">
+    <row r="12" spans="1:13" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="111" t="str">
         <f>Backlog!A14</f>
         <v>As a User, I want to be able to detect “R-Notation”, so I can work with polymers</v>
       </c>
-      <c r="B12" s="130"/>
+      <c r="B12" s="112"/>
       <c r="C12" s="87" t="str">
         <f>Backlog!C14</f>
         <v>INF</v>
       </c>
-      <c r="E12" s="111" t="str">
+      <c r="E12" s="125" t="str">
         <f>Backlog!A7</f>
         <v>As a Developer, I need workflow and processes for the github repo, so I can collaborate on code</v>
       </c>
-      <c r="F12" s="112"/>
+      <c r="F12" s="126"/>
       <c r="G12" s="87">
         <f>Backlog!C7</f>
         <v>5</v>
       </c>
-      <c r="H12" s="105"/>
-      <c r="I12" s="106"/>
+      <c r="H12" s="137"/>
+      <c r="I12" s="138"/>
       <c r="J12" s="86"/>
-      <c r="K12" s="105"/>
-      <c r="L12" s="106"/>
+      <c r="K12" s="137"/>
+      <c r="L12" s="138"/>
       <c r="M12" s="86"/>
     </row>
-    <row r="13" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="131"/>
-      <c r="B13" s="132"/>
+    <row r="13" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="113"/>
+      <c r="B13" s="114"/>
       <c r="C13" s="88" t="str">
         <f>Backlog!B14</f>
         <v>W</v>
       </c>
-      <c r="E13" s="113"/>
-      <c r="F13" s="114"/>
+      <c r="E13" s="127"/>
+      <c r="F13" s="128"/>
       <c r="G13" s="88" t="str">
         <f>Backlog!B7</f>
         <v>M</v>
       </c>
-      <c r="H13" s="107"/>
-      <c r="I13" s="108"/>
+      <c r="H13" s="139"/>
+      <c r="I13" s="140"/>
       <c r="J13" s="84"/>
-      <c r="K13" s="107"/>
-      <c r="L13" s="108"/>
+      <c r="K13" s="139"/>
+      <c r="L13" s="140"/>
       <c r="M13" s="84"/>
     </row>
-    <row r="14" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="135"/>
-      <c r="B14" s="136"/>
+    <row r="14" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="117"/>
+      <c r="B14" s="118"/>
       <c r="C14" s="90"/>
-      <c r="E14" s="115"/>
-      <c r="F14" s="116"/>
+      <c r="E14" s="129"/>
+      <c r="F14" s="130"/>
       <c r="G14" s="89"/>
-      <c r="H14" s="109"/>
-      <c r="I14" s="110"/>
+      <c r="H14" s="141"/>
+      <c r="I14" s="142"/>
       <c r="J14" s="85"/>
-      <c r="K14" s="109"/>
-      <c r="L14" s="110"/>
+      <c r="K14" s="141"/>
+      <c r="L14" s="142"/>
       <c r="M14" s="85"/>
     </row>
-    <row r="15" spans="1:13" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="123"/>
-      <c r="B15" s="124"/>
+    <row r="15" spans="1:13" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="119"/>
+      <c r="B15" s="120"/>
       <c r="C15" s="87"/>
-      <c r="E15" s="111" t="str">
+      <c r="E15" s="125" t="str">
         <f>Backlog!A8</f>
         <v>As a Developer, I need a testing enviroment and test documentation, so I can better contribute to the codebase</v>
       </c>
-      <c r="F15" s="112"/>
+      <c r="F15" s="126"/>
       <c r="G15" s="87">
         <f>Backlog!C8</f>
         <v>20</v>
       </c>
-      <c r="H15" s="105"/>
-      <c r="I15" s="106"/>
+      <c r="H15" s="137"/>
+      <c r="I15" s="138"/>
       <c r="J15" s="86"/>
-      <c r="K15" s="105"/>
-      <c r="L15" s="106"/>
+      <c r="K15" s="137"/>
+      <c r="L15" s="138"/>
       <c r="M15" s="86"/>
     </row>
-    <row r="16" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="125"/>
-      <c r="B16" s="126"/>
+    <row r="16" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="121"/>
+      <c r="B16" s="122"/>
       <c r="C16" s="88"/>
-      <c r="E16" s="113"/>
-      <c r="F16" s="114"/>
+      <c r="E16" s="127"/>
+      <c r="F16" s="128"/>
       <c r="G16" s="88" t="str">
         <f>Backlog!B8</f>
         <v>M</v>
       </c>
-      <c r="H16" s="107"/>
-      <c r="I16" s="108"/>
+      <c r="H16" s="139"/>
+      <c r="I16" s="140"/>
       <c r="J16" s="84"/>
-      <c r="K16" s="107"/>
-      <c r="L16" s="108"/>
+      <c r="K16" s="139"/>
+      <c r="L16" s="140"/>
       <c r="M16" s="84"/>
     </row>
-    <row r="17" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="127"/>
-      <c r="B17" s="128"/>
+    <row r="17" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="123"/>
+      <c r="B17" s="124"/>
       <c r="C17" s="89"/>
-      <c r="E17" s="115"/>
-      <c r="F17" s="116"/>
+      <c r="E17" s="129"/>
+      <c r="F17" s="130"/>
       <c r="G17" s="89"/>
-      <c r="H17" s="109"/>
-      <c r="I17" s="110"/>
+      <c r="H17" s="141"/>
+      <c r="I17" s="142"/>
       <c r="J17" s="85"/>
-      <c r="K17" s="109"/>
-      <c r="L17" s="110"/>
+      <c r="K17" s="141"/>
+      <c r="L17" s="142"/>
       <c r="M17" s="85"/>
     </row>
-    <row r="18" spans="1:13" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="123"/>
-      <c r="B18" s="124"/>
+    <row r="18" spans="1:13" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="119"/>
+      <c r="B18" s="120"/>
       <c r="C18" s="87"/>
-      <c r="E18" s="111" t="str">
+      <c r="E18" s="125" t="str">
         <f>Backlog!A9</f>
         <v>As a Developer, I need to have consolidated documentation from other developers, so I can better contribute to the codebase</v>
       </c>
-      <c r="F18" s="112"/>
+      <c r="F18" s="126"/>
       <c r="G18" s="87">
         <f>Backlog!C9</f>
         <v>13</v>
       </c>
-      <c r="H18" s="105"/>
-      <c r="I18" s="106"/>
+      <c r="H18" s="137"/>
+      <c r="I18" s="138"/>
       <c r="J18" s="86"/>
-      <c r="K18" s="105"/>
-      <c r="L18" s="106"/>
+      <c r="K18" s="137"/>
+      <c r="L18" s="138"/>
       <c r="M18" s="86"/>
     </row>
-    <row r="19" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="125"/>
-      <c r="B19" s="126"/>
+    <row r="19" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="121"/>
+      <c r="B19" s="122"/>
       <c r="C19" s="88"/>
-      <c r="E19" s="113"/>
-      <c r="F19" s="114"/>
+      <c r="E19" s="127"/>
+      <c r="F19" s="128"/>
       <c r="G19" s="88" t="str">
         <f>Backlog!B9</f>
         <v>M</v>
       </c>
-      <c r="H19" s="107"/>
-      <c r="I19" s="108"/>
+      <c r="H19" s="139"/>
+      <c r="I19" s="140"/>
       <c r="J19" s="84"/>
-      <c r="K19" s="107"/>
-      <c r="L19" s="108"/>
+      <c r="K19" s="139"/>
+      <c r="L19" s="140"/>
       <c r="M19" s="84"/>
     </row>
-    <row r="20" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="127"/>
-      <c r="B20" s="128"/>
+    <row r="20" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="123"/>
+      <c r="B20" s="124"/>
       <c r="C20" s="89"/>
-      <c r="E20" s="115"/>
-      <c r="F20" s="116"/>
+      <c r="E20" s="129"/>
+      <c r="F20" s="130"/>
       <c r="G20" s="89"/>
-      <c r="H20" s="109"/>
-      <c r="I20" s="110"/>
+      <c r="H20" s="141"/>
+      <c r="I20" s="142"/>
       <c r="J20" s="85"/>
-      <c r="K20" s="109"/>
-      <c r="L20" s="110"/>
+      <c r="K20" s="141"/>
+      <c r="L20" s="142"/>
       <c r="M20" s="85"/>
     </row>
-    <row r="21" spans="1:13" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="123"/>
-      <c r="B21" s="124"/>
+    <row r="21" spans="1:13" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="119"/>
+      <c r="B21" s="120"/>
       <c r="C21" s="87"/>
-      <c r="E21" s="111" t="str">
+      <c r="E21" s="125" t="str">
         <f>Backlog!A10</f>
         <v>As a Developer, I need to understand SMILES notation and .SD file structure, so I can desing the smile data structure.</v>
       </c>
-      <c r="F21" s="112"/>
+      <c r="F21" s="126"/>
       <c r="G21" s="87">
         <f>Backlog!C10</f>
         <v>5</v>
       </c>
-      <c r="H21" s="105"/>
-      <c r="I21" s="106"/>
+      <c r="H21" s="137"/>
+      <c r="I21" s="138"/>
       <c r="J21" s="86"/>
-      <c r="K21" s="105"/>
-      <c r="L21" s="106"/>
+      <c r="K21" s="137"/>
+      <c r="L21" s="138"/>
       <c r="M21" s="86"/>
     </row>
-    <row r="22" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="125"/>
-      <c r="B22" s="126"/>
+    <row r="22" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="121"/>
+      <c r="B22" s="122"/>
       <c r="C22" s="88"/>
-      <c r="E22" s="113"/>
-      <c r="F22" s="114"/>
+      <c r="E22" s="127"/>
+      <c r="F22" s="128"/>
       <c r="G22" s="88" t="str">
         <f>Backlog!B10</f>
         <v>M</v>
       </c>
-      <c r="H22" s="107"/>
-      <c r="I22" s="108"/>
+      <c r="H22" s="139"/>
+      <c r="I22" s="140"/>
       <c r="J22" s="84"/>
-      <c r="K22" s="107"/>
-      <c r="L22" s="108"/>
+      <c r="K22" s="139"/>
+      <c r="L22" s="140"/>
       <c r="M22" s="84"/>
     </row>
-    <row r="23" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="127"/>
-      <c r="B23" s="128"/>
+    <row r="23" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="123"/>
+      <c r="B23" s="124"/>
       <c r="C23" s="89"/>
-      <c r="E23" s="115"/>
-      <c r="F23" s="116"/>
+      <c r="E23" s="129"/>
+      <c r="F23" s="130"/>
       <c r="G23" s="89"/>
-      <c r="H23" s="109"/>
-      <c r="I23" s="110"/>
+      <c r="H23" s="141"/>
+      <c r="I23" s="142"/>
       <c r="J23" s="85"/>
-      <c r="K23" s="109"/>
-      <c r="L23" s="110"/>
+      <c r="K23" s="141"/>
+      <c r="L23" s="142"/>
       <c r="M23" s="85"/>
     </row>
-    <row r="24" spans="1:13" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="123"/>
-      <c r="B24" s="124"/>
+    <row r="24" spans="1:13" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="119"/>
+      <c r="B24" s="120"/>
       <c r="C24" s="87"/>
-      <c r="E24" s="111" t="str">
+      <c r="E24" s="125" t="str">
         <f>Backlog!A15</f>
         <v>As a User, I want to have a data structure for encoding polymers in “Smile Notation”, so I can work with polymers</v>
       </c>
-      <c r="F24" s="112"/>
+      <c r="F24" s="126"/>
       <c r="G24" s="87">
         <f>Backlog!C15</f>
         <v>13</v>
       </c>
-      <c r="H24" s="105"/>
-      <c r="I24" s="106"/>
+      <c r="H24" s="137"/>
+      <c r="I24" s="138"/>
       <c r="J24" s="86"/>
-      <c r="K24" s="105"/>
-      <c r="L24" s="106"/>
+      <c r="K24" s="137"/>
+      <c r="L24" s="138"/>
       <c r="M24" s="86"/>
     </row>
-    <row r="25" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="125"/>
-      <c r="B25" s="126"/>
+    <row r="25" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="121"/>
+      <c r="B25" s="122"/>
       <c r="C25" s="88"/>
-      <c r="E25" s="113"/>
-      <c r="F25" s="114"/>
+      <c r="E25" s="127"/>
+      <c r="F25" s="128"/>
       <c r="G25" s="88" t="str">
         <f>Backlog!B15</f>
         <v>M</v>
       </c>
-      <c r="H25" s="107"/>
-      <c r="I25" s="108"/>
+      <c r="H25" s="139"/>
+      <c r="I25" s="140"/>
       <c r="J25" s="84"/>
-      <c r="K25" s="107"/>
-      <c r="L25" s="108"/>
+      <c r="K25" s="139"/>
+      <c r="L25" s="140"/>
       <c r="M25" s="84"/>
     </row>
-    <row r="26" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="127"/>
-      <c r="B26" s="128"/>
+    <row r="26" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="123"/>
+      <c r="B26" s="124"/>
       <c r="C26" s="89"/>
-      <c r="E26" s="115"/>
-      <c r="F26" s="116"/>
+      <c r="E26" s="129"/>
+      <c r="F26" s="130"/>
       <c r="G26" s="89"/>
-      <c r="H26" s="109"/>
-      <c r="I26" s="110"/>
+      <c r="H26" s="141"/>
+      <c r="I26" s="142"/>
       <c r="J26" s="85"/>
-      <c r="K26" s="109"/>
-      <c r="L26" s="110"/>
+      <c r="K26" s="141"/>
+      <c r="L26" s="142"/>
       <c r="M26" s="85"/>
     </row>
-    <row r="27" spans="1:13" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="123"/>
-      <c r="B27" s="124"/>
+    <row r="27" spans="1:13" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="119"/>
+      <c r="B27" s="120"/>
       <c r="C27" s="87"/>
-      <c r="E27" s="117"/>
-      <c r="F27" s="118"/>
+      <c r="E27" s="131"/>
+      <c r="F27" s="132"/>
       <c r="G27" s="87"/>
-      <c r="H27" s="105"/>
-      <c r="I27" s="106"/>
+      <c r="H27" s="137"/>
+      <c r="I27" s="138"/>
       <c r="J27" s="86"/>
-      <c r="K27" s="105"/>
-      <c r="L27" s="106"/>
+      <c r="K27" s="137"/>
+      <c r="L27" s="138"/>
       <c r="M27" s="86"/>
     </row>
-    <row r="28" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="125"/>
-      <c r="B28" s="126"/>
+    <row r="28" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="121"/>
+      <c r="B28" s="122"/>
       <c r="C28" s="88"/>
-      <c r="E28" s="119"/>
-      <c r="F28" s="120"/>
+      <c r="E28" s="133"/>
+      <c r="F28" s="134"/>
       <c r="G28" s="88"/>
-      <c r="H28" s="107"/>
-      <c r="I28" s="108"/>
+      <c r="H28" s="139"/>
+      <c r="I28" s="140"/>
       <c r="J28" s="84"/>
-      <c r="K28" s="107"/>
-      <c r="L28" s="108"/>
+      <c r="K28" s="139"/>
+      <c r="L28" s="140"/>
       <c r="M28" s="84"/>
     </row>
-    <row r="29" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="127"/>
-      <c r="B29" s="128"/>
+    <row r="29" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="123"/>
+      <c r="B29" s="124"/>
       <c r="C29" s="89"/>
-      <c r="E29" s="121"/>
-      <c r="F29" s="122"/>
+      <c r="E29" s="135"/>
+      <c r="F29" s="136"/>
       <c r="G29" s="89"/>
-      <c r="H29" s="109"/>
-      <c r="I29" s="110"/>
+      <c r="H29" s="141"/>
+      <c r="I29" s="142"/>
       <c r="J29" s="85"/>
-      <c r="K29" s="109"/>
-      <c r="L29" s="110"/>
+      <c r="K29" s="141"/>
+      <c r="L29" s="142"/>
       <c r="M29" s="85"/>
     </row>
-    <row r="30" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="E1:M1"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="K2:M2"/>
-    <mergeCell ref="A1:C2"/>
-    <mergeCell ref="A3:B5"/>
-    <mergeCell ref="A6:B8"/>
-    <mergeCell ref="A9:B11"/>
-    <mergeCell ref="A12:B14"/>
-    <mergeCell ref="A15:B17"/>
-    <mergeCell ref="E3:F5"/>
-    <mergeCell ref="E6:F8"/>
-    <mergeCell ref="E9:F11"/>
-    <mergeCell ref="E12:F14"/>
-    <mergeCell ref="E15:F17"/>
+    <mergeCell ref="K18:L20"/>
+    <mergeCell ref="K21:L23"/>
+    <mergeCell ref="K24:L26"/>
+    <mergeCell ref="K27:L29"/>
+    <mergeCell ref="H21:I23"/>
+    <mergeCell ref="H24:I26"/>
+    <mergeCell ref="H27:I29"/>
+    <mergeCell ref="H18:I20"/>
+    <mergeCell ref="K3:L5"/>
+    <mergeCell ref="K6:L8"/>
+    <mergeCell ref="K9:L11"/>
+    <mergeCell ref="K12:L14"/>
+    <mergeCell ref="K15:L17"/>
+    <mergeCell ref="H3:I5"/>
+    <mergeCell ref="H6:I8"/>
+    <mergeCell ref="H9:I11"/>
+    <mergeCell ref="H12:I14"/>
+    <mergeCell ref="H15:I17"/>
     <mergeCell ref="E18:F20"/>
     <mergeCell ref="E21:F23"/>
     <mergeCell ref="E24:F26"/>
@@ -5636,24 +5648,21 @@
     <mergeCell ref="A24:B26"/>
     <mergeCell ref="A27:B29"/>
     <mergeCell ref="A18:B20"/>
-    <mergeCell ref="H3:I5"/>
-    <mergeCell ref="H6:I8"/>
-    <mergeCell ref="H9:I11"/>
-    <mergeCell ref="H12:I14"/>
-    <mergeCell ref="H15:I17"/>
-    <mergeCell ref="K3:L5"/>
-    <mergeCell ref="K6:L8"/>
-    <mergeCell ref="K9:L11"/>
-    <mergeCell ref="K12:L14"/>
-    <mergeCell ref="K15:L17"/>
-    <mergeCell ref="K18:L20"/>
-    <mergeCell ref="K21:L23"/>
-    <mergeCell ref="K24:L26"/>
-    <mergeCell ref="K27:L29"/>
-    <mergeCell ref="H21:I23"/>
-    <mergeCell ref="H24:I26"/>
-    <mergeCell ref="H27:I29"/>
-    <mergeCell ref="H18:I20"/>
+    <mergeCell ref="E3:F5"/>
+    <mergeCell ref="E6:F8"/>
+    <mergeCell ref="E9:F11"/>
+    <mergeCell ref="E12:F14"/>
+    <mergeCell ref="E15:F17"/>
+    <mergeCell ref="A3:B5"/>
+    <mergeCell ref="A6:B8"/>
+    <mergeCell ref="A9:B11"/>
+    <mergeCell ref="A12:B14"/>
+    <mergeCell ref="A15:B17"/>
+    <mergeCell ref="E1:M1"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="A1:C2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5667,20 +5676,20 @@
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9.109375" style="2"/>
     <col min="2" max="2" width="11" style="2" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26" style="2" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.7109375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="31.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="2"/>
+    <col min="6" max="6" width="20.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.6640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="31.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
         <v>11</v>
@@ -5701,7 +5710,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>22</v>
       </c>
@@ -5726,7 +5735,7 @@
         <v>24.5</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
@@ -5751,7 +5760,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>23</v>
       </c>
@@ -5776,7 +5785,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
         <v>24</v>
       </c>
@@ -5801,7 +5810,7 @@
         <v>24.5</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
         <v>52</v>
       </c>
@@ -5826,7 +5835,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
         <v>25</v>
       </c>
@@ -5864,18 +5873,18 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="143">
         <v>41557</v>
       </c>
@@ -5883,7 +5892,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="143"/>
       <c r="B3" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
Sprint Status as of 01/29/2014
</commit_message>
<xml_diff>
--- a/bookkeeping/Sprint1 BurnUp.xlsx
+++ b/bookkeeping/Sprint1 BurnUp.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11490" yWindow="0" windowWidth="16410" windowHeight="7815" tabRatio="601"/>
+    <workbookView xWindow="1020" yWindow="0" windowWidth="7476" windowHeight="3756" tabRatio="601"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks List" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="88">
   <si>
     <t>Sprint 1</t>
   </si>
@@ -408,7 +408,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="63">
+  <borders count="66">
     <border>
       <left/>
       <right/>
@@ -1230,6 +1230,39 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -1239,7 +1272,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="144">
+  <cellXfs count="151">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
@@ -1514,15 +1547,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1559,6 +1583,93 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1578,103 +1689,51 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="59" xfId="2" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="57" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="4" borderId="64" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="4" borderId="59" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="4" borderId="65" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="4" borderId="57" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1794,7 +1853,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Tasks List'!$E$80</c:f>
+              <c:f>'Tasks List'!$E$81</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1860,7 +1919,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Tasks List'!$E$77:$K$77</c:f>
+              <c:f>'Tasks List'!$E$78:$K$78</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1874,16 +1933,16 @@
                   <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>19</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>19</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>19</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>19</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1895,7 +1954,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Tasks List'!$F$80</c:f>
+              <c:f>'Tasks List'!$F$81</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1961,30 +2020,30 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Tasks List'!$E$78:$K$78</c:f>
+              <c:f>'Tasks List'!$E$79:$K$79</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>160</c:v>
+                  <c:v>162</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>160</c:v>
+                  <c:v>162</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>160</c:v>
+                  <c:v>162</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>160</c:v>
+                  <c:v>162</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>160</c:v>
+                  <c:v>162</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>160</c:v>
+                  <c:v>162</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>160</c:v>
+                  <c:v>162</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1996,7 +2055,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Tasks List'!$G$80</c:f>
+              <c:f>'Tasks List'!$G$81</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2065,7 +2124,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Tasks List'!$E$79:$K$79</c:f>
+              <c:f>'Tasks List'!$E$80:$K$80</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -2073,7 +2132,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>160</c:v>
+                  <c:v>162</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2105,11 +2164,11 @@
         </c:dropLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="260000424"/>
-        <c:axId val="259998072"/>
+        <c:axId val="255715648"/>
+        <c:axId val="255715256"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="260000424"/>
+        <c:axId val="255715648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2152,14 +2211,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="259998072"/>
+        <c:crossAx val="255715256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="259998072"/>
+        <c:axId val="255715256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2196,7 +2255,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="260000424"/>
+        <c:crossAx val="255715648"/>
         <c:crossesAt val="41548"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="10"/>
@@ -3175,24 +3234,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T99"/>
+  <dimension ref="A1:T100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+    <sheetView tabSelected="1" topLeftCell="B22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="47.42578125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="76.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" style="2" hidden="1" customWidth="1"/>
-    <col min="6" max="11" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="40.88671875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="76.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" style="2" hidden="1" customWidth="1"/>
+    <col min="6" max="11" width="11.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
@@ -3203,18 +3262,18 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="21"/>
       <c r="B2" s="22"/>
       <c r="D2" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="94" t="s">
+      <c r="F2" s="91" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="95"/>
-    </row>
-    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G2" s="92"/>
+    </row>
+    <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="18" t="s">
         <v>26</v>
       </c>
@@ -3223,7 +3282,7 @@
         <v>Nicholas</v>
       </c>
       <c r="F3" s="7" t="str">
-        <f>('Names-Hours'!H3) - (SUMIF(C9:C75,D3,D9:D75))&amp;+"/"&amp;+'Names-Hours'!D3</f>
+        <f>('Names-Hours'!H3) - (SUMIF(C9:C76,D3,D9:D76))&amp;+"/"&amp;+'Names-Hours'!D3</f>
         <v>-6.5/30</v>
       </c>
       <c r="G3" s="6" t="str">
@@ -3231,7 +3290,7 @@
         <v>Igor</v>
       </c>
       <c r="H3" s="7" t="str">
-        <f>('Names-Hours'!H3) -(SUMIF(C9:C75,G3,D9:D75)) &amp;+"/"&amp;+'Names-Hours'!D5</f>
+        <f>('Names-Hours'!H3) -(SUMIF(C9:C76,G3,D9:D76)) &amp;+"/"&amp;+'Names-Hours'!D5</f>
         <v>-3.5/30</v>
       </c>
       <c r="I3" s="6" t="str">
@@ -3239,11 +3298,11 @@
         <v>David</v>
       </c>
       <c r="J3" s="7" t="str">
-        <f>('Names-Hours'!H4) -(SUMIF(C9:C75,I3,D9:D75)) &amp;+"/"&amp;+ 'Names-Hours'!D7</f>
+        <f>('Names-Hours'!H4) -(SUMIF(C9:C76,I3,D9:D76)) &amp;+"/"&amp;+ 'Names-Hours'!D7</f>
         <v>3/30</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="19" t="s">
         <v>27</v>
       </c>
@@ -3253,7 +3312,7 @@
         <v>Konstantin</v>
       </c>
       <c r="F4" s="7" t="str">
-        <f>('Names-Hours'!H4) -(SUMIF(C9:C75,D4,D9:D75))&amp;+"/"&amp;+'Names-Hours'!D4</f>
+        <f>('Names-Hours'!H4) -(SUMIF(C9:C76,D4,D9:D76))&amp;+"/"&amp;+'Names-Hours'!D4</f>
         <v>-3/30</v>
       </c>
       <c r="G4" s="6" t="str">
@@ -3261,7 +3320,7 @@
         <v>Nathan</v>
       </c>
       <c r="H4" s="7" t="str">
-        <f>('Names-Hours'!H4) -(SUMIF(C9:C75,G4,D9:D75)) &amp;+"/"&amp;+'Names-Hours'!D6</f>
+        <f>('Names-Hours'!H4) -(SUMIF(C9:C76,G4,D9:D76)) &amp;+"/"&amp;+'Names-Hours'!D6</f>
         <v>-6.5/30</v>
       </c>
       <c r="I4" s="6" t="str">
@@ -3269,11 +3328,11 @@
         <v>Thomas</v>
       </c>
       <c r="J4" s="7" t="str">
-        <f>('Names-Hours'!H4) -(SUMIF(C9:C75,I4,D9:D75)) &amp;+"/"&amp;+ 'Names-Hours'!D8</f>
-        <v>0/30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <f>('Names-Hours'!H4) -(SUMIF(C9:C76,I4,D9:D76)) &amp;+"/"&amp;+ 'Names-Hours'!D8</f>
+        <v>-2/30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="9"/>
       <c r="D5" s="25" t="s">
         <v>21</v>
@@ -3285,36 +3344,36 @@
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
     </row>
-    <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:12" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="100" t="s">
+    <row r="6" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="1:12" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="97" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="100" t="s">
+      <c r="B7" s="97" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="96" t="s">
+      <c r="C7" s="93" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="98" t="s">
+      <c r="D7" s="95" t="s">
         <v>9</v>
       </c>
       <c r="E7" s="27"/>
-      <c r="F7" s="102" t="s">
+      <c r="F7" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="103"/>
-      <c r="H7" s="103"/>
-      <c r="I7" s="103"/>
-      <c r="J7" s="103"/>
-      <c r="K7" s="104"/>
+      <c r="G7" s="100"/>
+      <c r="H7" s="100"/>
+      <c r="I7" s="100"/>
+      <c r="J7" s="100"/>
+      <c r="K7" s="101"/>
       <c r="L7" s="16"/>
     </row>
-    <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="101"/>
-      <c r="B8" s="101"/>
-      <c r="C8" s="97"/>
-      <c r="D8" s="99"/>
+    <row r="8" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="98"/>
+      <c r="B8" s="98"/>
+      <c r="C8" s="94"/>
+      <c r="D8" s="96"/>
       <c r="E8" s="10">
         <v>41661</v>
       </c>
@@ -3337,8 +3396,8 @@
         <v>41675</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="16.149999999999999" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="93" t="s">
+    <row r="9" spans="1:12" ht="16.2" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="104" t="s">
         <v>53</v>
       </c>
       <c r="B9" s="36" t="s">
@@ -3362,8 +3421,8 @@
       <c r="J9" s="42"/>
       <c r="K9" s="43"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="91"/>
+    <row r="10" spans="1:12" ht="15" x14ac:dyDescent="0.3">
+      <c r="A10" s="102"/>
       <c r="B10" s="44" t="s">
         <v>32</v>
       </c>
@@ -3383,8 +3442,8 @@
       <c r="J10" s="34"/>
       <c r="K10" s="35"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="91"/>
+    <row r="11" spans="1:12" ht="15" x14ac:dyDescent="0.3">
+      <c r="A11" s="102"/>
       <c r="B11" s="46" t="s">
         <v>33</v>
       </c>
@@ -3397,13 +3456,15 @@
       <c r="E11" s="49"/>
       <c r="F11" s="50"/>
       <c r="G11" s="51"/>
-      <c r="H11" s="51"/>
+      <c r="H11" s="51">
+        <v>0.5</v>
+      </c>
       <c r="I11" s="52"/>
       <c r="J11" s="52"/>
       <c r="K11" s="53"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="91"/>
+    <row r="12" spans="1:12" ht="15" x14ac:dyDescent="0.3">
+      <c r="A12" s="102"/>
       <c r="B12" s="44" t="s">
         <v>33</v>
       </c>
@@ -3416,13 +3477,15 @@
       <c r="E12" s="45"/>
       <c r="F12" s="32"/>
       <c r="G12" s="33"/>
-      <c r="H12" s="33"/>
+      <c r="H12" s="33">
+        <v>2</v>
+      </c>
       <c r="I12" s="34"/>
       <c r="J12" s="34"/>
       <c r="K12" s="35"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="91"/>
+    <row r="13" spans="1:12" ht="15" x14ac:dyDescent="0.3">
+      <c r="A13" s="102"/>
       <c r="B13" s="46" t="s">
         <v>31</v>
       </c>
@@ -3440,8 +3503,8 @@
       <c r="J13" s="52"/>
       <c r="K13" s="53"/>
     </row>
-    <row r="14" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="92"/>
+    <row r="14" spans="1:12" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="103"/>
       <c r="B14" s="54" t="s">
         <v>54</v>
       </c>
@@ -3458,13 +3521,15 @@
       <c r="G14" s="57">
         <v>0.5</v>
       </c>
-      <c r="H14" s="57"/>
+      <c r="H14" s="57">
+        <v>1</v>
+      </c>
       <c r="I14" s="58"/>
       <c r="J14" s="58"/>
       <c r="K14" s="59"/>
     </row>
-    <row r="15" spans="1:12" ht="15.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="91" t="s">
+    <row r="15" spans="1:12" ht="15.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="102" t="s">
         <v>55</v>
       </c>
       <c r="B15" s="46" t="s">
@@ -3479,13 +3544,15 @@
       <c r="E15" s="49"/>
       <c r="F15" s="50"/>
       <c r="G15" s="51"/>
-      <c r="H15" s="51"/>
+      <c r="H15" s="51">
+        <v>1.5</v>
+      </c>
       <c r="I15" s="52"/>
       <c r="J15" s="52"/>
       <c r="K15" s="53"/>
     </row>
-    <row r="16" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="91"/>
+    <row r="16" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="102"/>
       <c r="B16" s="44" t="s">
         <v>35</v>
       </c>
@@ -3503,8 +3570,8 @@
       <c r="J16" s="34"/>
       <c r="K16" s="35"/>
     </row>
-    <row r="17" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="91"/>
+    <row r="17" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="102"/>
       <c r="B17" s="46" t="s">
         <v>35</v>
       </c>
@@ -3521,13 +3588,15 @@
       <c r="G17" s="51">
         <v>1</v>
       </c>
-      <c r="H17" s="51"/>
+      <c r="H17" s="51">
+        <v>1</v>
+      </c>
       <c r="I17" s="52"/>
       <c r="J17" s="52"/>
       <c r="K17" s="53"/>
     </row>
-    <row r="18" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="91"/>
+    <row r="18" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="102"/>
       <c r="B18" s="44" t="s">
         <v>35</v>
       </c>
@@ -3549,8 +3618,8 @@
       <c r="J18" s="34"/>
       <c r="K18" s="35"/>
     </row>
-    <row r="19" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="91"/>
+    <row r="19" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="102"/>
       <c r="B19" s="46" t="s">
         <v>35</v>
       </c>
@@ -3565,13 +3634,15 @@
         <v>2</v>
       </c>
       <c r="G19" s="51"/>
-      <c r="H19" s="51"/>
+      <c r="H19" s="51">
+        <v>2</v>
+      </c>
       <c r="I19" s="52"/>
       <c r="J19" s="52"/>
       <c r="K19" s="53"/>
     </row>
-    <row r="20" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="91"/>
+    <row r="20" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="102"/>
       <c r="B20" s="44" t="s">
         <v>35</v>
       </c>
@@ -3586,13 +3657,15 @@
       <c r="G20" s="33">
         <v>1</v>
       </c>
-      <c r="H20" s="33"/>
+      <c r="H20" s="33">
+        <v>1.5</v>
+      </c>
       <c r="I20" s="34"/>
       <c r="J20" s="34"/>
       <c r="K20" s="35"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="91"/>
+    <row r="21" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A21" s="102"/>
       <c r="B21" s="46" t="s">
         <v>34</v>
       </c>
@@ -3610,8 +3683,8 @@
       <c r="J21" s="52"/>
       <c r="K21" s="53"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="91"/>
+    <row r="22" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A22" s="102"/>
       <c r="B22" s="44" t="s">
         <v>34</v>
       </c>
@@ -3629,8 +3702,8 @@
       <c r="J22" s="34"/>
       <c r="K22" s="35"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="91"/>
+    <row r="23" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A23" s="102"/>
       <c r="B23" s="46" t="s">
         <v>36</v>
       </c>
@@ -3648,8 +3721,8 @@
       <c r="J23" s="52"/>
       <c r="K23" s="53"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="91"/>
+    <row r="24" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A24" s="102"/>
       <c r="B24" s="44" t="s">
         <v>36</v>
       </c>
@@ -3669,8 +3742,8 @@
       <c r="J24" s="34"/>
       <c r="K24" s="35"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="91"/>
+    <row r="25" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A25" s="102"/>
       <c r="B25" s="46" t="s">
         <v>36</v>
       </c>
@@ -3683,13 +3756,15 @@
       <c r="E25" s="49"/>
       <c r="F25" s="50"/>
       <c r="G25" s="51"/>
-      <c r="H25" s="51"/>
+      <c r="H25" s="51">
+        <v>1</v>
+      </c>
       <c r="I25" s="52"/>
       <c r="J25" s="52"/>
       <c r="K25" s="53"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="91"/>
+    <row r="26" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A26" s="102"/>
       <c r="B26" s="44" t="s">
         <v>36</v>
       </c>
@@ -3702,13 +3777,15 @@
       <c r="E26" s="45"/>
       <c r="F26" s="32"/>
       <c r="G26" s="33"/>
-      <c r="H26" s="33"/>
+      <c r="H26" s="33">
+        <v>0.5</v>
+      </c>
       <c r="I26" s="34"/>
       <c r="J26" s="34"/>
       <c r="K26" s="35"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="91"/>
+    <row r="27" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A27" s="102"/>
       <c r="B27" s="46" t="s">
         <v>36</v>
       </c>
@@ -3723,13 +3800,15 @@
       <c r="G27" s="51">
         <v>2.5</v>
       </c>
-      <c r="H27" s="51"/>
+      <c r="H27" s="51">
+        <v>0.5</v>
+      </c>
       <c r="I27" s="52"/>
       <c r="J27" s="52"/>
       <c r="K27" s="53"/>
     </row>
-    <row r="28" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="92"/>
+    <row r="28" spans="1:11" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="103"/>
       <c r="B28" s="54" t="s">
         <v>36</v>
       </c>
@@ -3744,13 +3823,15 @@
       <c r="G28" s="57">
         <v>0.5</v>
       </c>
-      <c r="H28" s="57"/>
+      <c r="H28" s="57">
+        <v>1</v>
+      </c>
       <c r="I28" s="58"/>
       <c r="J28" s="58"/>
       <c r="K28" s="59"/>
     </row>
-    <row r="29" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="91" t="s">
+    <row r="29" spans="1:11" ht="15.6" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="102" t="s">
         <v>56</v>
       </c>
       <c r="B29" s="46" t="s">
@@ -3770,8 +3851,8 @@
       <c r="J29" s="52"/>
       <c r="K29" s="53"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="91"/>
+    <row r="30" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A30" s="102"/>
       <c r="B30" s="44" t="s">
         <v>37</v>
       </c>
@@ -3784,13 +3865,15 @@
       <c r="E30" s="45"/>
       <c r="F30" s="32"/>
       <c r="G30" s="33"/>
-      <c r="H30" s="33"/>
+      <c r="H30" s="33">
+        <v>0.5</v>
+      </c>
       <c r="I30" s="34"/>
       <c r="J30" s="34"/>
       <c r="K30" s="35"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="91"/>
+    <row r="31" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A31" s="102"/>
       <c r="B31" s="46" t="s">
         <v>37</v>
       </c>
@@ -3810,8 +3893,8 @@
       <c r="J31" s="52"/>
       <c r="K31" s="53"/>
     </row>
-    <row r="32" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="91"/>
+    <row r="32" spans="1:11" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="102"/>
       <c r="B32" s="44" t="s">
         <v>37</v>
       </c>
@@ -3831,8 +3914,8 @@
       <c r="J32" s="34"/>
       <c r="K32" s="35"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="91"/>
+    <row r="33" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A33" s="102"/>
       <c r="B33" s="46" t="s">
         <v>37</v>
       </c>
@@ -3852,8 +3935,8 @@
       <c r="J33" s="52"/>
       <c r="K33" s="53"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="91"/>
+    <row r="34" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A34" s="102"/>
       <c r="B34" s="44" t="s">
         <v>37</v>
       </c>
@@ -3871,8 +3954,8 @@
       <c r="J34" s="34"/>
       <c r="K34" s="35"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="91"/>
+    <row r="35" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A35" s="102"/>
       <c r="B35" s="46" t="s">
         <v>38</v>
       </c>
@@ -3890,8 +3973,8 @@
       <c r="J35" s="52"/>
       <c r="K35" s="53"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="91"/>
+    <row r="36" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A36" s="102"/>
       <c r="B36" s="44" t="s">
         <v>38</v>
       </c>
@@ -3909,8 +3992,8 @@
       <c r="J36" s="34"/>
       <c r="K36" s="35"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="91"/>
+    <row r="37" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A37" s="102"/>
       <c r="B37" s="46" t="s">
         <v>38</v>
       </c>
@@ -3928,8 +4011,8 @@
       <c r="J37" s="52"/>
       <c r="K37" s="53"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="91"/>
+    <row r="38" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A38" s="102"/>
       <c r="B38" s="44" t="s">
         <v>38</v>
       </c>
@@ -3947,8 +4030,8 @@
       <c r="J38" s="34"/>
       <c r="K38" s="35"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="91"/>
+    <row r="39" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A39" s="102"/>
       <c r="B39" s="46" t="s">
         <v>38</v>
       </c>
@@ -3966,8 +4049,8 @@
       <c r="J39" s="52"/>
       <c r="K39" s="53"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="91"/>
+    <row r="40" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A40" s="102"/>
       <c r="B40" s="44" t="s">
         <v>38</v>
       </c>
@@ -3985,8 +4068,8 @@
       <c r="J40" s="34"/>
       <c r="K40" s="35"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="91"/>
+    <row r="41" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A41" s="102"/>
       <c r="B41" s="46" t="s">
         <v>39</v>
       </c>
@@ -3999,13 +4082,15 @@
       <c r="E41" s="49"/>
       <c r="F41" s="50"/>
       <c r="G41" s="51"/>
-      <c r="H41" s="51"/>
+      <c r="H41" s="51">
+        <v>2.5</v>
+      </c>
       <c r="I41" s="52"/>
       <c r="J41" s="52"/>
       <c r="K41" s="53"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="91"/>
+    <row r="42" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A42" s="102"/>
       <c r="B42" s="46" t="s">
         <v>40</v>
       </c>
@@ -4023,8 +4108,8 @@
       <c r="J42" s="52"/>
       <c r="K42" s="53"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="91"/>
+    <row r="43" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A43" s="102"/>
       <c r="B43" s="44" t="s">
         <v>40</v>
       </c>
@@ -4042,8 +4127,8 @@
       <c r="J43" s="34"/>
       <c r="K43" s="35"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="91"/>
+    <row r="44" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A44" s="102"/>
       <c r="B44" s="46" t="s">
         <v>40</v>
       </c>
@@ -4061,8 +4146,8 @@
       <c r="J44" s="52"/>
       <c r="K44" s="53"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="91"/>
+    <row r="45" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A45" s="102"/>
       <c r="B45" s="44" t="s">
         <v>40</v>
       </c>
@@ -4080,8 +4165,8 @@
       <c r="J45" s="34"/>
       <c r="K45" s="35"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="91"/>
+    <row r="46" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A46" s="102"/>
       <c r="B46" s="46" t="s">
         <v>40</v>
       </c>
@@ -4099,8 +4184,8 @@
       <c r="J46" s="52"/>
       <c r="K46" s="53"/>
     </row>
-    <row r="47" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="92"/>
+    <row r="47" spans="1:11" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="103"/>
       <c r="B47" s="54" t="s">
         <v>40</v>
       </c>
@@ -4118,8 +4203,8 @@
       <c r="J47" s="58"/>
       <c r="K47" s="59"/>
     </row>
-    <row r="48" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="91" t="s">
+    <row r="48" spans="1:11" ht="15.6" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="102" t="s">
         <v>57</v>
       </c>
       <c r="B48" s="46" t="s">
@@ -4139,8 +4224,8 @@
       <c r="J48" s="52"/>
       <c r="K48" s="53"/>
     </row>
-    <row r="49" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="91"/>
+    <row r="49" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="102"/>
       <c r="B49" s="44" t="s">
         <v>42</v>
       </c>
@@ -4158,8 +4243,8 @@
       <c r="J49" s="34"/>
       <c r="K49" s="35"/>
     </row>
-    <row r="50" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="92"/>
+    <row r="50" spans="1:11" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="103"/>
       <c r="B50" s="60" t="s">
         <v>43</v>
       </c>
@@ -4177,8 +4262,8 @@
       <c r="J50" s="66"/>
       <c r="K50" s="67"/>
     </row>
-    <row r="51" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="91" t="s">
+    <row r="51" spans="1:11" ht="15.6" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="102" t="s">
         <v>58</v>
       </c>
       <c r="B51" s="44" t="s">
@@ -4193,13 +4278,15 @@
       <c r="E51" s="45"/>
       <c r="F51" s="32"/>
       <c r="G51" s="33"/>
-      <c r="H51" s="33"/>
+      <c r="H51" s="33">
+        <v>0.5</v>
+      </c>
       <c r="I51" s="34"/>
       <c r="J51" s="34"/>
       <c r="K51" s="35"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="91"/>
+    <row r="52" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A52" s="102"/>
       <c r="B52" s="46" t="s">
         <v>45</v>
       </c>
@@ -4217,8 +4304,8 @@
       <c r="J52" s="52"/>
       <c r="K52" s="53"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="91"/>
+    <row r="53" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A53" s="102"/>
       <c r="B53" s="44" t="s">
         <v>46</v>
       </c>
@@ -4236,8 +4323,8 @@
       <c r="J53" s="34"/>
       <c r="K53" s="35"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="91"/>
+    <row r="54" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A54" s="102"/>
       <c r="B54" s="46" t="s">
         <v>62</v>
       </c>
@@ -4255,8 +4342,8 @@
       <c r="J54" s="52"/>
       <c r="K54" s="53"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" s="91"/>
+    <row r="55" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A55" s="102"/>
       <c r="B55" s="44" t="s">
         <v>62</v>
       </c>
@@ -4274,564 +4361,585 @@
       <c r="J55" s="34"/>
       <c r="K55" s="35"/>
     </row>
-    <row r="56" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="92"/>
-      <c r="B56" s="60" t="s">
+    <row r="56" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A56" s="102"/>
+      <c r="B56" s="44" t="s">
         <v>62</v>
       </c>
-      <c r="C56" s="61" t="s">
+      <c r="C56" s="144" t="s">
+        <v>25</v>
+      </c>
+      <c r="D56" s="145">
+        <v>2</v>
+      </c>
+      <c r="E56" s="146"/>
+      <c r="F56" s="147"/>
+      <c r="G56" s="148"/>
+      <c r="H56" s="148">
+        <v>1</v>
+      </c>
+      <c r="I56" s="149"/>
+      <c r="J56" s="149"/>
+      <c r="K56" s="150"/>
+    </row>
+    <row r="57" spans="1:11" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="103"/>
+      <c r="B57" s="60" t="s">
+        <v>62</v>
+      </c>
+      <c r="C57" s="61" t="s">
         <v>23</v>
       </c>
-      <c r="D56" s="62">
+      <c r="D57" s="62">
         <v>1</v>
       </c>
-      <c r="E56" s="63"/>
-      <c r="F56" s="64"/>
-      <c r="G56" s="65"/>
-      <c r="H56" s="65"/>
-      <c r="I56" s="66"/>
-      <c r="J56" s="66"/>
-      <c r="K56" s="67"/>
-    </row>
-    <row r="57" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="91" t="s">
+      <c r="E57" s="63"/>
+      <c r="F57" s="64"/>
+      <c r="G57" s="65"/>
+      <c r="H57" s="65"/>
+      <c r="I57" s="66"/>
+      <c r="J57" s="66"/>
+      <c r="K57" s="67"/>
+    </row>
+    <row r="58" spans="1:11" ht="15.6" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="102" t="s">
         <v>59</v>
       </c>
-      <c r="B57" s="44" t="s">
+      <c r="B58" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="C57" s="30" t="s">
+      <c r="C58" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="D57" s="31">
+      <c r="D58" s="31">
         <v>0.5</v>
       </c>
-      <c r="E57" s="45"/>
-      <c r="F57" s="32"/>
-      <c r="G57" s="33"/>
-      <c r="H57" s="33"/>
-      <c r="I57" s="34"/>
-      <c r="J57" s="34"/>
-      <c r="K57" s="35"/>
-    </row>
-    <row r="58" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="92"/>
-      <c r="B58" s="60" t="s">
+      <c r="E58" s="45"/>
+      <c r="F58" s="32"/>
+      <c r="G58" s="33"/>
+      <c r="H58" s="33"/>
+      <c r="I58" s="34"/>
+      <c r="J58" s="34"/>
+      <c r="K58" s="35"/>
+    </row>
+    <row r="59" spans="1:11" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="103"/>
+      <c r="B59" s="60" t="s">
         <v>48</v>
       </c>
-      <c r="C58" s="61" t="s">
+      <c r="C59" s="61" t="s">
         <v>24</v>
       </c>
-      <c r="D58" s="62">
+      <c r="D59" s="62">
         <v>0.5</v>
       </c>
-      <c r="E58" s="63"/>
-      <c r="F58" s="64"/>
-      <c r="G58" s="65"/>
-      <c r="H58" s="65"/>
-      <c r="I58" s="66"/>
-      <c r="J58" s="66"/>
-      <c r="K58" s="67"/>
-    </row>
-    <row r="59" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="91" t="s">
+      <c r="E59" s="63"/>
+      <c r="F59" s="64"/>
+      <c r="G59" s="65"/>
+      <c r="H59" s="65"/>
+      <c r="I59" s="66"/>
+      <c r="J59" s="66"/>
+      <c r="K59" s="67"/>
+    </row>
+    <row r="60" spans="1:11" ht="15.6" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="102" t="s">
         <v>60</v>
       </c>
-      <c r="B59" s="44" t="s">
+      <c r="B60" s="44" t="s">
         <v>49</v>
       </c>
-      <c r="C59" s="30" t="s">
+      <c r="C60" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="D59" s="31">
+      <c r="D60" s="31">
         <v>0.5</v>
       </c>
-      <c r="E59" s="45"/>
-      <c r="F59" s="32"/>
-      <c r="G59" s="33"/>
-      <c r="H59" s="33"/>
-      <c r="I59" s="34"/>
-      <c r="J59" s="34"/>
-      <c r="K59" s="35"/>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A60" s="91"/>
-      <c r="B60" s="46" t="s">
+      <c r="E60" s="45"/>
+      <c r="F60" s="32"/>
+      <c r="G60" s="33"/>
+      <c r="H60" s="33"/>
+      <c r="I60" s="34"/>
+      <c r="J60" s="34"/>
+      <c r="K60" s="35"/>
+    </row>
+    <row r="61" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A61" s="102"/>
+      <c r="B61" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="C60" s="47" t="s">
+      <c r="C61" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="D60" s="48">
+      <c r="D61" s="48">
         <v>0.5</v>
       </c>
-      <c r="E60" s="49"/>
-      <c r="F60" s="50"/>
-      <c r="G60" s="51"/>
-      <c r="H60" s="51"/>
-      <c r="I60" s="52"/>
-      <c r="J60" s="52"/>
-      <c r="K60" s="53"/>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A61" s="91"/>
-      <c r="B61" s="44" t="s">
+      <c r="E61" s="49"/>
+      <c r="F61" s="50"/>
+      <c r="G61" s="51"/>
+      <c r="H61" s="51"/>
+      <c r="I61" s="52"/>
+      <c r="J61" s="52"/>
+      <c r="K61" s="53"/>
+    </row>
+    <row r="62" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A62" s="102"/>
+      <c r="B62" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="C61" s="30" t="s">
+      <c r="C62" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="D61" s="31">
+      <c r="D62" s="31">
         <v>0.5</v>
       </c>
-      <c r="E61" s="45"/>
-      <c r="F61" s="32"/>
-      <c r="G61" s="33"/>
-      <c r="H61" s="33"/>
-      <c r="I61" s="34"/>
-      <c r="J61" s="34"/>
-      <c r="K61" s="35"/>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A62" s="91"/>
-      <c r="B62" s="46" t="s">
+      <c r="E62" s="45"/>
+      <c r="F62" s="32"/>
+      <c r="G62" s="33"/>
+      <c r="H62" s="33"/>
+      <c r="I62" s="34"/>
+      <c r="J62" s="34"/>
+      <c r="K62" s="35"/>
+    </row>
+    <row r="63" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A63" s="102"/>
+      <c r="B63" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="C62" s="47" t="s">
+      <c r="C63" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="D62" s="48">
+      <c r="D63" s="48">
         <v>0.5</v>
       </c>
-      <c r="E62" s="49"/>
-      <c r="F62" s="50"/>
-      <c r="G62" s="51"/>
-      <c r="H62" s="51"/>
-      <c r="I62" s="52"/>
-      <c r="J62" s="52"/>
-      <c r="K62" s="53"/>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A63" s="91"/>
-      <c r="B63" s="44" t="s">
+      <c r="E63" s="49"/>
+      <c r="F63" s="50"/>
+      <c r="G63" s="51"/>
+      <c r="H63" s="51"/>
+      <c r="I63" s="52"/>
+      <c r="J63" s="52"/>
+      <c r="K63" s="53"/>
+    </row>
+    <row r="64" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A64" s="102"/>
+      <c r="B64" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="C63" s="30" t="s">
+      <c r="C64" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="D63" s="31">
+      <c r="D64" s="31">
         <v>0.5</v>
       </c>
-      <c r="E63" s="45"/>
-      <c r="F63" s="32"/>
-      <c r="G63" s="33"/>
-      <c r="H63" s="33"/>
-      <c r="I63" s="34"/>
-      <c r="J63" s="34"/>
-      <c r="K63" s="35"/>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A64" s="91"/>
-      <c r="B64" s="46" t="s">
+      <c r="E64" s="45"/>
+      <c r="F64" s="32"/>
+      <c r="G64" s="33"/>
+      <c r="H64" s="33"/>
+      <c r="I64" s="34"/>
+      <c r="J64" s="34"/>
+      <c r="K64" s="35"/>
+    </row>
+    <row r="65" spans="1:12" ht="15" x14ac:dyDescent="0.3">
+      <c r="A65" s="102"/>
+      <c r="B65" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="C64" s="47" t="s">
+      <c r="C65" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="D64" s="48">
+      <c r="D65" s="48">
         <v>0.5</v>
       </c>
-      <c r="E64" s="49"/>
-      <c r="F64" s="50"/>
-      <c r="G64" s="51"/>
-      <c r="H64" s="51"/>
-      <c r="I64" s="52"/>
-      <c r="J64" s="52"/>
-      <c r="K64" s="53"/>
-    </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A65" s="91"/>
-      <c r="B65" s="44" t="s">
+      <c r="E65" s="49"/>
+      <c r="F65" s="50"/>
+      <c r="G65" s="51"/>
+      <c r="H65" s="51"/>
+      <c r="I65" s="52"/>
+      <c r="J65" s="52"/>
+      <c r="K65" s="53"/>
+    </row>
+    <row r="66" spans="1:12" ht="15" x14ac:dyDescent="0.3">
+      <c r="A66" s="102"/>
+      <c r="B66" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="C65" s="30" t="s">
+      <c r="C66" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="D65" s="31">
+      <c r="D66" s="31">
         <v>0.5</v>
       </c>
-      <c r="E65" s="45"/>
-      <c r="F65" s="32"/>
-      <c r="G65" s="33"/>
-      <c r="H65" s="33"/>
-      <c r="I65" s="34"/>
-      <c r="J65" s="34"/>
-      <c r="K65" s="35"/>
-    </row>
-    <row r="66" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="92"/>
-      <c r="B66" s="60" t="s">
+      <c r="E66" s="45"/>
+      <c r="F66" s="32"/>
+      <c r="G66" s="33"/>
+      <c r="H66" s="33"/>
+      <c r="I66" s="34"/>
+      <c r="J66" s="34"/>
+      <c r="K66" s="35"/>
+    </row>
+    <row r="67" spans="1:12" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="103"/>
+      <c r="B67" s="60" t="s">
         <v>50</v>
       </c>
-      <c r="C66" s="61" t="s">
+      <c r="C67" s="61" t="s">
         <v>25</v>
       </c>
-      <c r="D66" s="62">
+      <c r="D67" s="62">
         <v>0.5</v>
       </c>
-      <c r="E66" s="63"/>
-      <c r="F66" s="64"/>
-      <c r="G66" s="65"/>
-      <c r="H66" s="65"/>
-      <c r="I66" s="66"/>
-      <c r="J66" s="66"/>
-      <c r="K66" s="67"/>
-    </row>
-    <row r="67" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="91" t="s">
+      <c r="E67" s="63"/>
+      <c r="F67" s="64"/>
+      <c r="G67" s="65"/>
+      <c r="H67" s="65"/>
+      <c r="I67" s="66"/>
+      <c r="J67" s="66"/>
+      <c r="K67" s="67"/>
+    </row>
+    <row r="68" spans="1:12" ht="15.6" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="102" t="s">
         <v>61</v>
       </c>
-      <c r="B67" s="44" t="s">
+      <c r="B68" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="C67" s="30" t="s">
+      <c r="C68" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="D67" s="31">
+      <c r="D68" s="31">
         <v>2</v>
       </c>
-      <c r="E67" s="45"/>
-      <c r="F67" s="32"/>
-      <c r="G67" s="33"/>
-      <c r="H67" s="33"/>
-      <c r="I67" s="34"/>
-      <c r="J67" s="34"/>
-      <c r="K67" s="35"/>
-    </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A68" s="91"/>
-      <c r="B68" s="46" t="s">
+      <c r="E68" s="45"/>
+      <c r="F68" s="32"/>
+      <c r="G68" s="33"/>
+      <c r="H68" s="33"/>
+      <c r="I68" s="34"/>
+      <c r="J68" s="34"/>
+      <c r="K68" s="35"/>
+    </row>
+    <row r="69" spans="1:12" ht="15" x14ac:dyDescent="0.3">
+      <c r="A69" s="102"/>
+      <c r="B69" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="C68" s="47" t="s">
+      <c r="C69" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="D68" s="48">
+      <c r="D69" s="48">
         <v>2</v>
       </c>
-      <c r="E68" s="49"/>
-      <c r="F68" s="50"/>
-      <c r="G68" s="51"/>
-      <c r="H68" s="51"/>
-      <c r="I68" s="52"/>
-      <c r="J68" s="52"/>
-      <c r="K68" s="53"/>
-    </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A69" s="91"/>
-      <c r="B69" s="44" t="s">
+      <c r="E69" s="49"/>
+      <c r="F69" s="50"/>
+      <c r="G69" s="51"/>
+      <c r="H69" s="51"/>
+      <c r="I69" s="52"/>
+      <c r="J69" s="52"/>
+      <c r="K69" s="53"/>
+    </row>
+    <row r="70" spans="1:12" ht="15" x14ac:dyDescent="0.3">
+      <c r="A70" s="102"/>
+      <c r="B70" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="C69" s="30" t="s">
+      <c r="C70" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="D69" s="31">
+      <c r="D70" s="31">
         <v>1</v>
       </c>
-      <c r="E69" s="45"/>
-      <c r="F69" s="32"/>
-      <c r="G69" s="33"/>
-      <c r="H69" s="33"/>
-      <c r="I69" s="34"/>
-      <c r="J69" s="34"/>
-      <c r="K69" s="35"/>
-    </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A70" s="91"/>
-      <c r="B70" s="46" t="s">
+      <c r="E70" s="45"/>
+      <c r="F70" s="32"/>
+      <c r="G70" s="33"/>
+      <c r="H70" s="33"/>
+      <c r="I70" s="34"/>
+      <c r="J70" s="34"/>
+      <c r="K70" s="35"/>
+    </row>
+    <row r="71" spans="1:12" ht="15" x14ac:dyDescent="0.3">
+      <c r="A71" s="102"/>
+      <c r="B71" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="C70" s="47" t="s">
+      <c r="C71" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="D70" s="48">
+      <c r="D71" s="48">
         <v>1</v>
       </c>
-      <c r="E70" s="49"/>
-      <c r="F70" s="50"/>
-      <c r="G70" s="51"/>
-      <c r="H70" s="51"/>
-      <c r="I70" s="52"/>
-      <c r="J70" s="52"/>
-      <c r="K70" s="53"/>
-    </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A71" s="91"/>
-      <c r="B71" s="44" t="s">
+      <c r="E71" s="49"/>
+      <c r="F71" s="50"/>
+      <c r="G71" s="51"/>
+      <c r="H71" s="51"/>
+      <c r="I71" s="52"/>
+      <c r="J71" s="52"/>
+      <c r="K71" s="53"/>
+    </row>
+    <row r="72" spans="1:12" ht="15" x14ac:dyDescent="0.3">
+      <c r="A72" s="102"/>
+      <c r="B72" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="C71" s="30" t="s">
+      <c r="C72" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="D71" s="31">
+      <c r="D72" s="31">
         <v>1</v>
       </c>
-      <c r="E71" s="45"/>
-      <c r="F71" s="32"/>
-      <c r="G71" s="33"/>
-      <c r="H71" s="33"/>
-      <c r="I71" s="34"/>
-      <c r="J71" s="34"/>
-      <c r="K71" s="35"/>
-    </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A72" s="91"/>
-      <c r="B72" s="46" t="s">
+      <c r="E72" s="45"/>
+      <c r="F72" s="32"/>
+      <c r="G72" s="33"/>
+      <c r="H72" s="33"/>
+      <c r="I72" s="34"/>
+      <c r="J72" s="34"/>
+      <c r="K72" s="35"/>
+    </row>
+    <row r="73" spans="1:12" ht="15" x14ac:dyDescent="0.3">
+      <c r="A73" s="102"/>
+      <c r="B73" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="C72" s="47" t="s">
+      <c r="C73" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="D72" s="48">
+      <c r="D73" s="48">
         <v>1</v>
       </c>
-      <c r="E72" s="49"/>
-      <c r="F72" s="50"/>
-      <c r="G72" s="51"/>
-      <c r="H72" s="51"/>
-      <c r="I72" s="52"/>
-      <c r="J72" s="52"/>
-      <c r="K72" s="53"/>
-    </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A73" s="91"/>
-      <c r="B73" s="44" t="s">
+      <c r="E73" s="49"/>
+      <c r="F73" s="50"/>
+      <c r="G73" s="51"/>
+      <c r="H73" s="51"/>
+      <c r="I73" s="52"/>
+      <c r="J73" s="52"/>
+      <c r="K73" s="53"/>
+    </row>
+    <row r="74" spans="1:12" ht="15" x14ac:dyDescent="0.3">
+      <c r="A74" s="102"/>
+      <c r="B74" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="C73" s="30" t="s">
+      <c r="C74" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="D73" s="31">
+      <c r="D74" s="31">
         <v>1</v>
       </c>
-      <c r="E73" s="45"/>
-      <c r="F73" s="32"/>
-      <c r="G73" s="33"/>
-      <c r="H73" s="33"/>
-      <c r="I73" s="34"/>
-      <c r="J73" s="34"/>
-      <c r="K73" s="35"/>
-    </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A74" s="91"/>
-      <c r="B74" s="46" t="s">
+      <c r="E74" s="45"/>
+      <c r="F74" s="32"/>
+      <c r="G74" s="33"/>
+      <c r="H74" s="33"/>
+      <c r="I74" s="34"/>
+      <c r="J74" s="34"/>
+      <c r="K74" s="35"/>
+    </row>
+    <row r="75" spans="1:12" ht="15" x14ac:dyDescent="0.3">
+      <c r="A75" s="102"/>
+      <c r="B75" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="C74" s="47" t="s">
+      <c r="C75" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="D74" s="48">
+      <c r="D75" s="48">
         <v>1</v>
       </c>
-      <c r="E74" s="49"/>
-      <c r="F74" s="50"/>
-      <c r="G74" s="51"/>
-      <c r="H74" s="51"/>
-      <c r="I74" s="52"/>
-      <c r="J74" s="52"/>
-      <c r="K74" s="53"/>
-    </row>
-    <row r="75" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="92"/>
-      <c r="B75" s="54" t="s">
+      <c r="E75" s="49"/>
+      <c r="F75" s="50"/>
+      <c r="G75" s="51"/>
+      <c r="H75" s="51"/>
+      <c r="I75" s="52"/>
+      <c r="J75" s="52"/>
+      <c r="K75" s="53"/>
+    </row>
+    <row r="76" spans="1:12" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A76" s="103"/>
+      <c r="B76" s="54" t="s">
         <v>64</v>
       </c>
-      <c r="C75" s="14" t="s">
+      <c r="C76" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D75" s="15">
+      <c r="D76" s="15">
         <v>1</v>
       </c>
-      <c r="E75" s="55"/>
-      <c r="F75" s="56"/>
-      <c r="G75" s="57"/>
-      <c r="H75" s="57"/>
-      <c r="I75" s="58"/>
-      <c r="J75" s="58"/>
-      <c r="K75" s="59"/>
-    </row>
-    <row r="76" spans="1:20" ht="16.149999999999999" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D76" s="11">
-        <f>SUM(D9:D75)</f>
-        <v>160</v>
-      </c>
-      <c r="E76" s="12" t="str">
-        <f>E77&amp;+ "/" &amp;+ $D$76</f>
-        <v>0/160</v>
-      </c>
-      <c r="F76" s="12" t="str">
-        <f>F77&amp;+ "/" &amp;+ $D$76</f>
-        <v>6/160</v>
-      </c>
-      <c r="G76" s="12" t="str">
-        <f t="shared" ref="G76:K76" si="0">G77&amp;+ "/" &amp;+ $D$76</f>
-        <v>19/160</v>
-      </c>
-      <c r="H76" s="12" t="str">
+      <c r="E76" s="55"/>
+      <c r="F76" s="56"/>
+      <c r="G76" s="57"/>
+      <c r="H76" s="57"/>
+      <c r="I76" s="58"/>
+      <c r="J76" s="58"/>
+      <c r="K76" s="59"/>
+    </row>
+    <row r="77" spans="1:12" ht="16.2" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D77" s="11">
+        <f>SUM(D9:D76)</f>
+        <v>162</v>
+      </c>
+      <c r="E77" s="12" t="str">
+        <f>E78&amp;+ "/" &amp;+ $D$77</f>
+        <v>0/162</v>
+      </c>
+      <c r="F77" s="12" t="str">
+        <f>F78&amp;+ "/" &amp;+ $D$77</f>
+        <v>6/162</v>
+      </c>
+      <c r="G77" s="12" t="str">
+        <f t="shared" ref="G77:K77" si="0">G78&amp;+ "/" &amp;+ $D$77</f>
+        <v>19/162</v>
+      </c>
+      <c r="H77" s="12" t="str">
         <f t="shared" si="0"/>
-        <v>19/160</v>
-      </c>
-      <c r="I76" s="12" t="str">
+        <v>36/162</v>
+      </c>
+      <c r="I77" s="12" t="str">
         <f t="shared" si="0"/>
-        <v>19/160</v>
-      </c>
-      <c r="J76" s="12" t="str">
+        <v>36/162</v>
+      </c>
+      <c r="J77" s="12" t="str">
         <f t="shared" si="0"/>
-        <v>19/160</v>
-      </c>
-      <c r="K76" s="13" t="str">
+        <v>36/162</v>
+      </c>
+      <c r="K77" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>19/160</v>
-      </c>
-    </row>
-    <row r="77" spans="1:20" ht="15" hidden="1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="D77" s="1">
-        <f>SUM(D9:D75)</f>
-        <v>160</v>
-      </c>
-      <c r="E77" s="1">
-        <f>SUM(E9:E75)</f>
+        <v>36/162</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" ht="15" hidden="1" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="D78" s="1">
+        <f>SUM(D9:D76)</f>
+        <v>162</v>
+      </c>
+      <c r="E78" s="1">
+        <f>SUM(E9:E76)</f>
         <v>0</v>
       </c>
-      <c r="F77" s="1">
-        <f>SUM(F9:F75)</f>
+      <c r="F78" s="1">
+        <f>SUM(F9:F76)</f>
         <v>6</v>
       </c>
-      <c r="G77" s="1">
-        <f>SUM(G9:G75)+F77</f>
+      <c r="G78" s="1">
+        <f>SUM(G9:G76)+F78</f>
         <v>19</v>
       </c>
-      <c r="H77" s="1">
-        <f>SUM(H9:H75)+G77</f>
-        <v>19</v>
-      </c>
-      <c r="I77" s="1">
-        <f>SUM(I9:I75)+H77</f>
-        <v>19</v>
-      </c>
-      <c r="J77" s="1">
-        <f>SUM(J9:J75)+I77</f>
-        <v>19</v>
-      </c>
-      <c r="K77" s="1">
-        <f>SUM(K9:K75)+J77</f>
-        <v>19</v>
-      </c>
-      <c r="L77" s="1"/>
-    </row>
-    <row r="78" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D78" s="1"/>
-      <c r="E78" s="1">
-        <f>D76</f>
-        <v>160</v>
-      </c>
-      <c r="F78" s="1">
-        <f>E78</f>
-        <v>160</v>
-      </c>
-      <c r="G78" s="1">
-        <f>F78</f>
-        <v>160</v>
-      </c>
       <c r="H78" s="1">
-        <f t="shared" ref="H78:K78" si="1">G78</f>
-        <v>160</v>
+        <f>SUM(H9:H76)+G78</f>
+        <v>36</v>
       </c>
       <c r="I78" s="1">
-        <f t="shared" si="1"/>
-        <v>160</v>
+        <f>SUM(I9:I76)+H78</f>
+        <v>36</v>
       </c>
       <c r="J78" s="1">
-        <f t="shared" si="1"/>
-        <v>160</v>
+        <f>SUM(J9:J76)+I78</f>
+        <v>36</v>
       </c>
       <c r="K78" s="1">
-        <f t="shared" si="1"/>
-        <v>160</v>
+        <f>SUM(K9:K76)+J78</f>
+        <v>36</v>
       </c>
       <c r="L78" s="1"/>
     </row>
-    <row r="79" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D79" s="1"/>
       <c r="E79" s="1">
+        <f>D77</f>
+        <v>162</v>
+      </c>
+      <c r="F79" s="1">
+        <f>E79</f>
+        <v>162</v>
+      </c>
+      <c r="G79" s="1">
+        <f>F79</f>
+        <v>162</v>
+      </c>
+      <c r="H79" s="1">
+        <f t="shared" ref="H79:K79" si="1">G79</f>
+        <v>162</v>
+      </c>
+      <c r="I79" s="1">
+        <f t="shared" si="1"/>
+        <v>162</v>
+      </c>
+      <c r="J79" s="1">
+        <f t="shared" si="1"/>
+        <v>162</v>
+      </c>
+      <c r="K79" s="1">
+        <f t="shared" si="1"/>
+        <v>162</v>
+      </c>
+      <c r="L79" s="1"/>
+    </row>
+    <row r="80" spans="1:12" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D80" s="1"/>
+      <c r="E80" s="1">
         <v>0</v>
       </c>
-      <c r="K79" s="2">
-        <f>K78</f>
-        <v>160</v>
-      </c>
-    </row>
-    <row r="80" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
-      <c r="D80" s="1"/>
-      <c r="E80" s="5" t="s">
+      <c r="K80" s="2">
+        <f>K79</f>
+        <v>162</v>
+      </c>
+    </row>
+    <row r="81" spans="4:20" hidden="1" x14ac:dyDescent="0.3">
+      <c r="D81" s="1"/>
+      <c r="E81" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F80" s="5" t="s">
+      <c r="F81" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G80" s="5" t="s">
+      <c r="G81" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H80" s="5"/>
-      <c r="I80" s="5"/>
-      <c r="J80" s="4"/>
-      <c r="K80" s="4"/>
-      <c r="L80" s="4"/>
-      <c r="M80" s="4"/>
-      <c r="N80" s="4"/>
-      <c r="O80" s="4"/>
-      <c r="P80" s="4"/>
-      <c r="Q80" s="4"/>
-      <c r="R80" s="4"/>
-      <c r="S80" s="4"/>
-      <c r="T80" s="4"/>
-    </row>
-    <row r="81" spans="4:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="D81" s="1"/>
-      <c r="E81" s="1"/>
-      <c r="F81" s="1"/>
-      <c r="G81" s="1"/>
-      <c r="H81" s="1"/>
-      <c r="I81" s="1"/>
-    </row>
-    <row r="99" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R99" s="2" t="s">
+      <c r="H81" s="5"/>
+      <c r="I81" s="5"/>
+      <c r="J81" s="4"/>
+      <c r="K81" s="4"/>
+      <c r="L81" s="4"/>
+      <c r="M81" s="4"/>
+      <c r="N81" s="4"/>
+      <c r="O81" s="4"/>
+      <c r="P81" s="4"/>
+      <c r="Q81" s="4"/>
+      <c r="R81" s="4"/>
+      <c r="S81" s="4"/>
+      <c r="T81" s="4"/>
+    </row>
+    <row r="82" spans="4:20" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="D82" s="1"/>
+      <c r="E82" s="1"/>
+      <c r="F82" s="1"/>
+      <c r="G82" s="1"/>
+      <c r="H82" s="1"/>
+      <c r="I82" s="1"/>
+    </row>
+    <row r="100" spans="18:18" x14ac:dyDescent="0.3">
+      <c r="R100" s="2" t="s">
         <v>30</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A60:A67"/>
+    <mergeCell ref="A68:A76"/>
+    <mergeCell ref="A9:A14"/>
+    <mergeCell ref="A15:A28"/>
+    <mergeCell ref="A29:A47"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="A51:A57"/>
+    <mergeCell ref="A48:A50"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="F7:K7"/>
     <mergeCell ref="B7:B8"/>
-    <mergeCell ref="A59:A66"/>
-    <mergeCell ref="A67:A75"/>
-    <mergeCell ref="A9:A14"/>
-    <mergeCell ref="A15:A28"/>
-    <mergeCell ref="A29:A47"/>
-    <mergeCell ref="A57:A58"/>
-    <mergeCell ref="A51:A56"/>
-    <mergeCell ref="A48:A50"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Number" error="Please Enter Only Numbers. You may use .5 increments. " sqref="D9:D75">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Number" error="Please Enter Only Numbers. You may use .5 increments. " sqref="D9:D76">
       <formula1>0</formula1>
       <formula2>100000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Numbers Only" error="Please Enter Only Numbers. You may use .5 increments. " sqref="F9:K75">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Numbers Only" error="Please Enter Only Numbers. You may use .5 increments. " sqref="F9:K76">
       <formula1>0</formula1>
       <formula2>10000</formula2>
     </dataValidation>
@@ -4845,7 +4953,7 @@
           <x14:formula1>
             <xm:f>'Names-Hours'!$B$3:$B$9</xm:f>
           </x14:formula1>
-          <xm:sqref>C9:C75</xm:sqref>
+          <xm:sqref>C9:C76</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4861,15 +4969,15 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="78" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="23" t="s">
         <v>65</v>
       </c>
@@ -4877,8 +4985,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:4" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="69" t="s">
         <v>76</v>
       </c>
@@ -4892,7 +5000,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="71" t="s">
         <v>53</v>
       </c>
@@ -4906,7 +5014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="72" t="s">
         <v>55</v>
       </c>
@@ -4920,7 +5028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="72" t="s">
         <v>56</v>
       </c>
@@ -4934,7 +5042,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="72" t="s">
         <v>66</v>
       </c>
@@ -4948,7 +5056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="72" t="s">
         <v>67</v>
       </c>
@@ -4962,7 +5070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="72" t="s">
         <v>68</v>
       </c>
@@ -4976,7 +5084,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="72" t="s">
         <v>69</v>
       </c>
@@ -4990,7 +5098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="72" t="s">
         <v>70</v>
       </c>
@@ -5004,7 +5112,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="72" t="s">
         <v>71</v>
       </c>
@@ -5018,7 +5126,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="72" t="s">
         <v>72</v>
       </c>
@@ -5032,7 +5140,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="72" t="s">
         <v>73</v>
       </c>
@@ -5046,7 +5154,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="72" t="s">
         <v>74</v>
       </c>
@@ -5060,7 +5168,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="73" t="s">
         <v>75</v>
       </c>
@@ -5087,557 +5195,568 @@
       <selection activeCell="H21" sqref="H21:I23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="20.7109375" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" customWidth="1"/>
-    <col min="5" max="6" width="20.7109375" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" customWidth="1"/>
-    <col min="8" max="9" width="20.7109375" customWidth="1"/>
-    <col min="10" max="10" width="8.7109375" customWidth="1"/>
-    <col min="11" max="12" width="20.7109375" customWidth="1"/>
-    <col min="13" max="13" width="8.7109375" customWidth="1"/>
+    <col min="1" max="2" width="20.6640625" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" customWidth="1"/>
+    <col min="5" max="6" width="20.6640625" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" customWidth="1"/>
+    <col min="8" max="9" width="20.6640625" customWidth="1"/>
+    <col min="10" max="10" width="8.6640625" customWidth="1"/>
+    <col min="11" max="12" width="20.6640625" customWidth="1"/>
+    <col min="13" max="13" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="29.25" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="137" t="s">
+    <row r="1" spans="1:13" ht="29.4" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="105" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="138"/>
-      <c r="C1" s="139"/>
+      <c r="B1" s="106"/>
+      <c r="C1" s="107"/>
       <c r="D1" s="81"/>
-      <c r="E1" s="137" t="s">
+      <c r="E1" s="105" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="138"/>
-      <c r="G1" s="138"/>
-      <c r="H1" s="138"/>
-      <c r="I1" s="138"/>
-      <c r="J1" s="138"/>
-      <c r="K1" s="138"/>
-      <c r="L1" s="138"/>
-      <c r="M1" s="139"/>
-    </row>
-    <row r="2" spans="1:13" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="140"/>
-      <c r="B2" s="141"/>
-      <c r="C2" s="142"/>
+      <c r="F1" s="106"/>
+      <c r="G1" s="106"/>
+      <c r="H1" s="106"/>
+      <c r="I1" s="106"/>
+      <c r="J1" s="106"/>
+      <c r="K1" s="106"/>
+      <c r="L1" s="106"/>
+      <c r="M1" s="107"/>
+    </row>
+    <row r="2" spans="1:13" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="108"/>
+      <c r="B2" s="109"/>
+      <c r="C2" s="110"/>
       <c r="D2" s="81"/>
-      <c r="E2" s="140" t="s">
+      <c r="E2" s="108" t="s">
         <v>80</v>
       </c>
-      <c r="F2" s="141"/>
-      <c r="G2" s="142"/>
-      <c r="H2" s="141" t="s">
+      <c r="F2" s="109"/>
+      <c r="G2" s="110"/>
+      <c r="H2" s="109" t="s">
         <v>81</v>
       </c>
-      <c r="I2" s="141"/>
-      <c r="J2" s="142"/>
-      <c r="K2" s="141" t="s">
+      <c r="I2" s="109"/>
+      <c r="J2" s="110"/>
+      <c r="K2" s="109" t="s">
         <v>82</v>
       </c>
-      <c r="L2" s="141"/>
-      <c r="M2" s="142"/>
-    </row>
-    <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="129" t="str">
+      <c r="L2" s="109"/>
+      <c r="M2" s="110"/>
+    </row>
+    <row r="3" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="111" t="str">
         <f>Backlog!A11</f>
         <v>As a User, I want to be able to detect Par. in Chemical Diagram, so I can work with polymers</v>
       </c>
-      <c r="B3" s="130"/>
+      <c r="B3" s="112"/>
       <c r="C3" s="87">
         <f>Backlog!C11</f>
         <v>20</v>
       </c>
-      <c r="E3" s="105"/>
-      <c r="F3" s="106"/>
+      <c r="E3" s="131"/>
+      <c r="F3" s="132"/>
       <c r="G3" s="86"/>
-      <c r="H3" s="111" t="str">
+      <c r="H3" s="125" t="str">
         <f>Backlog!A4</f>
         <v>As a Developer, I need an architectural overview of OSRA’s processing, so I can understand the code base.</v>
       </c>
-      <c r="I3" s="112"/>
+      <c r="I3" s="126"/>
       <c r="J3" s="87">
         <f>Backlog!C4</f>
         <v>13</v>
       </c>
-      <c r="K3" s="105"/>
-      <c r="L3" s="106"/>
+      <c r="K3" s="131"/>
+      <c r="L3" s="132"/>
       <c r="M3" s="86"/>
     </row>
-    <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="131"/>
-      <c r="B4" s="132"/>
+    <row r="4" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="113"/>
+      <c r="B4" s="114"/>
       <c r="C4" s="88" t="str">
         <f>Backlog!B11</f>
         <v>M</v>
       </c>
-      <c r="E4" s="107"/>
-      <c r="F4" s="108"/>
+      <c r="E4" s="133"/>
+      <c r="F4" s="134"/>
       <c r="G4" s="84"/>
-      <c r="H4" s="113"/>
-      <c r="I4" s="114"/>
+      <c r="H4" s="127"/>
+      <c r="I4" s="128"/>
       <c r="J4" s="88" t="str">
         <f>Backlog!B4</f>
         <v>M</v>
       </c>
-      <c r="K4" s="107"/>
-      <c r="L4" s="108"/>
+      <c r="K4" s="133"/>
+      <c r="L4" s="134"/>
       <c r="M4" s="84"/>
     </row>
-    <row r="5" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="133"/>
-      <c r="B5" s="134"/>
+    <row r="5" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="115"/>
+      <c r="B5" s="116"/>
       <c r="C5" s="89"/>
-      <c r="E5" s="109"/>
-      <c r="F5" s="110"/>
+      <c r="E5" s="135"/>
+      <c r="F5" s="136"/>
       <c r="G5" s="85"/>
-      <c r="H5" s="115"/>
-      <c r="I5" s="116"/>
+      <c r="H5" s="129"/>
+      <c r="I5" s="130"/>
       <c r="J5" s="89"/>
-      <c r="K5" s="109"/>
-      <c r="L5" s="110"/>
+      <c r="K5" s="135"/>
+      <c r="L5" s="136"/>
       <c r="M5" s="85"/>
     </row>
-    <row r="6" spans="1:13" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="129" t="str">
+    <row r="6" spans="1:13" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="111" t="str">
         <f>Backlog!A12</f>
         <v>As a User, I want to be able to detect Brackets in Chemical Diagrams, so I can work with polymers</v>
       </c>
-      <c r="B6" s="130"/>
+      <c r="B6" s="112"/>
       <c r="C6" s="87">
         <f>Backlog!C12</f>
         <v>20</v>
       </c>
-      <c r="E6" s="105"/>
-      <c r="F6" s="106"/>
+      <c r="E6" s="131"/>
+      <c r="F6" s="132"/>
       <c r="G6" s="86"/>
-      <c r="H6" s="111" t="str">
+      <c r="H6" s="125" t="str">
         <f>Backlog!A5</f>
         <v>As a Developer, I need to review each aspect of OSRA’s architecture, so I can understand the code base.</v>
       </c>
-      <c r="I6" s="112"/>
+      <c r="I6" s="126"/>
       <c r="J6" s="87">
         <f>Backlog!C5</f>
         <v>20</v>
       </c>
-      <c r="K6" s="105"/>
-      <c r="L6" s="106"/>
+      <c r="K6" s="131"/>
+      <c r="L6" s="132"/>
       <c r="M6" s="86"/>
     </row>
-    <row r="7" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="131"/>
-      <c r="B7" s="132"/>
+    <row r="7" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="113"/>
+      <c r="B7" s="114"/>
       <c r="C7" s="88" t="str">
         <f>Backlog!B12</f>
         <v>S</v>
       </c>
-      <c r="E7" s="107"/>
-      <c r="F7" s="108"/>
+      <c r="E7" s="133"/>
+      <c r="F7" s="134"/>
       <c r="G7" s="84"/>
-      <c r="H7" s="113"/>
-      <c r="I7" s="114"/>
+      <c r="H7" s="127"/>
+      <c r="I7" s="128"/>
       <c r="J7" s="88" t="str">
         <f>Backlog!B5</f>
         <v>M</v>
       </c>
-      <c r="K7" s="107"/>
-      <c r="L7" s="108"/>
+      <c r="K7" s="133"/>
+      <c r="L7" s="134"/>
       <c r="M7" s="84"/>
     </row>
-    <row r="8" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="133"/>
-      <c r="B8" s="134"/>
+    <row r="8" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="115"/>
+      <c r="B8" s="116"/>
       <c r="C8" s="89"/>
-      <c r="E8" s="109"/>
-      <c r="F8" s="110"/>
+      <c r="E8" s="135"/>
+      <c r="F8" s="136"/>
       <c r="G8" s="85"/>
-      <c r="H8" s="115"/>
-      <c r="I8" s="116"/>
+      <c r="H8" s="129"/>
+      <c r="I8" s="130"/>
       <c r="J8" s="89"/>
-      <c r="K8" s="109"/>
-      <c r="L8" s="110"/>
+      <c r="K8" s="135"/>
+      <c r="L8" s="136"/>
       <c r="M8" s="85"/>
     </row>
-    <row r="9" spans="1:13" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="129" t="str">
+    <row r="9" spans="1:13" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="111" t="str">
         <f>Backlog!A13</f>
         <v>As a User, I want to be able to detect subscripts for polymer diagrams, so I can work with polymers</v>
       </c>
-      <c r="B9" s="130"/>
+      <c r="B9" s="112"/>
       <c r="C9" s="87">
         <f>Backlog!C13</f>
         <v>13</v>
       </c>
-      <c r="E9" s="105"/>
-      <c r="F9" s="106"/>
+      <c r="E9" s="131"/>
+      <c r="F9" s="132"/>
       <c r="G9" s="86"/>
-      <c r="H9" s="111" t="str">
+      <c r="H9" s="125" t="str">
         <f>Backlog!A6</f>
         <v>As a Developer, I need to get a basic grasp of O-Chem, so I can better understand use cases.</v>
       </c>
-      <c r="I9" s="112"/>
+      <c r="I9" s="126"/>
       <c r="J9" s="87">
         <f>Backlog!C6</f>
         <v>5</v>
       </c>
-      <c r="K9" s="105"/>
-      <c r="L9" s="106"/>
+      <c r="K9" s="131"/>
+      <c r="L9" s="132"/>
       <c r="M9" s="86"/>
     </row>
-    <row r="10" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="131"/>
-      <c r="B10" s="132"/>
+    <row r="10" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="113"/>
+      <c r="B10" s="114"/>
       <c r="C10" s="88" t="str">
         <f>Backlog!B13</f>
         <v>M</v>
       </c>
-      <c r="E10" s="107"/>
-      <c r="F10" s="108"/>
+      <c r="E10" s="133"/>
+      <c r="F10" s="134"/>
       <c r="G10" s="84"/>
-      <c r="H10" s="113"/>
-      <c r="I10" s="114"/>
+      <c r="H10" s="127"/>
+      <c r="I10" s="128"/>
       <c r="J10" s="88" t="str">
         <f>Backlog!B6</f>
         <v>M</v>
       </c>
-      <c r="K10" s="107"/>
-      <c r="L10" s="108"/>
+      <c r="K10" s="133"/>
+      <c r="L10" s="134"/>
       <c r="M10" s="84"/>
     </row>
-    <row r="11" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="133"/>
-      <c r="B11" s="134"/>
+    <row r="11" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="115"/>
+      <c r="B11" s="116"/>
       <c r="C11" s="89"/>
-      <c r="E11" s="109"/>
-      <c r="F11" s="110"/>
+      <c r="E11" s="135"/>
+      <c r="F11" s="136"/>
       <c r="G11" s="85"/>
-      <c r="H11" s="115"/>
-      <c r="I11" s="116"/>
+      <c r="H11" s="129"/>
+      <c r="I11" s="130"/>
       <c r="J11" s="89"/>
-      <c r="K11" s="109"/>
-      <c r="L11" s="110"/>
+      <c r="K11" s="135"/>
+      <c r="L11" s="136"/>
       <c r="M11" s="85"/>
     </row>
-    <row r="12" spans="1:13" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="129" t="str">
+    <row r="12" spans="1:13" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="111" t="str">
         <f>Backlog!A14</f>
         <v>As a User, I want to be able to detect “R-Notation”, so I can work with polymers</v>
       </c>
-      <c r="B12" s="130"/>
+      <c r="B12" s="112"/>
       <c r="C12" s="87" t="str">
         <f>Backlog!C14</f>
         <v>INF</v>
       </c>
-      <c r="E12" s="111" t="str">
+      <c r="E12" s="125" t="str">
         <f>Backlog!A7</f>
         <v>As a Developer, I need workflow and processes for the github repo, so I can collaborate on code</v>
       </c>
-      <c r="F12" s="112"/>
+      <c r="F12" s="126"/>
       <c r="G12" s="87">
         <f>Backlog!C7</f>
         <v>5</v>
       </c>
-      <c r="H12" s="105"/>
-      <c r="I12" s="106"/>
+      <c r="H12" s="131"/>
+      <c r="I12" s="132"/>
       <c r="J12" s="86"/>
-      <c r="K12" s="105"/>
-      <c r="L12" s="106"/>
+      <c r="K12" s="131"/>
+      <c r="L12" s="132"/>
       <c r="M12" s="86"/>
     </row>
-    <row r="13" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="131"/>
-      <c r="B13" s="132"/>
+    <row r="13" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="113"/>
+      <c r="B13" s="114"/>
       <c r="C13" s="88" t="str">
         <f>Backlog!B14</f>
         <v>W</v>
       </c>
-      <c r="E13" s="113"/>
-      <c r="F13" s="114"/>
+      <c r="E13" s="127"/>
+      <c r="F13" s="128"/>
       <c r="G13" s="88" t="str">
         <f>Backlog!B7</f>
         <v>M</v>
       </c>
-      <c r="H13" s="107"/>
-      <c r="I13" s="108"/>
+      <c r="H13" s="133"/>
+      <c r="I13" s="134"/>
       <c r="J13" s="84"/>
-      <c r="K13" s="107"/>
-      <c r="L13" s="108"/>
+      <c r="K13" s="133"/>
+      <c r="L13" s="134"/>
       <c r="M13" s="84"/>
     </row>
-    <row r="14" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="135"/>
-      <c r="B14" s="136"/>
+    <row r="14" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="117"/>
+      <c r="B14" s="118"/>
       <c r="C14" s="90"/>
-      <c r="E14" s="115"/>
-      <c r="F14" s="116"/>
+      <c r="E14" s="129"/>
+      <c r="F14" s="130"/>
       <c r="G14" s="89"/>
-      <c r="H14" s="109"/>
-      <c r="I14" s="110"/>
+      <c r="H14" s="135"/>
+      <c r="I14" s="136"/>
       <c r="J14" s="85"/>
-      <c r="K14" s="109"/>
-      <c r="L14" s="110"/>
+      <c r="K14" s="135"/>
+      <c r="L14" s="136"/>
       <c r="M14" s="85"/>
     </row>
-    <row r="15" spans="1:13" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="123"/>
-      <c r="B15" s="124"/>
+    <row r="15" spans="1:13" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="119"/>
+      <c r="B15" s="120"/>
       <c r="C15" s="87"/>
-      <c r="E15" s="111" t="str">
+      <c r="E15" s="125" t="str">
         <f>Backlog!A8</f>
         <v>As a Developer, I need a testing enviroment and test documentation, so I can better contribute to the codebase</v>
       </c>
-      <c r="F15" s="112"/>
+      <c r="F15" s="126"/>
       <c r="G15" s="87">
         <f>Backlog!C8</f>
         <v>20</v>
       </c>
-      <c r="H15" s="105"/>
-      <c r="I15" s="106"/>
+      <c r="H15" s="131"/>
+      <c r="I15" s="132"/>
       <c r="J15" s="86"/>
-      <c r="K15" s="105"/>
-      <c r="L15" s="106"/>
+      <c r="K15" s="131"/>
+      <c r="L15" s="132"/>
       <c r="M15" s="86"/>
     </row>
-    <row r="16" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="125"/>
-      <c r="B16" s="126"/>
+    <row r="16" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="121"/>
+      <c r="B16" s="122"/>
       <c r="C16" s="88"/>
-      <c r="E16" s="113"/>
-      <c r="F16" s="114"/>
+      <c r="E16" s="127"/>
+      <c r="F16" s="128"/>
       <c r="G16" s="88" t="str">
         <f>Backlog!B8</f>
         <v>M</v>
       </c>
-      <c r="H16" s="107"/>
-      <c r="I16" s="108"/>
+      <c r="H16" s="133"/>
+      <c r="I16" s="134"/>
       <c r="J16" s="84"/>
-      <c r="K16" s="107"/>
-      <c r="L16" s="108"/>
+      <c r="K16" s="133"/>
+      <c r="L16" s="134"/>
       <c r="M16" s="84"/>
     </row>
-    <row r="17" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="127"/>
-      <c r="B17" s="128"/>
+    <row r="17" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="123"/>
+      <c r="B17" s="124"/>
       <c r="C17" s="89"/>
-      <c r="E17" s="115"/>
-      <c r="F17" s="116"/>
+      <c r="E17" s="129"/>
+      <c r="F17" s="130"/>
       <c r="G17" s="89"/>
-      <c r="H17" s="109"/>
-      <c r="I17" s="110"/>
+      <c r="H17" s="135"/>
+      <c r="I17" s="136"/>
       <c r="J17" s="85"/>
-      <c r="K17" s="109"/>
-      <c r="L17" s="110"/>
+      <c r="K17" s="135"/>
+      <c r="L17" s="136"/>
       <c r="M17" s="85"/>
     </row>
-    <row r="18" spans="1:13" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="123"/>
-      <c r="B18" s="124"/>
+    <row r="18" spans="1:13" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="119"/>
+      <c r="B18" s="120"/>
       <c r="C18" s="87"/>
-      <c r="E18" s="111" t="str">
+      <c r="E18" s="125" t="str">
         <f>Backlog!A9</f>
         <v>As a Developer, I need to have consolidated documentation from other developers, so I can better contribute to the codebase</v>
       </c>
-      <c r="F18" s="112"/>
+      <c r="F18" s="126"/>
       <c r="G18" s="87">
         <f>Backlog!C9</f>
         <v>13</v>
       </c>
-      <c r="H18" s="105"/>
-      <c r="I18" s="106"/>
+      <c r="H18" s="131"/>
+      <c r="I18" s="132"/>
       <c r="J18" s="86"/>
-      <c r="K18" s="105"/>
-      <c r="L18" s="106"/>
+      <c r="K18" s="131"/>
+      <c r="L18" s="132"/>
       <c r="M18" s="86"/>
     </row>
-    <row r="19" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="125"/>
-      <c r="B19" s="126"/>
+    <row r="19" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="121"/>
+      <c r="B19" s="122"/>
       <c r="C19" s="88"/>
-      <c r="E19" s="113"/>
-      <c r="F19" s="114"/>
+      <c r="E19" s="127"/>
+      <c r="F19" s="128"/>
       <c r="G19" s="88" t="str">
         <f>Backlog!B9</f>
         <v>M</v>
       </c>
-      <c r="H19" s="107"/>
-      <c r="I19" s="108"/>
+      <c r="H19" s="133"/>
+      <c r="I19" s="134"/>
       <c r="J19" s="84"/>
-      <c r="K19" s="107"/>
-      <c r="L19" s="108"/>
+      <c r="K19" s="133"/>
+      <c r="L19" s="134"/>
       <c r="M19" s="84"/>
     </row>
-    <row r="20" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="127"/>
-      <c r="B20" s="128"/>
+    <row r="20" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="123"/>
+      <c r="B20" s="124"/>
       <c r="C20" s="89"/>
-      <c r="E20" s="115"/>
-      <c r="F20" s="116"/>
+      <c r="E20" s="129"/>
+      <c r="F20" s="130"/>
       <c r="G20" s="89"/>
-      <c r="H20" s="109"/>
-      <c r="I20" s="110"/>
+      <c r="H20" s="135"/>
+      <c r="I20" s="136"/>
       <c r="J20" s="85"/>
-      <c r="K20" s="109"/>
-      <c r="L20" s="110"/>
+      <c r="K20" s="135"/>
+      <c r="L20" s="136"/>
       <c r="M20" s="85"/>
     </row>
-    <row r="21" spans="1:13" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="123"/>
-      <c r="B21" s="124"/>
+    <row r="21" spans="1:13" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="119"/>
+      <c r="B21" s="120"/>
       <c r="C21" s="87"/>
-      <c r="E21" s="111" t="str">
+      <c r="E21" s="125" t="str">
         <f>Backlog!A10</f>
         <v>As a Developer, I need to understand SMILES notation and .SD file structure, so I can desing the smile data structure.</v>
       </c>
-      <c r="F21" s="112"/>
+      <c r="F21" s="126"/>
       <c r="G21" s="87">
         <f>Backlog!C10</f>
         <v>5</v>
       </c>
-      <c r="H21" s="105"/>
-      <c r="I21" s="106"/>
+      <c r="H21" s="131"/>
+      <c r="I21" s="132"/>
       <c r="J21" s="86"/>
-      <c r="K21" s="105"/>
-      <c r="L21" s="106"/>
+      <c r="K21" s="131"/>
+      <c r="L21" s="132"/>
       <c r="M21" s="86"/>
     </row>
-    <row r="22" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="125"/>
-      <c r="B22" s="126"/>
+    <row r="22" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="121"/>
+      <c r="B22" s="122"/>
       <c r="C22" s="88"/>
-      <c r="E22" s="113"/>
-      <c r="F22" s="114"/>
+      <c r="E22" s="127"/>
+      <c r="F22" s="128"/>
       <c r="G22" s="88" t="str">
         <f>Backlog!B10</f>
         <v>M</v>
       </c>
-      <c r="H22" s="107"/>
-      <c r="I22" s="108"/>
+      <c r="H22" s="133"/>
+      <c r="I22" s="134"/>
       <c r="J22" s="84"/>
-      <c r="K22" s="107"/>
-      <c r="L22" s="108"/>
+      <c r="K22" s="133"/>
+      <c r="L22" s="134"/>
       <c r="M22" s="84"/>
     </row>
-    <row r="23" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="127"/>
-      <c r="B23" s="128"/>
+    <row r="23" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="123"/>
+      <c r="B23" s="124"/>
       <c r="C23" s="89"/>
-      <c r="E23" s="115"/>
-      <c r="F23" s="116"/>
+      <c r="E23" s="129"/>
+      <c r="F23" s="130"/>
       <c r="G23" s="89"/>
-      <c r="H23" s="109"/>
-      <c r="I23" s="110"/>
+      <c r="H23" s="135"/>
+      <c r="I23" s="136"/>
       <c r="J23" s="85"/>
-      <c r="K23" s="109"/>
-      <c r="L23" s="110"/>
+      <c r="K23" s="135"/>
+      <c r="L23" s="136"/>
       <c r="M23" s="85"/>
     </row>
-    <row r="24" spans="1:13" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="123"/>
-      <c r="B24" s="124"/>
+    <row r="24" spans="1:13" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="119"/>
+      <c r="B24" s="120"/>
       <c r="C24" s="87"/>
-      <c r="E24" s="111" t="str">
+      <c r="E24" s="125" t="str">
         <f>Backlog!A15</f>
         <v>As a User, I want to have a data structure for encoding polymers in “Smile Notation”, so I can work with polymers</v>
       </c>
-      <c r="F24" s="112"/>
+      <c r="F24" s="126"/>
       <c r="G24" s="87">
         <f>Backlog!C15</f>
         <v>13</v>
       </c>
-      <c r="H24" s="105"/>
-      <c r="I24" s="106"/>
+      <c r="H24" s="131"/>
+      <c r="I24" s="132"/>
       <c r="J24" s="86"/>
-      <c r="K24" s="105"/>
-      <c r="L24" s="106"/>
+      <c r="K24" s="131"/>
+      <c r="L24" s="132"/>
       <c r="M24" s="86"/>
     </row>
-    <row r="25" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="125"/>
-      <c r="B25" s="126"/>
+    <row r="25" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="121"/>
+      <c r="B25" s="122"/>
       <c r="C25" s="88"/>
-      <c r="E25" s="113"/>
-      <c r="F25" s="114"/>
+      <c r="E25" s="127"/>
+      <c r="F25" s="128"/>
       <c r="G25" s="88" t="str">
         <f>Backlog!B15</f>
         <v>M</v>
       </c>
-      <c r="H25" s="107"/>
-      <c r="I25" s="108"/>
+      <c r="H25" s="133"/>
+      <c r="I25" s="134"/>
       <c r="J25" s="84"/>
-      <c r="K25" s="107"/>
-      <c r="L25" s="108"/>
+      <c r="K25" s="133"/>
+      <c r="L25" s="134"/>
       <c r="M25" s="84"/>
     </row>
-    <row r="26" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="127"/>
-      <c r="B26" s="128"/>
+    <row r="26" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="123"/>
+      <c r="B26" s="124"/>
       <c r="C26" s="89"/>
-      <c r="E26" s="115"/>
-      <c r="F26" s="116"/>
+      <c r="E26" s="129"/>
+      <c r="F26" s="130"/>
       <c r="G26" s="89"/>
-      <c r="H26" s="109"/>
-      <c r="I26" s="110"/>
+      <c r="H26" s="135"/>
+      <c r="I26" s="136"/>
       <c r="J26" s="85"/>
-      <c r="K26" s="109"/>
-      <c r="L26" s="110"/>
+      <c r="K26" s="135"/>
+      <c r="L26" s="136"/>
       <c r="M26" s="85"/>
     </row>
-    <row r="27" spans="1:13" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="123"/>
-      <c r="B27" s="124"/>
+    <row r="27" spans="1:13" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="119"/>
+      <c r="B27" s="120"/>
       <c r="C27" s="87"/>
-      <c r="E27" s="117"/>
-      <c r="F27" s="118"/>
+      <c r="E27" s="137"/>
+      <c r="F27" s="138"/>
       <c r="G27" s="87"/>
-      <c r="H27" s="105"/>
-      <c r="I27" s="106"/>
+      <c r="H27" s="131"/>
+      <c r="I27" s="132"/>
       <c r="J27" s="86"/>
-      <c r="K27" s="105"/>
-      <c r="L27" s="106"/>
+      <c r="K27" s="131"/>
+      <c r="L27" s="132"/>
       <c r="M27" s="86"/>
     </row>
-    <row r="28" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="125"/>
-      <c r="B28" s="126"/>
+    <row r="28" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="121"/>
+      <c r="B28" s="122"/>
       <c r="C28" s="88"/>
-      <c r="E28" s="119"/>
-      <c r="F28" s="120"/>
+      <c r="E28" s="139"/>
+      <c r="F28" s="140"/>
       <c r="G28" s="88"/>
-      <c r="H28" s="107"/>
-      <c r="I28" s="108"/>
+      <c r="H28" s="133"/>
+      <c r="I28" s="134"/>
       <c r="J28" s="84"/>
-      <c r="K28" s="107"/>
-      <c r="L28" s="108"/>
+      <c r="K28" s="133"/>
+      <c r="L28" s="134"/>
       <c r="M28" s="84"/>
     </row>
-    <row r="29" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="127"/>
-      <c r="B29" s="128"/>
+    <row r="29" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="123"/>
+      <c r="B29" s="124"/>
       <c r="C29" s="89"/>
-      <c r="E29" s="121"/>
-      <c r="F29" s="122"/>
+      <c r="E29" s="141"/>
+      <c r="F29" s="142"/>
       <c r="G29" s="89"/>
-      <c r="H29" s="109"/>
-      <c r="I29" s="110"/>
+      <c r="H29" s="135"/>
+      <c r="I29" s="136"/>
       <c r="J29" s="85"/>
-      <c r="K29" s="109"/>
-      <c r="L29" s="110"/>
+      <c r="K29" s="135"/>
+      <c r="L29" s="136"/>
       <c r="M29" s="85"/>
     </row>
-    <row r="30" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="E1:M1"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="K2:M2"/>
-    <mergeCell ref="A1:C2"/>
-    <mergeCell ref="A3:B5"/>
-    <mergeCell ref="A6:B8"/>
-    <mergeCell ref="A9:B11"/>
-    <mergeCell ref="A12:B14"/>
-    <mergeCell ref="A15:B17"/>
+    <mergeCell ref="K18:L20"/>
+    <mergeCell ref="K21:L23"/>
+    <mergeCell ref="K24:L26"/>
+    <mergeCell ref="K27:L29"/>
+    <mergeCell ref="H21:I23"/>
+    <mergeCell ref="H24:I26"/>
+    <mergeCell ref="H27:I29"/>
+    <mergeCell ref="H18:I20"/>
+    <mergeCell ref="K3:L5"/>
+    <mergeCell ref="K6:L8"/>
+    <mergeCell ref="K9:L11"/>
+    <mergeCell ref="K12:L14"/>
+    <mergeCell ref="K15:L17"/>
+    <mergeCell ref="E18:F20"/>
+    <mergeCell ref="E21:F23"/>
+    <mergeCell ref="E24:F26"/>
+    <mergeCell ref="E27:F29"/>
+    <mergeCell ref="A21:B23"/>
+    <mergeCell ref="A24:B26"/>
+    <mergeCell ref="A27:B29"/>
+    <mergeCell ref="A18:B20"/>
     <mergeCell ref="H3:I5"/>
     <mergeCell ref="H6:I8"/>
     <mergeCell ref="H9:I11"/>
@@ -5646,29 +5765,18 @@
     <mergeCell ref="E3:F5"/>
     <mergeCell ref="E6:F8"/>
     <mergeCell ref="E9:F11"/>
-    <mergeCell ref="E18:F20"/>
-    <mergeCell ref="E21:F23"/>
-    <mergeCell ref="E24:F26"/>
-    <mergeCell ref="E27:F29"/>
-    <mergeCell ref="A21:B23"/>
-    <mergeCell ref="A24:B26"/>
-    <mergeCell ref="A27:B29"/>
-    <mergeCell ref="A18:B20"/>
     <mergeCell ref="H12:I14"/>
     <mergeCell ref="H15:I17"/>
-    <mergeCell ref="K3:L5"/>
-    <mergeCell ref="K6:L8"/>
-    <mergeCell ref="K9:L11"/>
-    <mergeCell ref="K12:L14"/>
-    <mergeCell ref="K15:L17"/>
-    <mergeCell ref="K18:L20"/>
-    <mergeCell ref="K21:L23"/>
-    <mergeCell ref="K24:L26"/>
-    <mergeCell ref="K27:L29"/>
-    <mergeCell ref="H21:I23"/>
-    <mergeCell ref="H24:I26"/>
-    <mergeCell ref="H27:I29"/>
-    <mergeCell ref="H18:I20"/>
+    <mergeCell ref="A3:B5"/>
+    <mergeCell ref="A6:B8"/>
+    <mergeCell ref="A9:B11"/>
+    <mergeCell ref="A12:B14"/>
+    <mergeCell ref="A15:B17"/>
+    <mergeCell ref="E1:M1"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="A1:C2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5682,20 +5790,20 @@
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9.109375" style="2"/>
     <col min="2" max="2" width="11" style="2" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26" style="2" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.7109375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="31.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="2"/>
+    <col min="6" max="6" width="20.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.6640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="31.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
         <v>11</v>
@@ -5716,7 +5824,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>22</v>
       </c>
@@ -5741,7 +5849,7 @@
         <v>24.5</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
@@ -5766,7 +5874,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>23</v>
       </c>
@@ -5791,7 +5899,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
         <v>24</v>
       </c>
@@ -5816,7 +5924,7 @@
         <v>24.5</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
         <v>52</v>
       </c>
@@ -5841,7 +5949,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
         <v>25</v>
       </c>
@@ -5866,7 +5974,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
         <v>87</v>
       </c>
@@ -5904,18 +6012,18 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="143">
         <v>41557</v>
       </c>
@@ -5923,7 +6031,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="143"/>
       <c r="B3" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
Removed User Stories that we decided to move
</commit_message>
<xml_diff>
--- a/bookkeeping/Sprint1 BurnUp.xlsx
+++ b/bookkeeping/Sprint1 BurnUp.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="0" windowWidth="7476" windowHeight="3756" tabRatio="601"/>
+    <workbookView xWindow="1020" yWindow="0" windowWidth="7470" windowHeight="3750" tabRatio="601" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks List" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="81">
   <si>
     <t>Sprint 1</t>
   </si>
@@ -179,15 +179,6 @@
     <t>Create template for indevidual's documentation</t>
   </si>
   <si>
-    <t>Review .SD File contents</t>
-  </si>
-  <si>
-    <t>Review SMILES notation documentations</t>
-  </si>
-  <si>
-    <t>Create DB Schema</t>
-  </si>
-  <si>
     <t>David</t>
   </si>
   <si>
@@ -212,19 +203,7 @@
     <t>As a Developer, I need to have consolidated documentation from other developers, so I can be</t>
   </si>
   <si>
-    <t>As a Developer, I need to understand SMILES notation and .SD file structure, so I can desing</t>
-  </si>
-  <si>
-    <t>As a User, I want to have a data structure for encoding polymers in “Smile Notation”, so I c</t>
-  </si>
-  <si>
     <t>Create Development Workflow</t>
-  </si>
-  <si>
-    <t>Design DB Access Layer</t>
-  </si>
-  <si>
-    <t>Design Object Model</t>
   </si>
   <si>
     <t>Backlog</t>
@@ -1547,6 +1526,41 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="59" xfId="2" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="57" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="4" borderId="64" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="4" borderId="59" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="4" borderId="65" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="4" borderId="57" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1583,32 +1597,77 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1634,106 +1693,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="59" xfId="2" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="57" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="4" borderId="64" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="4" borderId="59" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="4" borderId="65" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="4" borderId="57" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1853,7 +1832,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Tasks List'!$E$81</c:f>
+              <c:f>'Tasks List'!$E$64</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1919,7 +1898,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Tasks List'!$E$78:$K$78</c:f>
+              <c:f>'Tasks List'!$E$61:$K$61</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1954,7 +1933,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Tasks List'!$F$81</c:f>
+              <c:f>'Tasks List'!$F$64</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2020,30 +1999,30 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Tasks List'!$E$79:$K$79</c:f>
+              <c:f>'Tasks List'!$E$62:$K$62</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>162</c:v>
+                  <c:v>147</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>162</c:v>
+                  <c:v>147</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>162</c:v>
+                  <c:v>147</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>162</c:v>
+                  <c:v>147</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>162</c:v>
+                  <c:v>147</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>162</c:v>
+                  <c:v>147</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>162</c:v>
+                  <c:v>147</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2055,7 +2034,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Tasks List'!$G$81</c:f>
+              <c:f>'Tasks List'!$G$64</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2124,7 +2103,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Tasks List'!$E$80:$K$80</c:f>
+              <c:f>'Tasks List'!$E$63:$K$63</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -2132,7 +2111,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>162</c:v>
+                  <c:v>147</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2164,11 +2143,11 @@
         </c:dropLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="255715648"/>
-        <c:axId val="255715256"/>
+        <c:axId val="301280016"/>
+        <c:axId val="301281584"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="255715648"/>
+        <c:axId val="301280016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2211,14 +2190,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="255715256"/>
+        <c:crossAx val="301281584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="255715256"/>
+        <c:axId val="301281584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2255,7 +2234,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="255715648"/>
+        <c:crossAx val="301280016"/>
         <c:crossesAt val="41548"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="10"/>
@@ -2936,7 +2915,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -3234,24 +3213,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T100"/>
+  <dimension ref="A1:T83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView topLeftCell="A40" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B83" sqref="B83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.88671875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="76.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.44140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="14.109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" style="2" hidden="1" customWidth="1"/>
-    <col min="6" max="11" width="11.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.109375" style="2"/>
+    <col min="1" max="1" width="40.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="76.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" style="2" hidden="1" customWidth="1"/>
+    <col min="6" max="11" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
@@ -3262,18 +3241,18 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="21"/>
       <c r="B2" s="22"/>
       <c r="D2" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="91" t="s">
+      <c r="F2" s="101" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="92"/>
-    </row>
-    <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G2" s="102"/>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>26</v>
       </c>
@@ -3282,27 +3261,27 @@
         <v>Nicholas</v>
       </c>
       <c r="F3" s="7" t="str">
-        <f>('Names-Hours'!H3) - (SUMIF(C9:C76,D3,D9:D76))&amp;+"/"&amp;+'Names-Hours'!D3</f>
-        <v>-6.5/30</v>
+        <f>('Names-Hours'!H3) - (SUMIF(C9:C59,D3,D9:D59))&amp;+"/"&amp;+'Names-Hours'!D3</f>
+        <v>-6/30</v>
       </c>
       <c r="G3" s="6" t="str">
         <f>'Names-Hours'!B5</f>
         <v>Igor</v>
       </c>
       <c r="H3" s="7" t="str">
-        <f>('Names-Hours'!H3) -(SUMIF(C9:C76,G3,D9:D76)) &amp;+"/"&amp;+'Names-Hours'!D5</f>
-        <v>-3.5/30</v>
+        <f>('Names-Hours'!H3) -(SUMIF(C9:C59,G3,D9:D59)) &amp;+"/"&amp;+'Names-Hours'!D5</f>
+        <v>0/30</v>
       </c>
       <c r="I3" s="6" t="str">
         <f>'Names-Hours'!B7</f>
         <v>David</v>
       </c>
       <c r="J3" s="7" t="str">
-        <f>('Names-Hours'!H4) -(SUMIF(C9:C76,I3,D9:D76)) &amp;+"/"&amp;+ 'Names-Hours'!D7</f>
-        <v>3/30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <f>('Names-Hours'!H4) -(SUMIF(C9:C59,I3,D9:D59)) &amp;+"/"&amp;+ 'Names-Hours'!D7</f>
+        <v>3.5/30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="19" t="s">
         <v>27</v>
       </c>
@@ -3312,27 +3291,27 @@
         <v>Konstantin</v>
       </c>
       <c r="F4" s="7" t="str">
-        <f>('Names-Hours'!H4) -(SUMIF(C9:C76,D4,D9:D76))&amp;+"/"&amp;+'Names-Hours'!D4</f>
-        <v>-3/30</v>
+        <f>('Names-Hours'!H4) -(SUMIF(C9:C59,D4,D9:D59))&amp;+"/"&amp;+'Names-Hours'!D4</f>
+        <v>2/30</v>
       </c>
       <c r="G4" s="6" t="str">
         <f>'Names-Hours'!B6</f>
         <v>Nathan</v>
       </c>
       <c r="H4" s="7" t="str">
-        <f>('Names-Hours'!H4) -(SUMIF(C9:C76,G4,D9:D76)) &amp;+"/"&amp;+'Names-Hours'!D6</f>
-        <v>-6.5/30</v>
+        <f>('Names-Hours'!H4) -(SUMIF(C9:C59,G4,D9:D59)) &amp;+"/"&amp;+'Names-Hours'!D6</f>
+        <v>-6/30</v>
       </c>
       <c r="I4" s="6" t="str">
         <f>'Names-Hours'!B8</f>
         <v>Thomas</v>
       </c>
       <c r="J4" s="7" t="str">
-        <f>('Names-Hours'!H4) -(SUMIF(C9:C76,I4,D9:D76)) &amp;+"/"&amp;+ 'Names-Hours'!D8</f>
-        <v>-2/30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <f>('Names-Hours'!H4) -(SUMIF(C9:C59,I4,D9:D59)) &amp;+"/"&amp;+ 'Names-Hours'!D8</f>
+        <v>3/30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="9"/>
       <c r="D5" s="25" t="s">
         <v>21</v>
@@ -3344,36 +3323,36 @@
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
     </row>
-    <row r="6" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="7" spans="1:12" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="97" t="s">
+    <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:12" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="107" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="97" t="s">
+      <c r="B7" s="107" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="93" t="s">
+      <c r="C7" s="103" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="95" t="s">
+      <c r="D7" s="105" t="s">
         <v>9</v>
       </c>
       <c r="E7" s="27"/>
-      <c r="F7" s="99" t="s">
+      <c r="F7" s="109" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="100"/>
-      <c r="H7" s="100"/>
-      <c r="I7" s="100"/>
-      <c r="J7" s="100"/>
-      <c r="K7" s="101"/>
+      <c r="G7" s="110"/>
+      <c r="H7" s="110"/>
+      <c r="I7" s="110"/>
+      <c r="J7" s="110"/>
+      <c r="K7" s="111"/>
       <c r="L7" s="16"/>
     </row>
-    <row r="8" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="98"/>
-      <c r="B8" s="98"/>
-      <c r="C8" s="94"/>
-      <c r="D8" s="96"/>
+    <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="108"/>
+      <c r="B8" s="108"/>
+      <c r="C8" s="104"/>
+      <c r="D8" s="106"/>
       <c r="E8" s="10">
         <v>41661</v>
       </c>
@@ -3396,9 +3375,9 @@
         <v>41675</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="16.2" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="104" t="s">
-        <v>53</v>
+    <row r="9" spans="1:12" ht="16.149999999999999" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="100" t="s">
+        <v>50</v>
       </c>
       <c r="B9" s="36" t="s">
         <v>32</v>
@@ -3421,8 +3400,8 @@
       <c r="J9" s="42"/>
       <c r="K9" s="43"/>
     </row>
-    <row r="10" spans="1:12" ht="15" x14ac:dyDescent="0.3">
-      <c r="A10" s="102"/>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="98"/>
       <c r="B10" s="44" t="s">
         <v>32</v>
       </c>
@@ -3442,8 +3421,8 @@
       <c r="J10" s="34"/>
       <c r="K10" s="35"/>
     </row>
-    <row r="11" spans="1:12" ht="15" x14ac:dyDescent="0.3">
-      <c r="A11" s="102"/>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="98"/>
       <c r="B11" s="46" t="s">
         <v>33</v>
       </c>
@@ -3463,8 +3442,8 @@
       <c r="J11" s="52"/>
       <c r="K11" s="53"/>
     </row>
-    <row r="12" spans="1:12" ht="15" x14ac:dyDescent="0.3">
-      <c r="A12" s="102"/>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="98"/>
       <c r="B12" s="44" t="s">
         <v>33</v>
       </c>
@@ -3484,13 +3463,13 @@
       <c r="J12" s="34"/>
       <c r="K12" s="35"/>
     </row>
-    <row r="13" spans="1:12" ht="15" x14ac:dyDescent="0.3">
-      <c r="A13" s="102"/>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="98"/>
       <c r="B13" s="46" t="s">
         <v>31</v>
       </c>
       <c r="C13" s="47" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D13" s="48">
         <v>3</v>
@@ -3503,10 +3482,10 @@
       <c r="J13" s="52"/>
       <c r="K13" s="53"/>
     </row>
-    <row r="14" spans="1:12" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="103"/>
+    <row r="14" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="99"/>
       <c r="B14" s="54" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C14" s="14" t="s">
         <v>22</v>
@@ -3528,9 +3507,9 @@
       <c r="J14" s="58"/>
       <c r="K14" s="59"/>
     </row>
-    <row r="15" spans="1:12" ht="15.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="102" t="s">
-        <v>55</v>
+    <row r="15" spans="1:12" ht="15.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="98" t="s">
+        <v>52</v>
       </c>
       <c r="B15" s="46" t="s">
         <v>35</v>
@@ -3551,8 +3530,8 @@
       <c r="J15" s="52"/>
       <c r="K15" s="53"/>
     </row>
-    <row r="16" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="102"/>
+    <row r="16" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="98"/>
       <c r="B16" s="44" t="s">
         <v>35</v>
       </c>
@@ -3570,8 +3549,8 @@
       <c r="J16" s="34"/>
       <c r="K16" s="35"/>
     </row>
-    <row r="17" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="102"/>
+    <row r="17" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="98"/>
       <c r="B17" s="46" t="s">
         <v>35</v>
       </c>
@@ -3595,8 +3574,8 @@
       <c r="J17" s="52"/>
       <c r="K17" s="53"/>
     </row>
-    <row r="18" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="102"/>
+    <row r="18" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="98"/>
       <c r="B18" s="44" t="s">
         <v>35</v>
       </c>
@@ -3618,13 +3597,13 @@
       <c r="J18" s="34"/>
       <c r="K18" s="35"/>
     </row>
-    <row r="19" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="102"/>
+    <row r="19" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="98"/>
       <c r="B19" s="46" t="s">
         <v>35</v>
       </c>
       <c r="C19" s="47" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D19" s="48">
         <v>8</v>
@@ -3641,8 +3620,8 @@
       <c r="J19" s="52"/>
       <c r="K19" s="53"/>
     </row>
-    <row r="20" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="102"/>
+    <row r="20" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="98"/>
       <c r="B20" s="44" t="s">
         <v>35</v>
       </c>
@@ -3664,8 +3643,8 @@
       <c r="J20" s="34"/>
       <c r="K20" s="35"/>
     </row>
-    <row r="21" spans="1:11" ht="15" x14ac:dyDescent="0.3">
-      <c r="A21" s="102"/>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="98"/>
       <c r="B21" s="46" t="s">
         <v>34</v>
       </c>
@@ -3683,8 +3662,8 @@
       <c r="J21" s="52"/>
       <c r="K21" s="53"/>
     </row>
-    <row r="22" spans="1:11" ht="15" x14ac:dyDescent="0.3">
-      <c r="A22" s="102"/>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="98"/>
       <c r="B22" s="44" t="s">
         <v>34</v>
       </c>
@@ -3702,8 +3681,8 @@
       <c r="J22" s="34"/>
       <c r="K22" s="35"/>
     </row>
-    <row r="23" spans="1:11" ht="15" x14ac:dyDescent="0.3">
-      <c r="A23" s="102"/>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="98"/>
       <c r="B23" s="46" t="s">
         <v>36</v>
       </c>
@@ -3721,8 +3700,8 @@
       <c r="J23" s="52"/>
       <c r="K23" s="53"/>
     </row>
-    <row r="24" spans="1:11" ht="15" x14ac:dyDescent="0.3">
-      <c r="A24" s="102"/>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="98"/>
       <c r="B24" s="44" t="s">
         <v>36</v>
       </c>
@@ -3742,8 +3721,8 @@
       <c r="J24" s="34"/>
       <c r="K24" s="35"/>
     </row>
-    <row r="25" spans="1:11" ht="15" x14ac:dyDescent="0.3">
-      <c r="A25" s="102"/>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="98"/>
       <c r="B25" s="46" t="s">
         <v>36</v>
       </c>
@@ -3763,8 +3742,8 @@
       <c r="J25" s="52"/>
       <c r="K25" s="53"/>
     </row>
-    <row r="26" spans="1:11" ht="15" x14ac:dyDescent="0.3">
-      <c r="A26" s="102"/>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="98"/>
       <c r="B26" s="44" t="s">
         <v>36</v>
       </c>
@@ -3784,13 +3763,13 @@
       <c r="J26" s="34"/>
       <c r="K26" s="35"/>
     </row>
-    <row r="27" spans="1:11" ht="15" x14ac:dyDescent="0.3">
-      <c r="A27" s="102"/>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="98"/>
       <c r="B27" s="46" t="s">
         <v>36</v>
       </c>
       <c r="C27" s="47" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D27" s="48">
         <v>3</v>
@@ -3807,8 +3786,8 @@
       <c r="J27" s="52"/>
       <c r="K27" s="53"/>
     </row>
-    <row r="28" spans="1:11" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="103"/>
+    <row r="28" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="99"/>
       <c r="B28" s="54" t="s">
         <v>36</v>
       </c>
@@ -3830,9 +3809,9 @@
       <c r="J28" s="58"/>
       <c r="K28" s="59"/>
     </row>
-    <row r="29" spans="1:11" ht="15.6" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="102" t="s">
-        <v>56</v>
+    <row r="29" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="98" t="s">
+        <v>53</v>
       </c>
       <c r="B29" s="46" t="s">
         <v>37</v>
@@ -3851,8 +3830,8 @@
       <c r="J29" s="52"/>
       <c r="K29" s="53"/>
     </row>
-    <row r="30" spans="1:11" ht="15" x14ac:dyDescent="0.3">
-      <c r="A30" s="102"/>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="98"/>
       <c r="B30" s="44" t="s">
         <v>37</v>
       </c>
@@ -3872,8 +3851,8 @@
       <c r="J30" s="34"/>
       <c r="K30" s="35"/>
     </row>
-    <row r="31" spans="1:11" ht="15" x14ac:dyDescent="0.3">
-      <c r="A31" s="102"/>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="98"/>
       <c r="B31" s="46" t="s">
         <v>37</v>
       </c>
@@ -3893,8 +3872,8 @@
       <c r="J31" s="52"/>
       <c r="K31" s="53"/>
     </row>
-    <row r="32" spans="1:11" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="102"/>
+    <row r="32" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="98"/>
       <c r="B32" s="44" t="s">
         <v>37</v>
       </c>
@@ -3914,13 +3893,13 @@
       <c r="J32" s="34"/>
       <c r="K32" s="35"/>
     </row>
-    <row r="33" spans="1:11" ht="15" x14ac:dyDescent="0.3">
-      <c r="A33" s="102"/>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="98"/>
       <c r="B33" s="46" t="s">
         <v>37</v>
       </c>
       <c r="C33" s="47" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D33" s="48">
         <v>3</v>
@@ -3935,8 +3914,8 @@
       <c r="J33" s="52"/>
       <c r="K33" s="53"/>
     </row>
-    <row r="34" spans="1:11" ht="15" x14ac:dyDescent="0.3">
-      <c r="A34" s="102"/>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="98"/>
       <c r="B34" s="44" t="s">
         <v>37</v>
       </c>
@@ -3954,8 +3933,8 @@
       <c r="J34" s="34"/>
       <c r="K34" s="35"/>
     </row>
-    <row r="35" spans="1:11" ht="15" x14ac:dyDescent="0.3">
-      <c r="A35" s="102"/>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="98"/>
       <c r="B35" s="46" t="s">
         <v>38</v>
       </c>
@@ -3973,8 +3952,8 @@
       <c r="J35" s="52"/>
       <c r="K35" s="53"/>
     </row>
-    <row r="36" spans="1:11" ht="15" x14ac:dyDescent="0.3">
-      <c r="A36" s="102"/>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="98"/>
       <c r="B36" s="44" t="s">
         <v>38</v>
       </c>
@@ -3992,8 +3971,8 @@
       <c r="J36" s="34"/>
       <c r="K36" s="35"/>
     </row>
-    <row r="37" spans="1:11" ht="15" x14ac:dyDescent="0.3">
-      <c r="A37" s="102"/>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="98"/>
       <c r="B37" s="46" t="s">
         <v>38</v>
       </c>
@@ -4011,8 +3990,8 @@
       <c r="J37" s="52"/>
       <c r="K37" s="53"/>
     </row>
-    <row r="38" spans="1:11" ht="15" x14ac:dyDescent="0.3">
-      <c r="A38" s="102"/>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="98"/>
       <c r="B38" s="44" t="s">
         <v>38</v>
       </c>
@@ -4030,13 +4009,13 @@
       <c r="J38" s="34"/>
       <c r="K38" s="35"/>
     </row>
-    <row r="39" spans="1:11" ht="15" x14ac:dyDescent="0.3">
-      <c r="A39" s="102"/>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="98"/>
       <c r="B39" s="46" t="s">
         <v>38</v>
       </c>
       <c r="C39" s="47" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D39" s="48">
         <v>2</v>
@@ -4049,8 +4028,8 @@
       <c r="J39" s="52"/>
       <c r="K39" s="53"/>
     </row>
-    <row r="40" spans="1:11" ht="15" x14ac:dyDescent="0.3">
-      <c r="A40" s="102"/>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="98"/>
       <c r="B40" s="44" t="s">
         <v>38</v>
       </c>
@@ -4068,13 +4047,13 @@
       <c r="J40" s="34"/>
       <c r="K40" s="35"/>
     </row>
-    <row r="41" spans="1:11" ht="15" x14ac:dyDescent="0.3">
-      <c r="A41" s="102"/>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="98"/>
       <c r="B41" s="46" t="s">
         <v>39</v>
       </c>
       <c r="C41" s="47" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D41" s="48">
         <v>2.5</v>
@@ -4089,8 +4068,8 @@
       <c r="J41" s="52"/>
       <c r="K41" s="53"/>
     </row>
-    <row r="42" spans="1:11" ht="15" x14ac:dyDescent="0.3">
-      <c r="A42" s="102"/>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="98"/>
       <c r="B42" s="46" t="s">
         <v>40</v>
       </c>
@@ -4108,8 +4087,8 @@
       <c r="J42" s="52"/>
       <c r="K42" s="53"/>
     </row>
-    <row r="43" spans="1:11" ht="15" x14ac:dyDescent="0.3">
-      <c r="A43" s="102"/>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="98"/>
       <c r="B43" s="44" t="s">
         <v>40</v>
       </c>
@@ -4127,8 +4106,8 @@
       <c r="J43" s="34"/>
       <c r="K43" s="35"/>
     </row>
-    <row r="44" spans="1:11" ht="15" x14ac:dyDescent="0.3">
-      <c r="A44" s="102"/>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="98"/>
       <c r="B44" s="46" t="s">
         <v>40</v>
       </c>
@@ -4146,8 +4125,8 @@
       <c r="J44" s="52"/>
       <c r="K44" s="53"/>
     </row>
-    <row r="45" spans="1:11" ht="15" x14ac:dyDescent="0.3">
-      <c r="A45" s="102"/>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="98"/>
       <c r="B45" s="44" t="s">
         <v>40</v>
       </c>
@@ -4165,13 +4144,13 @@
       <c r="J45" s="34"/>
       <c r="K45" s="35"/>
     </row>
-    <row r="46" spans="1:11" ht="15" x14ac:dyDescent="0.3">
-      <c r="A46" s="102"/>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="98"/>
       <c r="B46" s="46" t="s">
         <v>40</v>
       </c>
       <c r="C46" s="47" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D46" s="48">
         <v>0.5</v>
@@ -4184,8 +4163,8 @@
       <c r="J46" s="52"/>
       <c r="K46" s="53"/>
     </row>
-    <row r="47" spans="1:11" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="103"/>
+    <row r="47" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="99"/>
       <c r="B47" s="54" t="s">
         <v>40</v>
       </c>
@@ -4203,9 +4182,9 @@
       <c r="J47" s="58"/>
       <c r="K47" s="59"/>
     </row>
-    <row r="48" spans="1:11" ht="15.6" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="102" t="s">
-        <v>57</v>
+    <row r="48" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="98" t="s">
+        <v>54</v>
       </c>
       <c r="B48" s="46" t="s">
         <v>41</v>
@@ -4224,8 +4203,8 @@
       <c r="J48" s="52"/>
       <c r="K48" s="53"/>
     </row>
-    <row r="49" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="102"/>
+    <row r="49" spans="1:20" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="98"/>
       <c r="B49" s="44" t="s">
         <v>42</v>
       </c>
@@ -4243,8 +4222,8 @@
       <c r="J49" s="34"/>
       <c r="K49" s="35"/>
     </row>
-    <row r="50" spans="1:11" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="103"/>
+    <row r="50" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="99"/>
       <c r="B50" s="60" t="s">
         <v>43</v>
       </c>
@@ -4262,9 +4241,9 @@
       <c r="J50" s="66"/>
       <c r="K50" s="67"/>
     </row>
-    <row r="51" spans="1:11" ht="15.6" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="102" t="s">
-        <v>58</v>
+    <row r="51" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="98" t="s">
+        <v>55</v>
       </c>
       <c r="B51" s="44" t="s">
         <v>44</v>
@@ -4285,8 +4264,8 @@
       <c r="J51" s="34"/>
       <c r="K51" s="35"/>
     </row>
-    <row r="52" spans="1:11" ht="15" x14ac:dyDescent="0.3">
-      <c r="A52" s="102"/>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A52" s="98"/>
       <c r="B52" s="46" t="s">
         <v>45</v>
       </c>
@@ -4304,8 +4283,8 @@
       <c r="J52" s="52"/>
       <c r="K52" s="53"/>
     </row>
-    <row r="53" spans="1:11" ht="15" x14ac:dyDescent="0.3">
-      <c r="A53" s="102"/>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A53" s="98"/>
       <c r="B53" s="44" t="s">
         <v>46</v>
       </c>
@@ -4323,10 +4302,10 @@
       <c r="J53" s="34"/>
       <c r="K53" s="35"/>
     </row>
-    <row r="54" spans="1:11" ht="15" x14ac:dyDescent="0.3">
-      <c r="A54" s="102"/>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A54" s="98"/>
       <c r="B54" s="46" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C54" s="47" t="s">
         <v>24</v>
@@ -4342,10 +4321,10 @@
       <c r="J54" s="52"/>
       <c r="K54" s="53"/>
     </row>
-    <row r="55" spans="1:11" ht="15" x14ac:dyDescent="0.3">
-      <c r="A55" s="102"/>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A55" s="98"/>
       <c r="B55" s="44" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C55" s="30" t="s">
         <v>22</v>
@@ -4361,31 +4340,31 @@
       <c r="J55" s="34"/>
       <c r="K55" s="35"/>
     </row>
-    <row r="56" spans="1:11" ht="15" x14ac:dyDescent="0.3">
-      <c r="A56" s="102"/>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A56" s="98"/>
       <c r="B56" s="44" t="s">
-        <v>62</v>
-      </c>
-      <c r="C56" s="144" t="s">
+        <v>57</v>
+      </c>
+      <c r="C56" s="91" t="s">
         <v>25</v>
       </c>
-      <c r="D56" s="145">
+      <c r="D56" s="92">
         <v>2</v>
       </c>
-      <c r="E56" s="146"/>
-      <c r="F56" s="147"/>
-      <c r="G56" s="148"/>
-      <c r="H56" s="148">
+      <c r="E56" s="93"/>
+      <c r="F56" s="94"/>
+      <c r="G56" s="95"/>
+      <c r="H56" s="95">
         <v>1</v>
       </c>
-      <c r="I56" s="149"/>
-      <c r="J56" s="149"/>
-      <c r="K56" s="150"/>
-    </row>
-    <row r="57" spans="1:11" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="103"/>
+      <c r="I56" s="96"/>
+      <c r="J56" s="96"/>
+      <c r="K56" s="97"/>
+    </row>
+    <row r="57" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="99"/>
       <c r="B57" s="60" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C57" s="61" t="s">
         <v>23</v>
@@ -4401,9 +4380,9 @@
       <c r="J57" s="66"/>
       <c r="K57" s="67"/>
     </row>
-    <row r="58" spans="1:11" ht="15.6" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="102" t="s">
-        <v>59</v>
+    <row r="58" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="98" t="s">
+        <v>56</v>
       </c>
       <c r="B58" s="44" t="s">
         <v>47</v>
@@ -4422,8 +4401,8 @@
       <c r="J58" s="34"/>
       <c r="K58" s="35"/>
     </row>
-    <row r="59" spans="1:11" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="103"/>
+    <row r="59" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="99"/>
       <c r="B59" s="60" t="s">
         <v>48</v>
       </c>
@@ -4441,505 +4420,176 @@
       <c r="J59" s="66"/>
       <c r="K59" s="67"/>
     </row>
-    <row r="60" spans="1:11" ht="15.6" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="102" t="s">
-        <v>60</v>
-      </c>
-      <c r="B60" s="44" t="s">
-        <v>49</v>
-      </c>
-      <c r="C60" s="30" t="s">
-        <v>3</v>
-      </c>
-      <c r="D60" s="31">
-        <v>0.5</v>
-      </c>
-      <c r="E60" s="45"/>
-      <c r="F60" s="32"/>
-      <c r="G60" s="33"/>
-      <c r="H60" s="33"/>
-      <c r="I60" s="34"/>
-      <c r="J60" s="34"/>
-      <c r="K60" s="35"/>
-    </row>
-    <row r="61" spans="1:11" ht="15" x14ac:dyDescent="0.3">
-      <c r="A61" s="102"/>
-      <c r="B61" s="46" t="s">
-        <v>49</v>
-      </c>
-      <c r="C61" s="47" t="s">
-        <v>25</v>
-      </c>
-      <c r="D61" s="48">
-        <v>0.5</v>
-      </c>
-      <c r="E61" s="49"/>
-      <c r="F61" s="50"/>
-      <c r="G61" s="51"/>
-      <c r="H61" s="51"/>
-      <c r="I61" s="52"/>
-      <c r="J61" s="52"/>
-      <c r="K61" s="53"/>
-    </row>
-    <row r="62" spans="1:11" ht="15" x14ac:dyDescent="0.3">
-      <c r="A62" s="102"/>
-      <c r="B62" s="44" t="s">
-        <v>50</v>
-      </c>
-      <c r="C62" s="30" t="s">
-        <v>3</v>
-      </c>
-      <c r="D62" s="31">
-        <v>0.5</v>
-      </c>
-      <c r="E62" s="45"/>
-      <c r="F62" s="32"/>
-      <c r="G62" s="33"/>
-      <c r="H62" s="33"/>
-      <c r="I62" s="34"/>
-      <c r="J62" s="34"/>
-      <c r="K62" s="35"/>
-    </row>
-    <row r="63" spans="1:11" ht="15" x14ac:dyDescent="0.3">
-      <c r="A63" s="102"/>
-      <c r="B63" s="46" t="s">
-        <v>50</v>
-      </c>
-      <c r="C63" s="47" t="s">
-        <v>22</v>
-      </c>
-      <c r="D63" s="48">
-        <v>0.5</v>
-      </c>
-      <c r="E63" s="49"/>
-      <c r="F63" s="50"/>
-      <c r="G63" s="51"/>
-      <c r="H63" s="51"/>
-      <c r="I63" s="52"/>
-      <c r="J63" s="52"/>
-      <c r="K63" s="53"/>
-    </row>
-    <row r="64" spans="1:11" ht="15" x14ac:dyDescent="0.3">
-      <c r="A64" s="102"/>
-      <c r="B64" s="44" t="s">
-        <v>50</v>
-      </c>
-      <c r="C64" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="D64" s="31">
-        <v>0.5</v>
-      </c>
-      <c r="E64" s="45"/>
-      <c r="F64" s="32"/>
-      <c r="G64" s="33"/>
-      <c r="H64" s="33"/>
-      <c r="I64" s="34"/>
-      <c r="J64" s="34"/>
-      <c r="K64" s="35"/>
-    </row>
-    <row r="65" spans="1:12" ht="15" x14ac:dyDescent="0.3">
-      <c r="A65" s="102"/>
-      <c r="B65" s="46" t="s">
-        <v>50</v>
-      </c>
-      <c r="C65" s="47" t="s">
-        <v>24</v>
-      </c>
-      <c r="D65" s="48">
-        <v>0.5</v>
-      </c>
-      <c r="E65" s="49"/>
-      <c r="F65" s="50"/>
-      <c r="G65" s="51"/>
-      <c r="H65" s="51"/>
-      <c r="I65" s="52"/>
-      <c r="J65" s="52"/>
-      <c r="K65" s="53"/>
-    </row>
-    <row r="66" spans="1:12" ht="15" x14ac:dyDescent="0.3">
-      <c r="A66" s="102"/>
-      <c r="B66" s="44" t="s">
-        <v>50</v>
-      </c>
-      <c r="C66" s="30" t="s">
-        <v>52</v>
-      </c>
-      <c r="D66" s="31">
-        <v>0.5</v>
-      </c>
-      <c r="E66" s="45"/>
-      <c r="F66" s="32"/>
-      <c r="G66" s="33"/>
-      <c r="H66" s="33"/>
-      <c r="I66" s="34"/>
-      <c r="J66" s="34"/>
-      <c r="K66" s="35"/>
-    </row>
-    <row r="67" spans="1:12" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="103"/>
-      <c r="B67" s="60" t="s">
-        <v>50</v>
-      </c>
-      <c r="C67" s="61" t="s">
-        <v>25</v>
-      </c>
-      <c r="D67" s="62">
-        <v>0.5</v>
-      </c>
-      <c r="E67" s="63"/>
-      <c r="F67" s="64"/>
-      <c r="G67" s="65"/>
-      <c r="H67" s="65"/>
-      <c r="I67" s="66"/>
-      <c r="J67" s="66"/>
-      <c r="K67" s="67"/>
-    </row>
-    <row r="68" spans="1:12" ht="15.6" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="102" t="s">
-        <v>61</v>
-      </c>
-      <c r="B68" s="44" t="s">
-        <v>51</v>
-      </c>
-      <c r="C68" s="30" t="s">
-        <v>25</v>
-      </c>
-      <c r="D68" s="31">
-        <v>2</v>
-      </c>
-      <c r="E68" s="45"/>
-      <c r="F68" s="32"/>
-      <c r="G68" s="33"/>
-      <c r="H68" s="33"/>
-      <c r="I68" s="34"/>
-      <c r="J68" s="34"/>
-      <c r="K68" s="35"/>
-    </row>
-    <row r="69" spans="1:12" ht="15" x14ac:dyDescent="0.3">
-      <c r="A69" s="102"/>
-      <c r="B69" s="46" t="s">
-        <v>51</v>
-      </c>
-      <c r="C69" s="47" t="s">
-        <v>3</v>
-      </c>
-      <c r="D69" s="48">
-        <v>2</v>
-      </c>
-      <c r="E69" s="49"/>
-      <c r="F69" s="50"/>
-      <c r="G69" s="51"/>
-      <c r="H69" s="51"/>
-      <c r="I69" s="52"/>
-      <c r="J69" s="52"/>
-      <c r="K69" s="53"/>
-    </row>
-    <row r="70" spans="1:12" ht="15" x14ac:dyDescent="0.3">
-      <c r="A70" s="102"/>
-      <c r="B70" s="44" t="s">
-        <v>51</v>
-      </c>
-      <c r="C70" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="D70" s="31">
-        <v>1</v>
-      </c>
-      <c r="E70" s="45"/>
-      <c r="F70" s="32"/>
-      <c r="G70" s="33"/>
-      <c r="H70" s="33"/>
-      <c r="I70" s="34"/>
-      <c r="J70" s="34"/>
-      <c r="K70" s="35"/>
-    </row>
-    <row r="71" spans="1:12" ht="15" x14ac:dyDescent="0.3">
-      <c r="A71" s="102"/>
-      <c r="B71" s="46" t="s">
-        <v>63</v>
-      </c>
-      <c r="C71" s="47" t="s">
-        <v>25</v>
-      </c>
-      <c r="D71" s="48">
-        <v>1</v>
-      </c>
-      <c r="E71" s="49"/>
-      <c r="F71" s="50"/>
-      <c r="G71" s="51"/>
-      <c r="H71" s="51"/>
-      <c r="I71" s="52"/>
-      <c r="J71" s="52"/>
-      <c r="K71" s="53"/>
-    </row>
-    <row r="72" spans="1:12" ht="15" x14ac:dyDescent="0.3">
-      <c r="A72" s="102"/>
-      <c r="B72" s="44" t="s">
-        <v>63</v>
-      </c>
-      <c r="C72" s="30" t="s">
-        <v>3</v>
-      </c>
-      <c r="D72" s="31">
-        <v>1</v>
-      </c>
-      <c r="E72" s="45"/>
-      <c r="F72" s="32"/>
-      <c r="G72" s="33"/>
-      <c r="H72" s="33"/>
-      <c r="I72" s="34"/>
-      <c r="J72" s="34"/>
-      <c r="K72" s="35"/>
-    </row>
-    <row r="73" spans="1:12" ht="15" x14ac:dyDescent="0.3">
-      <c r="A73" s="102"/>
-      <c r="B73" s="46" t="s">
-        <v>63</v>
-      </c>
-      <c r="C73" s="47" t="s">
-        <v>23</v>
-      </c>
-      <c r="D73" s="48">
-        <v>1</v>
-      </c>
-      <c r="E73" s="49"/>
-      <c r="F73" s="50"/>
-      <c r="G73" s="51"/>
-      <c r="H73" s="51"/>
-      <c r="I73" s="52"/>
-      <c r="J73" s="52"/>
-      <c r="K73" s="53"/>
-    </row>
-    <row r="74" spans="1:12" ht="15" x14ac:dyDescent="0.3">
-      <c r="A74" s="102"/>
-      <c r="B74" s="44" t="s">
-        <v>64</v>
-      </c>
-      <c r="C74" s="30" t="s">
-        <v>25</v>
-      </c>
-      <c r="D74" s="31">
-        <v>1</v>
-      </c>
-      <c r="E74" s="45"/>
-      <c r="F74" s="32"/>
-      <c r="G74" s="33"/>
-      <c r="H74" s="33"/>
-      <c r="I74" s="34"/>
-      <c r="J74" s="34"/>
-      <c r="K74" s="35"/>
-    </row>
-    <row r="75" spans="1:12" ht="15" x14ac:dyDescent="0.3">
-      <c r="A75" s="102"/>
-      <c r="B75" s="46" t="s">
-        <v>64</v>
-      </c>
-      <c r="C75" s="47" t="s">
-        <v>23</v>
-      </c>
-      <c r="D75" s="48">
-        <v>1</v>
-      </c>
-      <c r="E75" s="49"/>
-      <c r="F75" s="50"/>
-      <c r="G75" s="51"/>
-      <c r="H75" s="51"/>
-      <c r="I75" s="52"/>
-      <c r="J75" s="52"/>
-      <c r="K75" s="53"/>
-    </row>
-    <row r="76" spans="1:12" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A76" s="103"/>
-      <c r="B76" s="54" t="s">
-        <v>64</v>
-      </c>
-      <c r="C76" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="D76" s="15">
-        <v>1</v>
-      </c>
-      <c r="E76" s="55"/>
-      <c r="F76" s="56"/>
-      <c r="G76" s="57"/>
-      <c r="H76" s="57"/>
-      <c r="I76" s="58"/>
-      <c r="J76" s="58"/>
-      <c r="K76" s="59"/>
-    </row>
-    <row r="77" spans="1:12" ht="16.2" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D77" s="11">
-        <f>SUM(D9:D76)</f>
-        <v>162</v>
-      </c>
-      <c r="E77" s="12" t="str">
-        <f>E78&amp;+ "/" &amp;+ $D$77</f>
-        <v>0/162</v>
-      </c>
-      <c r="F77" s="12" t="str">
-        <f>F78&amp;+ "/" &amp;+ $D$77</f>
-        <v>6/162</v>
-      </c>
-      <c r="G77" s="12" t="str">
-        <f t="shared" ref="G77:K77" si="0">G78&amp;+ "/" &amp;+ $D$77</f>
-        <v>19/162</v>
-      </c>
-      <c r="H77" s="12" t="str">
+    <row r="60" spans="1:20" ht="16.149999999999999" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D60" s="11">
+        <f>SUM(D9:D59)</f>
+        <v>147</v>
+      </c>
+      <c r="E60" s="12" t="str">
+        <f>E61&amp;+ "/" &amp;+ $D$60</f>
+        <v>0/147</v>
+      </c>
+      <c r="F60" s="12" t="str">
+        <f>F61&amp;+ "/" &amp;+ $D$60</f>
+        <v>6/147</v>
+      </c>
+      <c r="G60" s="12" t="str">
+        <f t="shared" ref="G60:K60" si="0">G61&amp;+ "/" &amp;+ $D$60</f>
+        <v>19/147</v>
+      </c>
+      <c r="H60" s="12" t="str">
         <f t="shared" si="0"/>
-        <v>36/162</v>
-      </c>
-      <c r="I77" s="12" t="str">
+        <v>36/147</v>
+      </c>
+      <c r="I60" s="12" t="str">
         <f t="shared" si="0"/>
-        <v>36/162</v>
-      </c>
-      <c r="J77" s="12" t="str">
+        <v>36/147</v>
+      </c>
+      <c r="J60" s="12" t="str">
         <f t="shared" si="0"/>
-        <v>36/162</v>
-      </c>
-      <c r="K77" s="13" t="str">
+        <v>36/147</v>
+      </c>
+      <c r="K60" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>36/162</v>
-      </c>
-    </row>
-    <row r="78" spans="1:12" ht="15" hidden="1" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="D78" s="1">
-        <f>SUM(D9:D76)</f>
-        <v>162</v>
-      </c>
-      <c r="E78" s="1">
-        <f>SUM(E9:E76)</f>
+        <v>36/147</v>
+      </c>
+    </row>
+    <row r="61" spans="1:20" ht="15" hidden="1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="D61" s="1">
+        <f>SUM(D9:D59)</f>
+        <v>147</v>
+      </c>
+      <c r="E61" s="1">
+        <f>SUM(E9:E59)</f>
         <v>0</v>
       </c>
-      <c r="F78" s="1">
-        <f>SUM(F9:F76)</f>
+      <c r="F61" s="1">
+        <f>SUM(F9:F59)</f>
         <v>6</v>
       </c>
-      <c r="G78" s="1">
-        <f>SUM(G9:G76)+F78</f>
+      <c r="G61" s="1">
+        <f>SUM(G9:G59)+F61</f>
         <v>19</v>
       </c>
-      <c r="H78" s="1">
-        <f>SUM(H9:H76)+G78</f>
+      <c r="H61" s="1">
+        <f>SUM(H9:H59)+G61</f>
         <v>36</v>
       </c>
-      <c r="I78" s="1">
-        <f>SUM(I9:I76)+H78</f>
+      <c r="I61" s="1">
+        <f>SUM(I9:I59)+H61</f>
         <v>36</v>
       </c>
-      <c r="J78" s="1">
-        <f>SUM(J9:J76)+I78</f>
+      <c r="J61" s="1">
+        <f>SUM(J9:J59)+I61</f>
         <v>36</v>
       </c>
-      <c r="K78" s="1">
-        <f>SUM(K9:K76)+J78</f>
+      <c r="K61" s="1">
+        <f>SUM(K9:K59)+J61</f>
         <v>36</v>
       </c>
-      <c r="L78" s="1"/>
-    </row>
-    <row r="79" spans="1:12" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D79" s="1"/>
-      <c r="E79" s="1">
-        <f>D77</f>
-        <v>162</v>
-      </c>
-      <c r="F79" s="1">
-        <f>E79</f>
-        <v>162</v>
-      </c>
-      <c r="G79" s="1">
-        <f>F79</f>
-        <v>162</v>
-      </c>
-      <c r="H79" s="1">
-        <f t="shared" ref="H79:K79" si="1">G79</f>
-        <v>162</v>
-      </c>
-      <c r="I79" s="1">
+      <c r="L61" s="1"/>
+    </row>
+    <row r="62" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D62" s="1"/>
+      <c r="E62" s="1">
+        <f>D60</f>
+        <v>147</v>
+      </c>
+      <c r="F62" s="1">
+        <f>E62</f>
+        <v>147</v>
+      </c>
+      <c r="G62" s="1">
+        <f>F62</f>
+        <v>147</v>
+      </c>
+      <c r="H62" s="1">
+        <f t="shared" ref="H62:K62" si="1">G62</f>
+        <v>147</v>
+      </c>
+      <c r="I62" s="1">
         <f t="shared" si="1"/>
-        <v>162</v>
-      </c>
-      <c r="J79" s="1">
+        <v>147</v>
+      </c>
+      <c r="J62" s="1">
         <f t="shared" si="1"/>
-        <v>162</v>
-      </c>
-      <c r="K79" s="1">
+        <v>147</v>
+      </c>
+      <c r="K62" s="1">
         <f t="shared" si="1"/>
-        <v>162</v>
-      </c>
-      <c r="L79" s="1"/>
-    </row>
-    <row r="80" spans="1:12" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D80" s="1"/>
-      <c r="E80" s="1">
+        <v>147</v>
+      </c>
+      <c r="L62" s="1"/>
+    </row>
+    <row r="63" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D63" s="1"/>
+      <c r="E63" s="1">
         <v>0</v>
       </c>
-      <c r="K80" s="2">
-        <f>K79</f>
-        <v>162</v>
-      </c>
-    </row>
-    <row r="81" spans="4:20" hidden="1" x14ac:dyDescent="0.3">
-      <c r="D81" s="1"/>
-      <c r="E81" s="5" t="s">
+      <c r="K63" s="2">
+        <f>K62</f>
+        <v>147</v>
+      </c>
+    </row>
+    <row r="64" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D64" s="1"/>
+      <c r="E64" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F81" s="5" t="s">
+      <c r="F64" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G81" s="5" t="s">
+      <c r="G64" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H81" s="5"/>
-      <c r="I81" s="5"/>
-      <c r="J81" s="4"/>
-      <c r="K81" s="4"/>
-      <c r="L81" s="4"/>
-      <c r="M81" s="4"/>
-      <c r="N81" s="4"/>
-      <c r="O81" s="4"/>
-      <c r="P81" s="4"/>
-      <c r="Q81" s="4"/>
-      <c r="R81" s="4"/>
-      <c r="S81" s="4"/>
-      <c r="T81" s="4"/>
-    </row>
-    <row r="82" spans="4:20" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="D82" s="1"/>
-      <c r="E82" s="1"/>
-      <c r="F82" s="1"/>
-      <c r="G82" s="1"/>
-      <c r="H82" s="1"/>
-      <c r="I82" s="1"/>
-    </row>
-    <row r="100" spans="18:18" x14ac:dyDescent="0.3">
-      <c r="R100" s="2" t="s">
+      <c r="H64" s="5"/>
+      <c r="I64" s="5"/>
+      <c r="J64" s="4"/>
+      <c r="K64" s="4"/>
+      <c r="L64" s="4"/>
+      <c r="M64" s="4"/>
+      <c r="N64" s="4"/>
+      <c r="O64" s="4"/>
+      <c r="P64" s="4"/>
+      <c r="Q64" s="4"/>
+      <c r="R64" s="4"/>
+      <c r="S64" s="4"/>
+      <c r="T64" s="4"/>
+    </row>
+    <row r="65" spans="4:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="D65" s="1"/>
+      <c r="E65" s="1"/>
+      <c r="F65" s="1"/>
+      <c r="G65" s="1"/>
+      <c r="H65" s="1"/>
+      <c r="I65" s="1"/>
+    </row>
+    <row r="83" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R83" s="2" t="s">
         <v>30</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="A60:A67"/>
-    <mergeCell ref="A68:A76"/>
+  <mergeCells count="12">
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="F7:K7"/>
+    <mergeCell ref="B7:B8"/>
     <mergeCell ref="A9:A14"/>
     <mergeCell ref="A15:A28"/>
     <mergeCell ref="A29:A47"/>
     <mergeCell ref="A58:A59"/>
     <mergeCell ref="A51:A57"/>
     <mergeCell ref="A48:A50"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="F7:K7"/>
-    <mergeCell ref="B7:B8"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Number" error="Please Enter Only Numbers. You may use .5 increments. " sqref="D9:D76">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Number" error="Please Enter Only Numbers. You may use .5 increments. " sqref="D9:D59">
       <formula1>0</formula1>
       <formula2>100000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Numbers Only" error="Please Enter Only Numbers. You may use .5 increments. " sqref="F9:K76">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Numbers Only" error="Please Enter Only Numbers. You may use .5 increments. " sqref="F9:K59">
       <formula1>0</formula1>
       <formula2>10000</formula2>
     </dataValidation>
@@ -4953,7 +4603,7 @@
           <x14:formula1>
             <xm:f>'Names-Hours'!$B$3:$B$9</xm:f>
           </x14:formula1>
-          <xm:sqref>C9:C76</xm:sqref>
+          <xm:sqref>C9:C59</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4969,43 +4619,43 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="78" customWidth="1"/>
-    <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="23" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B1" s="23" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:4" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="69" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="82" t="s">
         <v>76</v>
       </c>
-      <c r="B3" s="82" t="s">
-        <v>83</v>
-      </c>
       <c r="C3" s="70" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="D3" s="70" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="83" t="s">
         <v>77</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="71" t="s">
-        <v>53</v>
-      </c>
-      <c r="B4" s="83" t="s">
-        <v>84</v>
       </c>
       <c r="C4" s="74">
         <v>13</v>
@@ -5014,12 +4664,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="72" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B5" s="83" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C5" s="76">
         <v>20</v>
@@ -5028,12 +4678,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="72" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B6" s="83" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C6" s="76">
         <v>5</v>
@@ -5042,12 +4692,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="72" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="B7" s="83" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C7" s="76">
         <v>5</v>
@@ -5056,12 +4706,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="72" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B8" s="83" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C8" s="76">
         <v>20</v>
@@ -5070,12 +4720,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="72" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B9" s="83" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C9" s="76">
         <v>13</v>
@@ -5084,12 +4734,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="72" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B10" s="83" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C10" s="76">
         <v>5</v>
@@ -5098,12 +4748,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="72" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B11" s="83" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C11" s="76">
         <v>20</v>
@@ -5112,12 +4762,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="72" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B12" s="83" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C12" s="76">
         <v>20</v>
@@ -5126,12 +4776,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="72" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="B13" s="83" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C13" s="76">
         <v>13</v>
@@ -5140,26 +4790,26 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="72" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B14" s="83" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C14" s="76" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D14" s="80" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="72" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B15" s="83" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C15" s="76">
         <v>13</v>
@@ -5168,12 +4818,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="73" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="B16" s="83" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C16" s="78">
         <v>5</v>
@@ -5195,568 +4845,557 @@
       <selection activeCell="H21" sqref="H21:I23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="20.6640625" customWidth="1"/>
-    <col min="3" max="3" width="8.6640625" customWidth="1"/>
-    <col min="5" max="6" width="20.6640625" customWidth="1"/>
-    <col min="7" max="7" width="8.6640625" customWidth="1"/>
-    <col min="8" max="9" width="20.6640625" customWidth="1"/>
-    <col min="10" max="10" width="8.6640625" customWidth="1"/>
-    <col min="11" max="12" width="20.6640625" customWidth="1"/>
-    <col min="13" max="13" width="8.6640625" customWidth="1"/>
+    <col min="1" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" customWidth="1"/>
+    <col min="5" max="6" width="20.7109375" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" customWidth="1"/>
+    <col min="8" max="9" width="20.7109375" customWidth="1"/>
+    <col min="10" max="10" width="8.7109375" customWidth="1"/>
+    <col min="11" max="12" width="20.7109375" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="29.4" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="105" t="s">
-        <v>65</v>
-      </c>
-      <c r="B1" s="106"/>
-      <c r="C1" s="107"/>
+    <row r="1" spans="1:13" ht="29.25" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="144" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="145"/>
+      <c r="C1" s="146"/>
       <c r="D1" s="81"/>
-      <c r="E1" s="105" t="s">
+      <c r="E1" s="144" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="106"/>
-      <c r="G1" s="106"/>
-      <c r="H1" s="106"/>
-      <c r="I1" s="106"/>
-      <c r="J1" s="106"/>
-      <c r="K1" s="106"/>
-      <c r="L1" s="106"/>
-      <c r="M1" s="107"/>
-    </row>
-    <row r="2" spans="1:13" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="108"/>
-      <c r="B2" s="109"/>
-      <c r="C2" s="110"/>
+      <c r="F1" s="145"/>
+      <c r="G1" s="145"/>
+      <c r="H1" s="145"/>
+      <c r="I1" s="145"/>
+      <c r="J1" s="145"/>
+      <c r="K1" s="145"/>
+      <c r="L1" s="145"/>
+      <c r="M1" s="146"/>
+    </row>
+    <row r="2" spans="1:13" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="147"/>
+      <c r="B2" s="148"/>
+      <c r="C2" s="149"/>
       <c r="D2" s="81"/>
-      <c r="E2" s="108" t="s">
-        <v>80</v>
-      </c>
-      <c r="F2" s="109"/>
-      <c r="G2" s="110"/>
-      <c r="H2" s="109" t="s">
-        <v>81</v>
-      </c>
-      <c r="I2" s="109"/>
-      <c r="J2" s="110"/>
-      <c r="K2" s="109" t="s">
-        <v>82</v>
-      </c>
-      <c r="L2" s="109"/>
-      <c r="M2" s="110"/>
-    </row>
-    <row r="3" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="111" t="str">
+      <c r="E2" s="147" t="s">
+        <v>73</v>
+      </c>
+      <c r="F2" s="148"/>
+      <c r="G2" s="149"/>
+      <c r="H2" s="148" t="s">
+        <v>74</v>
+      </c>
+      <c r="I2" s="148"/>
+      <c r="J2" s="149"/>
+      <c r="K2" s="148" t="s">
+        <v>75</v>
+      </c>
+      <c r="L2" s="148"/>
+      <c r="M2" s="149"/>
+    </row>
+    <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="136" t="str">
         <f>Backlog!A11</f>
         <v>As a User, I want to be able to detect Par. in Chemical Diagram, so I can work with polymers</v>
       </c>
-      <c r="B3" s="112"/>
+      <c r="B3" s="137"/>
       <c r="C3" s="87">
         <f>Backlog!C11</f>
         <v>20</v>
       </c>
-      <c r="E3" s="131"/>
-      <c r="F3" s="132"/>
+      <c r="E3" s="112"/>
+      <c r="F3" s="113"/>
       <c r="G3" s="86"/>
-      <c r="H3" s="125" t="str">
+      <c r="H3" s="118" t="str">
         <f>Backlog!A4</f>
         <v>As a Developer, I need an architectural overview of OSRA’s processing, so I can understand the code base.</v>
       </c>
-      <c r="I3" s="126"/>
+      <c r="I3" s="119"/>
       <c r="J3" s="87">
         <f>Backlog!C4</f>
         <v>13</v>
       </c>
-      <c r="K3" s="131"/>
-      <c r="L3" s="132"/>
+      <c r="K3" s="112"/>
+      <c r="L3" s="113"/>
       <c r="M3" s="86"/>
     </row>
-    <row r="4" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="113"/>
-      <c r="B4" s="114"/>
+    <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="138"/>
+      <c r="B4" s="139"/>
       <c r="C4" s="88" t="str">
         <f>Backlog!B11</f>
         <v>M</v>
       </c>
-      <c r="E4" s="133"/>
-      <c r="F4" s="134"/>
+      <c r="E4" s="114"/>
+      <c r="F4" s="115"/>
       <c r="G4" s="84"/>
-      <c r="H4" s="127"/>
-      <c r="I4" s="128"/>
+      <c r="H4" s="120"/>
+      <c r="I4" s="121"/>
       <c r="J4" s="88" t="str">
         <f>Backlog!B4</f>
         <v>M</v>
       </c>
-      <c r="K4" s="133"/>
-      <c r="L4" s="134"/>
+      <c r="K4" s="114"/>
+      <c r="L4" s="115"/>
       <c r="M4" s="84"/>
     </row>
-    <row r="5" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="115"/>
-      <c r="B5" s="116"/>
+    <row r="5" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="140"/>
+      <c r="B5" s="141"/>
       <c r="C5" s="89"/>
-      <c r="E5" s="135"/>
-      <c r="F5" s="136"/>
+      <c r="E5" s="116"/>
+      <c r="F5" s="117"/>
       <c r="G5" s="85"/>
-      <c r="H5" s="129"/>
-      <c r="I5" s="130"/>
+      <c r="H5" s="122"/>
+      <c r="I5" s="123"/>
       <c r="J5" s="89"/>
-      <c r="K5" s="135"/>
-      <c r="L5" s="136"/>
+      <c r="K5" s="116"/>
+      <c r="L5" s="117"/>
       <c r="M5" s="85"/>
     </row>
-    <row r="6" spans="1:13" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="111" t="str">
+    <row r="6" spans="1:13" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="136" t="str">
         <f>Backlog!A12</f>
         <v>As a User, I want to be able to detect Brackets in Chemical Diagrams, so I can work with polymers</v>
       </c>
-      <c r="B6" s="112"/>
+      <c r="B6" s="137"/>
       <c r="C6" s="87">
         <f>Backlog!C12</f>
         <v>20</v>
       </c>
-      <c r="E6" s="131"/>
-      <c r="F6" s="132"/>
+      <c r="E6" s="112"/>
+      <c r="F6" s="113"/>
       <c r="G6" s="86"/>
-      <c r="H6" s="125" t="str">
+      <c r="H6" s="118" t="str">
         <f>Backlog!A5</f>
         <v>As a Developer, I need to review each aspect of OSRA’s architecture, so I can understand the code base.</v>
       </c>
-      <c r="I6" s="126"/>
+      <c r="I6" s="119"/>
       <c r="J6" s="87">
         <f>Backlog!C5</f>
         <v>20</v>
       </c>
-      <c r="K6" s="131"/>
-      <c r="L6" s="132"/>
+      <c r="K6" s="112"/>
+      <c r="L6" s="113"/>
       <c r="M6" s="86"/>
     </row>
-    <row r="7" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="113"/>
-      <c r="B7" s="114"/>
+    <row r="7" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="138"/>
+      <c r="B7" s="139"/>
       <c r="C7" s="88" t="str">
         <f>Backlog!B12</f>
         <v>S</v>
       </c>
-      <c r="E7" s="133"/>
-      <c r="F7" s="134"/>
+      <c r="E7" s="114"/>
+      <c r="F7" s="115"/>
       <c r="G7" s="84"/>
-      <c r="H7" s="127"/>
-      <c r="I7" s="128"/>
+      <c r="H7" s="120"/>
+      <c r="I7" s="121"/>
       <c r="J7" s="88" t="str">
         <f>Backlog!B5</f>
         <v>M</v>
       </c>
-      <c r="K7" s="133"/>
-      <c r="L7" s="134"/>
+      <c r="K7" s="114"/>
+      <c r="L7" s="115"/>
       <c r="M7" s="84"/>
     </row>
-    <row r="8" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="115"/>
-      <c r="B8" s="116"/>
+    <row r="8" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="140"/>
+      <c r="B8" s="141"/>
       <c r="C8" s="89"/>
-      <c r="E8" s="135"/>
-      <c r="F8" s="136"/>
+      <c r="E8" s="116"/>
+      <c r="F8" s="117"/>
       <c r="G8" s="85"/>
-      <c r="H8" s="129"/>
-      <c r="I8" s="130"/>
+      <c r="H8" s="122"/>
+      <c r="I8" s="123"/>
       <c r="J8" s="89"/>
-      <c r="K8" s="135"/>
-      <c r="L8" s="136"/>
+      <c r="K8" s="116"/>
+      <c r="L8" s="117"/>
       <c r="M8" s="85"/>
     </row>
-    <row r="9" spans="1:13" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="111" t="str">
+    <row r="9" spans="1:13" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="136" t="str">
         <f>Backlog!A13</f>
         <v>As a User, I want to be able to detect subscripts for polymer diagrams, so I can work with polymers</v>
       </c>
-      <c r="B9" s="112"/>
+      <c r="B9" s="137"/>
       <c r="C9" s="87">
         <f>Backlog!C13</f>
         <v>13</v>
       </c>
-      <c r="E9" s="131"/>
-      <c r="F9" s="132"/>
+      <c r="E9" s="112"/>
+      <c r="F9" s="113"/>
       <c r="G9" s="86"/>
-      <c r="H9" s="125" t="str">
+      <c r="H9" s="118" t="str">
         <f>Backlog!A6</f>
         <v>As a Developer, I need to get a basic grasp of O-Chem, so I can better understand use cases.</v>
       </c>
-      <c r="I9" s="126"/>
+      <c r="I9" s="119"/>
       <c r="J9" s="87">
         <f>Backlog!C6</f>
         <v>5</v>
       </c>
-      <c r="K9" s="131"/>
-      <c r="L9" s="132"/>
+      <c r="K9" s="112"/>
+      <c r="L9" s="113"/>
       <c r="M9" s="86"/>
     </row>
-    <row r="10" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="113"/>
-      <c r="B10" s="114"/>
+    <row r="10" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="138"/>
+      <c r="B10" s="139"/>
       <c r="C10" s="88" t="str">
         <f>Backlog!B13</f>
         <v>M</v>
       </c>
-      <c r="E10" s="133"/>
-      <c r="F10" s="134"/>
+      <c r="E10" s="114"/>
+      <c r="F10" s="115"/>
       <c r="G10" s="84"/>
-      <c r="H10" s="127"/>
-      <c r="I10" s="128"/>
+      <c r="H10" s="120"/>
+      <c r="I10" s="121"/>
       <c r="J10" s="88" t="str">
         <f>Backlog!B6</f>
         <v>M</v>
       </c>
-      <c r="K10" s="133"/>
-      <c r="L10" s="134"/>
+      <c r="K10" s="114"/>
+      <c r="L10" s="115"/>
       <c r="M10" s="84"/>
     </row>
-    <row r="11" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="115"/>
-      <c r="B11" s="116"/>
+    <row r="11" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="140"/>
+      <c r="B11" s="141"/>
       <c r="C11" s="89"/>
-      <c r="E11" s="135"/>
-      <c r="F11" s="136"/>
+      <c r="E11" s="116"/>
+      <c r="F11" s="117"/>
       <c r="G11" s="85"/>
-      <c r="H11" s="129"/>
-      <c r="I11" s="130"/>
+      <c r="H11" s="122"/>
+      <c r="I11" s="123"/>
       <c r="J11" s="89"/>
-      <c r="K11" s="135"/>
-      <c r="L11" s="136"/>
+      <c r="K11" s="116"/>
+      <c r="L11" s="117"/>
       <c r="M11" s="85"/>
     </row>
-    <row r="12" spans="1:13" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="111" t="str">
+    <row r="12" spans="1:13" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="136" t="str">
         <f>Backlog!A14</f>
         <v>As a User, I want to be able to detect “R-Notation”, so I can work with polymers</v>
       </c>
-      <c r="B12" s="112"/>
+      <c r="B12" s="137"/>
       <c r="C12" s="87" t="str">
         <f>Backlog!C14</f>
         <v>INF</v>
       </c>
-      <c r="E12" s="125" t="str">
+      <c r="E12" s="118" t="str">
         <f>Backlog!A7</f>
         <v>As a Developer, I need workflow and processes for the github repo, so I can collaborate on code</v>
       </c>
-      <c r="F12" s="126"/>
+      <c r="F12" s="119"/>
       <c r="G12" s="87">
         <f>Backlog!C7</f>
         <v>5</v>
       </c>
-      <c r="H12" s="131"/>
-      <c r="I12" s="132"/>
+      <c r="H12" s="112"/>
+      <c r="I12" s="113"/>
       <c r="J12" s="86"/>
-      <c r="K12" s="131"/>
-      <c r="L12" s="132"/>
+      <c r="K12" s="112"/>
+      <c r="L12" s="113"/>
       <c r="M12" s="86"/>
     </row>
-    <row r="13" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="113"/>
-      <c r="B13" s="114"/>
+    <row r="13" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="138"/>
+      <c r="B13" s="139"/>
       <c r="C13" s="88" t="str">
         <f>Backlog!B14</f>
         <v>W</v>
       </c>
-      <c r="E13" s="127"/>
-      <c r="F13" s="128"/>
+      <c r="E13" s="120"/>
+      <c r="F13" s="121"/>
       <c r="G13" s="88" t="str">
         <f>Backlog!B7</f>
         <v>M</v>
       </c>
-      <c r="H13" s="133"/>
-      <c r="I13" s="134"/>
+      <c r="H13" s="114"/>
+      <c r="I13" s="115"/>
       <c r="J13" s="84"/>
-      <c r="K13" s="133"/>
-      <c r="L13" s="134"/>
+      <c r="K13" s="114"/>
+      <c r="L13" s="115"/>
       <c r="M13" s="84"/>
     </row>
-    <row r="14" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="117"/>
-      <c r="B14" s="118"/>
+    <row r="14" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="142"/>
+      <c r="B14" s="143"/>
       <c r="C14" s="90"/>
-      <c r="E14" s="129"/>
-      <c r="F14" s="130"/>
+      <c r="E14" s="122"/>
+      <c r="F14" s="123"/>
       <c r="G14" s="89"/>
-      <c r="H14" s="135"/>
-      <c r="I14" s="136"/>
+      <c r="H14" s="116"/>
+      <c r="I14" s="117"/>
       <c r="J14" s="85"/>
-      <c r="K14" s="135"/>
-      <c r="L14" s="136"/>
+      <c r="K14" s="116"/>
+      <c r="L14" s="117"/>
       <c r="M14" s="85"/>
     </row>
-    <row r="15" spans="1:13" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="119"/>
-      <c r="B15" s="120"/>
+    <row r="15" spans="1:13" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="130"/>
+      <c r="B15" s="131"/>
       <c r="C15" s="87"/>
-      <c r="E15" s="125" t="str">
+      <c r="E15" s="118" t="str">
         <f>Backlog!A8</f>
         <v>As a Developer, I need a testing enviroment and test documentation, so I can better contribute to the codebase</v>
       </c>
-      <c r="F15" s="126"/>
+      <c r="F15" s="119"/>
       <c r="G15" s="87">
         <f>Backlog!C8</f>
         <v>20</v>
       </c>
-      <c r="H15" s="131"/>
-      <c r="I15" s="132"/>
+      <c r="H15" s="112"/>
+      <c r="I15" s="113"/>
       <c r="J15" s="86"/>
-      <c r="K15" s="131"/>
-      <c r="L15" s="132"/>
+      <c r="K15" s="112"/>
+      <c r="L15" s="113"/>
       <c r="M15" s="86"/>
     </row>
-    <row r="16" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="121"/>
-      <c r="B16" s="122"/>
+    <row r="16" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="132"/>
+      <c r="B16" s="133"/>
       <c r="C16" s="88"/>
-      <c r="E16" s="127"/>
-      <c r="F16" s="128"/>
+      <c r="E16" s="120"/>
+      <c r="F16" s="121"/>
       <c r="G16" s="88" t="str">
         <f>Backlog!B8</f>
         <v>M</v>
       </c>
-      <c r="H16" s="133"/>
-      <c r="I16" s="134"/>
+      <c r="H16" s="114"/>
+      <c r="I16" s="115"/>
       <c r="J16" s="84"/>
-      <c r="K16" s="133"/>
-      <c r="L16" s="134"/>
+      <c r="K16" s="114"/>
+      <c r="L16" s="115"/>
       <c r="M16" s="84"/>
     </row>
-    <row r="17" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="123"/>
-      <c r="B17" s="124"/>
+    <row r="17" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="134"/>
+      <c r="B17" s="135"/>
       <c r="C17" s="89"/>
-      <c r="E17" s="129"/>
-      <c r="F17" s="130"/>
+      <c r="E17" s="122"/>
+      <c r="F17" s="123"/>
       <c r="G17" s="89"/>
-      <c r="H17" s="135"/>
-      <c r="I17" s="136"/>
+      <c r="H17" s="116"/>
+      <c r="I17" s="117"/>
       <c r="J17" s="85"/>
-      <c r="K17" s="135"/>
-      <c r="L17" s="136"/>
+      <c r="K17" s="116"/>
+      <c r="L17" s="117"/>
       <c r="M17" s="85"/>
     </row>
-    <row r="18" spans="1:13" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="119"/>
-      <c r="B18" s="120"/>
+    <row r="18" spans="1:13" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="130"/>
+      <c r="B18" s="131"/>
       <c r="C18" s="87"/>
-      <c r="E18" s="125" t="str">
+      <c r="E18" s="118" t="str">
         <f>Backlog!A9</f>
         <v>As a Developer, I need to have consolidated documentation from other developers, so I can better contribute to the codebase</v>
       </c>
-      <c r="F18" s="126"/>
+      <c r="F18" s="119"/>
       <c r="G18" s="87">
         <f>Backlog!C9</f>
         <v>13</v>
       </c>
-      <c r="H18" s="131"/>
-      <c r="I18" s="132"/>
+      <c r="H18" s="112"/>
+      <c r="I18" s="113"/>
       <c r="J18" s="86"/>
-      <c r="K18" s="131"/>
-      <c r="L18" s="132"/>
+      <c r="K18" s="112"/>
+      <c r="L18" s="113"/>
       <c r="M18" s="86"/>
     </row>
-    <row r="19" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="121"/>
-      <c r="B19" s="122"/>
+    <row r="19" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="132"/>
+      <c r="B19" s="133"/>
       <c r="C19" s="88"/>
-      <c r="E19" s="127"/>
-      <c r="F19" s="128"/>
+      <c r="E19" s="120"/>
+      <c r="F19" s="121"/>
       <c r="G19" s="88" t="str">
         <f>Backlog!B9</f>
         <v>M</v>
       </c>
-      <c r="H19" s="133"/>
-      <c r="I19" s="134"/>
+      <c r="H19" s="114"/>
+      <c r="I19" s="115"/>
       <c r="J19" s="84"/>
-      <c r="K19" s="133"/>
-      <c r="L19" s="134"/>
+      <c r="K19" s="114"/>
+      <c r="L19" s="115"/>
       <c r="M19" s="84"/>
     </row>
-    <row r="20" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="123"/>
-      <c r="B20" s="124"/>
+    <row r="20" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="134"/>
+      <c r="B20" s="135"/>
       <c r="C20" s="89"/>
-      <c r="E20" s="129"/>
-      <c r="F20" s="130"/>
+      <c r="E20" s="122"/>
+      <c r="F20" s="123"/>
       <c r="G20" s="89"/>
-      <c r="H20" s="135"/>
-      <c r="I20" s="136"/>
+      <c r="H20" s="116"/>
+      <c r="I20" s="117"/>
       <c r="J20" s="85"/>
-      <c r="K20" s="135"/>
-      <c r="L20" s="136"/>
+      <c r="K20" s="116"/>
+      <c r="L20" s="117"/>
       <c r="M20" s="85"/>
     </row>
-    <row r="21" spans="1:13" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="119"/>
-      <c r="B21" s="120"/>
+    <row r="21" spans="1:13" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="130"/>
+      <c r="B21" s="131"/>
       <c r="C21" s="87"/>
-      <c r="E21" s="125" t="str">
+      <c r="E21" s="118" t="str">
         <f>Backlog!A10</f>
         <v>As a Developer, I need to understand SMILES notation and .SD file structure, so I can desing the smile data structure.</v>
       </c>
-      <c r="F21" s="126"/>
+      <c r="F21" s="119"/>
       <c r="G21" s="87">
         <f>Backlog!C10</f>
         <v>5</v>
       </c>
-      <c r="H21" s="131"/>
-      <c r="I21" s="132"/>
+      <c r="H21" s="112"/>
+      <c r="I21" s="113"/>
       <c r="J21" s="86"/>
-      <c r="K21" s="131"/>
-      <c r="L21" s="132"/>
+      <c r="K21" s="112"/>
+      <c r="L21" s="113"/>
       <c r="M21" s="86"/>
     </row>
-    <row r="22" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="121"/>
-      <c r="B22" s="122"/>
+    <row r="22" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="132"/>
+      <c r="B22" s="133"/>
       <c r="C22" s="88"/>
-      <c r="E22" s="127"/>
-      <c r="F22" s="128"/>
+      <c r="E22" s="120"/>
+      <c r="F22" s="121"/>
       <c r="G22" s="88" t="str">
         <f>Backlog!B10</f>
         <v>M</v>
       </c>
-      <c r="H22" s="133"/>
-      <c r="I22" s="134"/>
+      <c r="H22" s="114"/>
+      <c r="I22" s="115"/>
       <c r="J22" s="84"/>
-      <c r="K22" s="133"/>
-      <c r="L22" s="134"/>
+      <c r="K22" s="114"/>
+      <c r="L22" s="115"/>
       <c r="M22" s="84"/>
     </row>
-    <row r="23" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="123"/>
-      <c r="B23" s="124"/>
+    <row r="23" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="134"/>
+      <c r="B23" s="135"/>
       <c r="C23" s="89"/>
-      <c r="E23" s="129"/>
-      <c r="F23" s="130"/>
+      <c r="E23" s="122"/>
+      <c r="F23" s="123"/>
       <c r="G23" s="89"/>
-      <c r="H23" s="135"/>
-      <c r="I23" s="136"/>
+      <c r="H23" s="116"/>
+      <c r="I23" s="117"/>
       <c r="J23" s="85"/>
-      <c r="K23" s="135"/>
-      <c r="L23" s="136"/>
+      <c r="K23" s="116"/>
+      <c r="L23" s="117"/>
       <c r="M23" s="85"/>
     </row>
-    <row r="24" spans="1:13" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="119"/>
-      <c r="B24" s="120"/>
+    <row r="24" spans="1:13" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="130"/>
+      <c r="B24" s="131"/>
       <c r="C24" s="87"/>
-      <c r="E24" s="125" t="str">
+      <c r="E24" s="118" t="str">
         <f>Backlog!A15</f>
         <v>As a User, I want to have a data structure for encoding polymers in “Smile Notation”, so I can work with polymers</v>
       </c>
-      <c r="F24" s="126"/>
+      <c r="F24" s="119"/>
       <c r="G24" s="87">
         <f>Backlog!C15</f>
         <v>13</v>
       </c>
-      <c r="H24" s="131"/>
-      <c r="I24" s="132"/>
+      <c r="H24" s="112"/>
+      <c r="I24" s="113"/>
       <c r="J24" s="86"/>
-      <c r="K24" s="131"/>
-      <c r="L24" s="132"/>
+      <c r="K24" s="112"/>
+      <c r="L24" s="113"/>
       <c r="M24" s="86"/>
     </row>
-    <row r="25" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="121"/>
-      <c r="B25" s="122"/>
+    <row r="25" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="132"/>
+      <c r="B25" s="133"/>
       <c r="C25" s="88"/>
-      <c r="E25" s="127"/>
-      <c r="F25" s="128"/>
+      <c r="E25" s="120"/>
+      <c r="F25" s="121"/>
       <c r="G25" s="88" t="str">
         <f>Backlog!B15</f>
         <v>M</v>
       </c>
-      <c r="H25" s="133"/>
-      <c r="I25" s="134"/>
+      <c r="H25" s="114"/>
+      <c r="I25" s="115"/>
       <c r="J25" s="84"/>
-      <c r="K25" s="133"/>
-      <c r="L25" s="134"/>
+      <c r="K25" s="114"/>
+      <c r="L25" s="115"/>
       <c r="M25" s="84"/>
     </row>
-    <row r="26" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="123"/>
-      <c r="B26" s="124"/>
+    <row r="26" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="134"/>
+      <c r="B26" s="135"/>
       <c r="C26" s="89"/>
-      <c r="E26" s="129"/>
-      <c r="F26" s="130"/>
+      <c r="E26" s="122"/>
+      <c r="F26" s="123"/>
       <c r="G26" s="89"/>
-      <c r="H26" s="135"/>
-      <c r="I26" s="136"/>
+      <c r="H26" s="116"/>
+      <c r="I26" s="117"/>
       <c r="J26" s="85"/>
-      <c r="K26" s="135"/>
-      <c r="L26" s="136"/>
+      <c r="K26" s="116"/>
+      <c r="L26" s="117"/>
       <c r="M26" s="85"/>
     </row>
-    <row r="27" spans="1:13" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="119"/>
-      <c r="B27" s="120"/>
+    <row r="27" spans="1:13" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="130"/>
+      <c r="B27" s="131"/>
       <c r="C27" s="87"/>
-      <c r="E27" s="137"/>
-      <c r="F27" s="138"/>
+      <c r="E27" s="124"/>
+      <c r="F27" s="125"/>
       <c r="G27" s="87"/>
-      <c r="H27" s="131"/>
-      <c r="I27" s="132"/>
+      <c r="H27" s="112"/>
+      <c r="I27" s="113"/>
       <c r="J27" s="86"/>
-      <c r="K27" s="131"/>
-      <c r="L27" s="132"/>
+      <c r="K27" s="112"/>
+      <c r="L27" s="113"/>
       <c r="M27" s="86"/>
     </row>
-    <row r="28" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="121"/>
-      <c r="B28" s="122"/>
+    <row r="28" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="132"/>
+      <c r="B28" s="133"/>
       <c r="C28" s="88"/>
-      <c r="E28" s="139"/>
-      <c r="F28" s="140"/>
+      <c r="E28" s="126"/>
+      <c r="F28" s="127"/>
       <c r="G28" s="88"/>
-      <c r="H28" s="133"/>
-      <c r="I28" s="134"/>
+      <c r="H28" s="114"/>
+      <c r="I28" s="115"/>
       <c r="J28" s="84"/>
-      <c r="K28" s="133"/>
-      <c r="L28" s="134"/>
+      <c r="K28" s="114"/>
+      <c r="L28" s="115"/>
       <c r="M28" s="84"/>
     </row>
-    <row r="29" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="123"/>
-      <c r="B29" s="124"/>
+    <row r="29" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="134"/>
+      <c r="B29" s="135"/>
       <c r="C29" s="89"/>
-      <c r="E29" s="141"/>
-      <c r="F29" s="142"/>
+      <c r="E29" s="128"/>
+      <c r="F29" s="129"/>
       <c r="G29" s="89"/>
-      <c r="H29" s="135"/>
-      <c r="I29" s="136"/>
+      <c r="H29" s="116"/>
+      <c r="I29" s="117"/>
       <c r="J29" s="85"/>
-      <c r="K29" s="135"/>
-      <c r="L29" s="136"/>
+      <c r="K29" s="116"/>
+      <c r="L29" s="117"/>
       <c r="M29" s="85"/>
     </row>
-    <row r="30" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="K18:L20"/>
-    <mergeCell ref="K21:L23"/>
-    <mergeCell ref="K24:L26"/>
-    <mergeCell ref="K27:L29"/>
-    <mergeCell ref="H21:I23"/>
-    <mergeCell ref="H24:I26"/>
-    <mergeCell ref="H27:I29"/>
-    <mergeCell ref="H18:I20"/>
-    <mergeCell ref="K3:L5"/>
-    <mergeCell ref="K6:L8"/>
-    <mergeCell ref="K9:L11"/>
-    <mergeCell ref="K12:L14"/>
-    <mergeCell ref="K15:L17"/>
-    <mergeCell ref="E18:F20"/>
-    <mergeCell ref="E21:F23"/>
-    <mergeCell ref="E24:F26"/>
-    <mergeCell ref="E27:F29"/>
-    <mergeCell ref="A21:B23"/>
-    <mergeCell ref="A24:B26"/>
-    <mergeCell ref="A27:B29"/>
-    <mergeCell ref="A18:B20"/>
+    <mergeCell ref="E1:M1"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="A1:C2"/>
+    <mergeCell ref="A3:B5"/>
+    <mergeCell ref="A6:B8"/>
+    <mergeCell ref="A9:B11"/>
+    <mergeCell ref="A12:B14"/>
+    <mergeCell ref="A15:B17"/>
     <mergeCell ref="H3:I5"/>
     <mergeCell ref="H6:I8"/>
     <mergeCell ref="H9:I11"/>
@@ -5767,16 +5406,27 @@
     <mergeCell ref="E9:F11"/>
     <mergeCell ref="H12:I14"/>
     <mergeCell ref="H15:I17"/>
-    <mergeCell ref="A3:B5"/>
-    <mergeCell ref="A6:B8"/>
-    <mergeCell ref="A9:B11"/>
-    <mergeCell ref="A12:B14"/>
-    <mergeCell ref="A15:B17"/>
-    <mergeCell ref="E1:M1"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="K2:M2"/>
-    <mergeCell ref="A1:C2"/>
+    <mergeCell ref="E18:F20"/>
+    <mergeCell ref="E21:F23"/>
+    <mergeCell ref="E24:F26"/>
+    <mergeCell ref="E27:F29"/>
+    <mergeCell ref="A21:B23"/>
+    <mergeCell ref="A24:B26"/>
+    <mergeCell ref="A27:B29"/>
+    <mergeCell ref="A18:B20"/>
+    <mergeCell ref="K3:L5"/>
+    <mergeCell ref="K6:L8"/>
+    <mergeCell ref="K9:L11"/>
+    <mergeCell ref="K12:L14"/>
+    <mergeCell ref="K15:L17"/>
+    <mergeCell ref="K18:L20"/>
+    <mergeCell ref="K21:L23"/>
+    <mergeCell ref="K24:L26"/>
+    <mergeCell ref="K27:L29"/>
+    <mergeCell ref="H21:I23"/>
+    <mergeCell ref="H24:I26"/>
+    <mergeCell ref="H27:I29"/>
+    <mergeCell ref="H18:I20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5790,20 +5440,20 @@
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="2"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
     <col min="2" max="2" width="11" style="2" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26" style="2" customWidth="1"/>
-    <col min="6" max="6" width="20.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.6640625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="31.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.109375" style="2"/>
+    <col min="6" max="6" width="20.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.7109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="31.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
         <v>11</v>
@@ -5824,7 +5474,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>22</v>
       </c>
@@ -5849,7 +5499,7 @@
         <v>24.5</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
@@ -5874,7 +5524,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>23</v>
       </c>
@@ -5899,7 +5549,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>24</v>
       </c>
@@ -5924,9 +5574,9 @@
         <v>24.5</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C7" s="2">
         <v>15</v>
@@ -5949,7 +5599,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>25</v>
       </c>
@@ -5974,9 +5624,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C9" s="2">
         <v>8</v>
@@ -6012,27 +5662,27 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="143">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="150">
         <v>41557</v>
       </c>
       <c r="B2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="143"/>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="150"/>
       <c r="B3" t="s">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
Sprint1 Wrap up and sprint 2 start
</commit_message>
<xml_diff>
--- a/bookkeeping/Sprint1 BurnUp.xlsx
+++ b/bookkeeping/Sprint1 BurnUp.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\konst_000\Documents\GitHub\UCSC-IBM-POSRA\bookkeeping\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="0" windowWidth="7470" windowHeight="3750" tabRatio="601" activeTab="3"/>
+    <workbookView xWindow="3060" yWindow="0" windowWidth="7476" windowHeight="3756" tabRatio="601"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks List" sheetId="1" r:id="rId1"/>
@@ -1552,15 +1552,6 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1597,6 +1588,57 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1668,48 +1710,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1915,13 +1915,13 @@
                   <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>36</c:v>
+                  <c:v>39.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>36</c:v>
+                  <c:v>53.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>36</c:v>
+                  <c:v>83.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2143,11 +2143,11 @@
         </c:dropLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="301280016"/>
-        <c:axId val="301281584"/>
+        <c:axId val="284815760"/>
+        <c:axId val="284816152"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="301280016"/>
+        <c:axId val="284815760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2190,14 +2190,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="301281584"/>
+        <c:crossAx val="284816152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="301281584"/>
+        <c:axId val="284816152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2234,7 +2234,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="301280016"/>
+        <c:crossAx val="284815760"/>
         <c:crossesAt val="41548"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="10"/>
@@ -2915,10 +2915,10 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </chartsheet>
 </file>
@@ -3215,22 +3215,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T83"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B83" sqref="B83"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="40.85546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="76.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" style="2" hidden="1" customWidth="1"/>
-    <col min="6" max="11" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="40.88671875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="76.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" style="2" hidden="1" customWidth="1"/>
+    <col min="6" max="11" width="11.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
@@ -3241,18 +3241,18 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="21"/>
       <c r="B2" s="22"/>
       <c r="D2" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="101" t="s">
+      <c r="F2" s="98" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="102"/>
-    </row>
-    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G2" s="99"/>
+    </row>
+    <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="18" t="s">
         <v>26</v>
       </c>
@@ -3281,7 +3281,7 @@
         <v>3.5/30</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="19" t="s">
         <v>27</v>
       </c>
@@ -3311,7 +3311,7 @@
         <v>3/30</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="9"/>
       <c r="D5" s="25" t="s">
         <v>21</v>
@@ -3323,36 +3323,36 @@
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
     </row>
-    <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:12" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="107" t="s">
+    <row r="6" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="1:12" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="104" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="107" t="s">
+      <c r="B7" s="104" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="103" t="s">
+      <c r="C7" s="100" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="105" t="s">
+      <c r="D7" s="102" t="s">
         <v>9</v>
       </c>
       <c r="E7" s="27"/>
-      <c r="F7" s="109" t="s">
+      <c r="F7" s="106" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="110"/>
-      <c r="H7" s="110"/>
-      <c r="I7" s="110"/>
-      <c r="J7" s="110"/>
-      <c r="K7" s="111"/>
+      <c r="G7" s="107"/>
+      <c r="H7" s="107"/>
+      <c r="I7" s="107"/>
+      <c r="J7" s="107"/>
+      <c r="K7" s="108"/>
       <c r="L7" s="16"/>
     </row>
-    <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="108"/>
-      <c r="B8" s="108"/>
-      <c r="C8" s="104"/>
-      <c r="D8" s="106"/>
+    <row r="8" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="105"/>
+      <c r="B8" s="105"/>
+      <c r="C8" s="101"/>
+      <c r="D8" s="103"/>
       <c r="E8" s="10">
         <v>41661</v>
       </c>
@@ -3375,8 +3375,8 @@
         <v>41675</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="16.149999999999999" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="100" t="s">
+    <row r="9" spans="1:12" ht="16.2" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="109" t="s">
         <v>50</v>
       </c>
       <c r="B9" s="36" t="s">
@@ -3398,10 +3398,12 @@
       <c r="H9" s="41"/>
       <c r="I9" s="42"/>
       <c r="J9" s="42"/>
-      <c r="K9" s="43"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="98"/>
+      <c r="K9" s="43">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15" x14ac:dyDescent="0.3">
+      <c r="A10" s="110"/>
       <c r="B10" s="44" t="s">
         <v>32</v>
       </c>
@@ -3421,8 +3423,8 @@
       <c r="J10" s="34"/>
       <c r="K10" s="35"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="98"/>
+    <row r="11" spans="1:12" ht="15" x14ac:dyDescent="0.3">
+      <c r="A11" s="110"/>
       <c r="B11" s="46" t="s">
         <v>33</v>
       </c>
@@ -3442,8 +3444,8 @@
       <c r="J11" s="52"/>
       <c r="K11" s="53"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="98"/>
+    <row r="12" spans="1:12" ht="15" x14ac:dyDescent="0.3">
+      <c r="A12" s="110"/>
       <c r="B12" s="44" t="s">
         <v>33</v>
       </c>
@@ -3463,8 +3465,8 @@
       <c r="J12" s="34"/>
       <c r="K12" s="35"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="98"/>
+    <row r="13" spans="1:12" ht="15" x14ac:dyDescent="0.3">
+      <c r="A13" s="110"/>
       <c r="B13" s="46" t="s">
         <v>31</v>
       </c>
@@ -3479,11 +3481,13 @@
       <c r="G13" s="51"/>
       <c r="H13" s="51"/>
       <c r="I13" s="52"/>
-      <c r="J13" s="52"/>
+      <c r="J13" s="52">
+        <v>2</v>
+      </c>
       <c r="K13" s="53"/>
     </row>
-    <row r="14" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="99"/>
+    <row r="14" spans="1:12" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="111"/>
       <c r="B14" s="54" t="s">
         <v>51</v>
       </c>
@@ -3504,11 +3508,13 @@
         <v>1</v>
       </c>
       <c r="I14" s="58"/>
-      <c r="J14" s="58"/>
+      <c r="J14" s="58">
+        <v>3</v>
+      </c>
       <c r="K14" s="59"/>
     </row>
-    <row r="15" spans="1:12" ht="15.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="98" t="s">
+    <row r="15" spans="1:12" ht="15.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="110" t="s">
         <v>52</v>
       </c>
       <c r="B15" s="46" t="s">
@@ -3527,11 +3533,13 @@
         <v>1.5</v>
       </c>
       <c r="I15" s="52"/>
-      <c r="J15" s="52"/>
+      <c r="J15" s="52">
+        <v>1.5</v>
+      </c>
       <c r="K15" s="53"/>
     </row>
-    <row r="16" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="98"/>
+    <row r="16" spans="1:12" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="110"/>
       <c r="B16" s="44" t="s">
         <v>35</v>
       </c>
@@ -3546,11 +3554,15 @@
       <c r="G16" s="33"/>
       <c r="H16" s="33"/>
       <c r="I16" s="34"/>
-      <c r="J16" s="34"/>
-      <c r="K16" s="35"/>
-    </row>
-    <row r="17" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="98"/>
+      <c r="J16" s="34">
+        <v>1.5</v>
+      </c>
+      <c r="K16" s="35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="110"/>
       <c r="B17" s="46" t="s">
         <v>35</v>
       </c>
@@ -3571,11 +3583,15 @@
         <v>1</v>
       </c>
       <c r="I17" s="52"/>
-      <c r="J17" s="52"/>
-      <c r="K17" s="53"/>
-    </row>
-    <row r="18" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="98"/>
+      <c r="J17" s="52">
+        <v>1.5</v>
+      </c>
+      <c r="K17" s="53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="110"/>
       <c r="B18" s="44" t="s">
         <v>35</v>
       </c>
@@ -3594,11 +3610,15 @@
       </c>
       <c r="H18" s="33"/>
       <c r="I18" s="34"/>
-      <c r="J18" s="34"/>
-      <c r="K18" s="35"/>
-    </row>
-    <row r="19" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="98"/>
+      <c r="J18" s="34">
+        <v>1.5</v>
+      </c>
+      <c r="K18" s="35">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="110"/>
       <c r="B19" s="46" t="s">
         <v>35</v>
       </c>
@@ -3617,11 +3637,13 @@
         <v>2</v>
       </c>
       <c r="I19" s="52"/>
-      <c r="J19" s="52"/>
+      <c r="J19" s="52">
+        <v>1.5</v>
+      </c>
       <c r="K19" s="53"/>
     </row>
-    <row r="20" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="98"/>
+    <row r="20" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="110"/>
       <c r="B20" s="44" t="s">
         <v>35</v>
       </c>
@@ -3640,11 +3662,15 @@
         <v>1.5</v>
       </c>
       <c r="I20" s="34"/>
-      <c r="J20" s="34"/>
-      <c r="K20" s="35"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="98"/>
+      <c r="J20" s="34">
+        <v>1.5</v>
+      </c>
+      <c r="K20" s="35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A21" s="110"/>
       <c r="B21" s="46" t="s">
         <v>34</v>
       </c>
@@ -3662,8 +3688,8 @@
       <c r="J21" s="52"/>
       <c r="K21" s="53"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="98"/>
+    <row r="22" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A22" s="110"/>
       <c r="B22" s="44" t="s">
         <v>34</v>
       </c>
@@ -3681,8 +3707,8 @@
       <c r="J22" s="34"/>
       <c r="K22" s="35"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="98"/>
+    <row r="23" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A23" s="110"/>
       <c r="B23" s="46" t="s">
         <v>36</v>
       </c>
@@ -3696,12 +3722,14 @@
       <c r="F23" s="50"/>
       <c r="G23" s="51"/>
       <c r="H23" s="51"/>
-      <c r="I23" s="52"/>
+      <c r="I23" s="52">
+        <v>1</v>
+      </c>
       <c r="J23" s="52"/>
       <c r="K23" s="53"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="98"/>
+    <row r="24" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A24" s="110"/>
       <c r="B24" s="44" t="s">
         <v>36</v>
       </c>
@@ -3721,8 +3749,8 @@
       <c r="J24" s="34"/>
       <c r="K24" s="35"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="98"/>
+    <row r="25" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A25" s="110"/>
       <c r="B25" s="46" t="s">
         <v>36</v>
       </c>
@@ -3740,10 +3768,12 @@
       </c>
       <c r="I25" s="52"/>
       <c r="J25" s="52"/>
-      <c r="K25" s="53"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="98"/>
+      <c r="K25" s="53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A26" s="110"/>
       <c r="B26" s="44" t="s">
         <v>36</v>
       </c>
@@ -3759,12 +3789,14 @@
       <c r="H26" s="33">
         <v>0.5</v>
       </c>
-      <c r="I26" s="34"/>
+      <c r="I26" s="34">
+        <v>0.5</v>
+      </c>
       <c r="J26" s="34"/>
       <c r="K26" s="35"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="98"/>
+    <row r="27" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A27" s="110"/>
       <c r="B27" s="46" t="s">
         <v>36</v>
       </c>
@@ -3786,8 +3818,8 @@
       <c r="J27" s="52"/>
       <c r="K27" s="53"/>
     </row>
-    <row r="28" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="99"/>
+    <row r="28" spans="1:11" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="111"/>
       <c r="B28" s="54" t="s">
         <v>36</v>
       </c>
@@ -3807,10 +3839,12 @@
       </c>
       <c r="I28" s="58"/>
       <c r="J28" s="58"/>
-      <c r="K28" s="59"/>
-    </row>
-    <row r="29" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="98" t="s">
+      <c r="K28" s="59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="15.6" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="110" t="s">
         <v>53</v>
       </c>
       <c r="B29" s="46" t="s">
@@ -3828,10 +3862,12 @@
       <c r="H29" s="51"/>
       <c r="I29" s="52"/>
       <c r="J29" s="52"/>
-      <c r="K29" s="53"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="98"/>
+      <c r="K29" s="53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A30" s="110"/>
       <c r="B30" s="44" t="s">
         <v>37</v>
       </c>
@@ -3851,8 +3887,8 @@
       <c r="J30" s="34"/>
       <c r="K30" s="35"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="98"/>
+    <row r="31" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A31" s="110"/>
       <c r="B31" s="46" t="s">
         <v>37</v>
       </c>
@@ -3872,8 +3908,8 @@
       <c r="J31" s="52"/>
       <c r="K31" s="53"/>
     </row>
-    <row r="32" spans="1:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="98"/>
+    <row r="32" spans="1:11" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="110"/>
       <c r="B32" s="44" t="s">
         <v>37</v>
       </c>
@@ -3893,8 +3929,8 @@
       <c r="J32" s="34"/>
       <c r="K32" s="35"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="98"/>
+    <row r="33" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A33" s="110"/>
       <c r="B33" s="46" t="s">
         <v>37</v>
       </c>
@@ -3914,8 +3950,8 @@
       <c r="J33" s="52"/>
       <c r="K33" s="53"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="98"/>
+    <row r="34" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A34" s="110"/>
       <c r="B34" s="44" t="s">
         <v>37</v>
       </c>
@@ -3933,8 +3969,8 @@
       <c r="J34" s="34"/>
       <c r="K34" s="35"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="98"/>
+    <row r="35" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A35" s="110"/>
       <c r="B35" s="46" t="s">
         <v>38</v>
       </c>
@@ -3950,10 +3986,12 @@
       <c r="H35" s="51"/>
       <c r="I35" s="52"/>
       <c r="J35" s="52"/>
-      <c r="K35" s="53"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="98"/>
+      <c r="K35" s="53">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A36" s="110"/>
       <c r="B36" s="44" t="s">
         <v>38</v>
       </c>
@@ -3969,10 +4007,12 @@
       <c r="H36" s="33"/>
       <c r="I36" s="34"/>
       <c r="J36" s="34"/>
-      <c r="K36" s="35"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="98"/>
+      <c r="K36" s="35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A37" s="110"/>
       <c r="B37" s="46" t="s">
         <v>38</v>
       </c>
@@ -3988,10 +4028,12 @@
       <c r="H37" s="51"/>
       <c r="I37" s="52"/>
       <c r="J37" s="52"/>
-      <c r="K37" s="53"/>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="98"/>
+      <c r="K37" s="53">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A38" s="110"/>
       <c r="B38" s="44" t="s">
         <v>38</v>
       </c>
@@ -4007,10 +4049,12 @@
       <c r="H38" s="33"/>
       <c r="I38" s="34"/>
       <c r="J38" s="34"/>
-      <c r="K38" s="35"/>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="98"/>
+      <c r="K38" s="35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A39" s="110"/>
       <c r="B39" s="46" t="s">
         <v>38</v>
       </c>
@@ -4026,10 +4070,12 @@
       <c r="H39" s="51"/>
       <c r="I39" s="52"/>
       <c r="J39" s="52"/>
-      <c r="K39" s="53"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="98"/>
+      <c r="K39" s="53">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A40" s="110"/>
       <c r="B40" s="44" t="s">
         <v>38</v>
       </c>
@@ -4045,10 +4091,12 @@
       <c r="H40" s="33"/>
       <c r="I40" s="34"/>
       <c r="J40" s="34"/>
-      <c r="K40" s="35"/>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="98"/>
+      <c r="K40" s="35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A41" s="110"/>
       <c r="B41" s="46" t="s">
         <v>39</v>
       </c>
@@ -4066,10 +4114,12 @@
       </c>
       <c r="I41" s="52"/>
       <c r="J41" s="52"/>
-      <c r="K41" s="53"/>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="98"/>
+      <c r="K41" s="53">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A42" s="110"/>
       <c r="B42" s="46" t="s">
         <v>40</v>
       </c>
@@ -4085,10 +4135,12 @@
       <c r="H42" s="51"/>
       <c r="I42" s="52"/>
       <c r="J42" s="52"/>
-      <c r="K42" s="53"/>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="98"/>
+      <c r="K42" s="53">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A43" s="110"/>
       <c r="B43" s="44" t="s">
         <v>40</v>
       </c>
@@ -4104,10 +4156,12 @@
       <c r="H43" s="33"/>
       <c r="I43" s="34"/>
       <c r="J43" s="34"/>
-      <c r="K43" s="35"/>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="98"/>
+      <c r="K43" s="35">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A44" s="110"/>
       <c r="B44" s="46" t="s">
         <v>40</v>
       </c>
@@ -4123,10 +4177,12 @@
       <c r="H44" s="51"/>
       <c r="I44" s="52"/>
       <c r="J44" s="52"/>
-      <c r="K44" s="53"/>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="98"/>
+      <c r="K44" s="53">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A45" s="110"/>
       <c r="B45" s="44" t="s">
         <v>40</v>
       </c>
@@ -4142,10 +4198,12 @@
       <c r="H45" s="33"/>
       <c r="I45" s="34"/>
       <c r="J45" s="34"/>
-      <c r="K45" s="35"/>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="98"/>
+      <c r="K45" s="35">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A46" s="110"/>
       <c r="B46" s="46" t="s">
         <v>40</v>
       </c>
@@ -4161,10 +4219,12 @@
       <c r="H46" s="51"/>
       <c r="I46" s="52"/>
       <c r="J46" s="52"/>
-      <c r="K46" s="53"/>
-    </row>
-    <row r="47" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="99"/>
+      <c r="K46" s="53">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="111"/>
       <c r="B47" s="54" t="s">
         <v>40</v>
       </c>
@@ -4180,10 +4240,12 @@
       <c r="H47" s="57"/>
       <c r="I47" s="58"/>
       <c r="J47" s="58"/>
-      <c r="K47" s="59"/>
-    </row>
-    <row r="48" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="98" t="s">
+      <c r="K47" s="59">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="15.6" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="110" t="s">
         <v>54</v>
       </c>
       <c r="B48" s="46" t="s">
@@ -4199,12 +4261,14 @@
       <c r="F48" s="50"/>
       <c r="G48" s="51"/>
       <c r="H48" s="51"/>
-      <c r="I48" s="52"/>
+      <c r="I48" s="52">
+        <v>0.5</v>
+      </c>
       <c r="J48" s="52"/>
       <c r="K48" s="53"/>
     </row>
-    <row r="49" spans="1:20" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="98"/>
+    <row r="49" spans="1:20" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="110"/>
       <c r="B49" s="44" t="s">
         <v>42</v>
       </c>
@@ -4218,12 +4282,14 @@
       <c r="F49" s="32"/>
       <c r="G49" s="33"/>
       <c r="H49" s="33"/>
-      <c r="I49" s="34"/>
+      <c r="I49" s="34">
+        <v>0.5</v>
+      </c>
       <c r="J49" s="34"/>
       <c r="K49" s="35"/>
     </row>
-    <row r="50" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="99"/>
+    <row r="50" spans="1:20" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="111"/>
       <c r="B50" s="60" t="s">
         <v>43</v>
       </c>
@@ -4237,12 +4303,14 @@
       <c r="F50" s="64"/>
       <c r="G50" s="65"/>
       <c r="H50" s="65"/>
-      <c r="I50" s="66"/>
+      <c r="I50" s="66">
+        <v>0.5</v>
+      </c>
       <c r="J50" s="66"/>
       <c r="K50" s="67"/>
     </row>
-    <row r="51" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="98" t="s">
+    <row r="51" spans="1:20" ht="15.6" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="110" t="s">
         <v>55</v>
       </c>
       <c r="B51" s="44" t="s">
@@ -4264,8 +4332,8 @@
       <c r="J51" s="34"/>
       <c r="K51" s="35"/>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A52" s="98"/>
+    <row r="52" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+      <c r="A52" s="110"/>
       <c r="B52" s="46" t="s">
         <v>45</v>
       </c>
@@ -4283,8 +4351,8 @@
       <c r="J52" s="52"/>
       <c r="K52" s="53"/>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A53" s="98"/>
+    <row r="53" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+      <c r="A53" s="110"/>
       <c r="B53" s="44" t="s">
         <v>46</v>
       </c>
@@ -4302,8 +4370,8 @@
       <c r="J53" s="34"/>
       <c r="K53" s="35"/>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A54" s="98"/>
+    <row r="54" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+      <c r="A54" s="110"/>
       <c r="B54" s="46" t="s">
         <v>57</v>
       </c>
@@ -4321,8 +4389,8 @@
       <c r="J54" s="52"/>
       <c r="K54" s="53"/>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A55" s="98"/>
+    <row r="55" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+      <c r="A55" s="110"/>
       <c r="B55" s="44" t="s">
         <v>57</v>
       </c>
@@ -4340,8 +4408,8 @@
       <c r="J55" s="34"/>
       <c r="K55" s="35"/>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A56" s="98"/>
+    <row r="56" spans="1:20" ht="15" x14ac:dyDescent="0.3">
+      <c r="A56" s="110"/>
       <c r="B56" s="44" t="s">
         <v>57</v>
       </c>
@@ -4359,10 +4427,12 @@
       </c>
       <c r="I56" s="96"/>
       <c r="J56" s="96"/>
-      <c r="K56" s="97"/>
-    </row>
-    <row r="57" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="99"/>
+      <c r="K56" s="97">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:20" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="111"/>
       <c r="B57" s="60" t="s">
         <v>57</v>
       </c>
@@ -4380,8 +4450,8 @@
       <c r="J57" s="66"/>
       <c r="K57" s="67"/>
     </row>
-    <row r="58" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="98" t="s">
+    <row r="58" spans="1:20" ht="15.6" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="110" t="s">
         <v>56</v>
       </c>
       <c r="B58" s="44" t="s">
@@ -4397,12 +4467,14 @@
       <c r="F58" s="32"/>
       <c r="G58" s="33"/>
       <c r="H58" s="33"/>
-      <c r="I58" s="34"/>
+      <c r="I58" s="34">
+        <v>0.5</v>
+      </c>
       <c r="J58" s="34"/>
       <c r="K58" s="35"/>
     </row>
-    <row r="59" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="99"/>
+    <row r="59" spans="1:20" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="111"/>
       <c r="B59" s="60" t="s">
         <v>48</v>
       </c>
@@ -4418,9 +4490,11 @@
       <c r="H59" s="65"/>
       <c r="I59" s="66"/>
       <c r="J59" s="66"/>
-      <c r="K59" s="67"/>
-    </row>
-    <row r="60" spans="1:20" ht="16.149999999999999" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K59" s="67">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:20" ht="16.2" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D60" s="11">
         <f>SUM(D9:D59)</f>
         <v>147</v>
@@ -4443,18 +4517,18 @@
       </c>
       <c r="I60" s="12" t="str">
         <f t="shared" si="0"/>
-        <v>36/147</v>
+        <v>39.5/147</v>
       </c>
       <c r="J60" s="12" t="str">
         <f t="shared" si="0"/>
-        <v>36/147</v>
+        <v>53.5/147</v>
       </c>
       <c r="K60" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>36/147</v>
-      </c>
-    </row>
-    <row r="61" spans="1:20" ht="15" hidden="1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+        <v>83.5/147</v>
+      </c>
+    </row>
+    <row r="61" spans="1:20" ht="15" hidden="1" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="D61" s="1">
         <f>SUM(D9:D59)</f>
         <v>147</v>
@@ -4477,19 +4551,19 @@
       </c>
       <c r="I61" s="1">
         <f>SUM(I9:I59)+H61</f>
-        <v>36</v>
+        <v>39.5</v>
       </c>
       <c r="J61" s="1">
         <f>SUM(J9:J59)+I61</f>
-        <v>36</v>
+        <v>53.5</v>
       </c>
       <c r="K61" s="1">
         <f>SUM(K9:K59)+J61</f>
-        <v>36</v>
+        <v>83.5</v>
       </c>
       <c r="L61" s="1"/>
     </row>
-    <row r="62" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D62" s="1"/>
       <c r="E62" s="1">
         <f>D60</f>
@@ -4521,7 +4595,7 @@
       </c>
       <c r="L62" s="1"/>
     </row>
-    <row r="63" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D63" s="1"/>
       <c r="E63" s="1">
         <v>0</v>
@@ -4531,7 +4605,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="64" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="D64" s="1"/>
       <c r="E64" s="5" t="s">
         <v>14</v>
@@ -4556,7 +4630,7 @@
       <c r="S64" s="4"/>
       <c r="T64" s="4"/>
     </row>
-    <row r="65" spans="4:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="4:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="D65" s="1"/>
       <c r="E65" s="1"/>
       <c r="F65" s="1"/>
@@ -4564,25 +4638,25 @@
       <c r="H65" s="1"/>
       <c r="I65" s="1"/>
     </row>
-    <row r="83" spans="18:18" x14ac:dyDescent="0.25">
+    <row r="83" spans="18:18" x14ac:dyDescent="0.3">
       <c r="R83" s="2" t="s">
         <v>30</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A9:A14"/>
+    <mergeCell ref="A15:A28"/>
+    <mergeCell ref="A29:A47"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="A51:A57"/>
+    <mergeCell ref="A48:A50"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="F7:K7"/>
     <mergeCell ref="B7:B8"/>
-    <mergeCell ref="A9:A14"/>
-    <mergeCell ref="A15:A28"/>
-    <mergeCell ref="A29:A47"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="A51:A57"/>
-    <mergeCell ref="A48:A50"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Number" error="Please Enter Only Numbers. You may use .5 increments. " sqref="D9:D59">
@@ -4619,15 +4693,15 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="78" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="23" t="s">
         <v>58</v>
       </c>
@@ -4635,8 +4709,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:4" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="69" t="s">
         <v>69</v>
       </c>
@@ -4650,7 +4724,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="71" t="s">
         <v>50</v>
       </c>
@@ -4664,7 +4738,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="72" t="s">
         <v>52</v>
       </c>
@@ -4678,7 +4752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="72" t="s">
         <v>53</v>
       </c>
@@ -4692,7 +4766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="72" t="s">
         <v>59</v>
       </c>
@@ -4706,7 +4780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="72" t="s">
         <v>60</v>
       </c>
@@ -4720,7 +4794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="72" t="s">
         <v>61</v>
       </c>
@@ -4734,7 +4808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="72" t="s">
         <v>62</v>
       </c>
@@ -4748,7 +4822,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="72" t="s">
         <v>63</v>
       </c>
@@ -4762,7 +4836,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="72" t="s">
         <v>64</v>
       </c>
@@ -4776,7 +4850,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="72" t="s">
         <v>65</v>
       </c>
@@ -4790,7 +4864,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="72" t="s">
         <v>66</v>
       </c>
@@ -4804,7 +4878,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="72" t="s">
         <v>67</v>
       </c>
@@ -4818,7 +4892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="73" t="s">
         <v>68</v>
       </c>
@@ -4842,582 +4916,566 @@
   <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H21" sqref="H21:I23"/>
+      <selection activeCell="H15" sqref="H15:I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="20.7109375" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" customWidth="1"/>
-    <col min="5" max="6" width="20.7109375" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" customWidth="1"/>
-    <col min="8" max="9" width="20.7109375" customWidth="1"/>
-    <col min="10" max="10" width="8.7109375" customWidth="1"/>
-    <col min="11" max="12" width="20.7109375" customWidth="1"/>
-    <col min="13" max="13" width="8.7109375" customWidth="1"/>
+    <col min="1" max="2" width="21.6640625" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" customWidth="1"/>
+    <col min="5" max="6" width="21.6640625" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" customWidth="1"/>
+    <col min="8" max="9" width="21.6640625" customWidth="1"/>
+    <col min="10" max="10" width="8.6640625" customWidth="1"/>
+    <col min="11" max="12" width="21.6640625" customWidth="1"/>
+    <col min="13" max="13" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="29.25" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="144" t="s">
+    <row r="1" spans="1:13" ht="29.4" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="120" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="145"/>
-      <c r="C1" s="146"/>
+      <c r="B1" s="121"/>
+      <c r="C1" s="122"/>
       <c r="D1" s="81"/>
-      <c r="E1" s="144" t="s">
+      <c r="E1" s="120" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="145"/>
-      <c r="G1" s="145"/>
-      <c r="H1" s="145"/>
-      <c r="I1" s="145"/>
-      <c r="J1" s="145"/>
-      <c r="K1" s="145"/>
-      <c r="L1" s="145"/>
-      <c r="M1" s="146"/>
-    </row>
-    <row r="2" spans="1:13" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="147"/>
-      <c r="B2" s="148"/>
-      <c r="C2" s="149"/>
+      <c r="F1" s="121"/>
+      <c r="G1" s="121"/>
+      <c r="H1" s="121"/>
+      <c r="I1" s="121"/>
+      <c r="J1" s="121"/>
+      <c r="K1" s="121"/>
+      <c r="L1" s="121"/>
+      <c r="M1" s="122"/>
+    </row>
+    <row r="2" spans="1:13" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="123"/>
+      <c r="B2" s="124"/>
+      <c r="C2" s="125"/>
       <c r="D2" s="81"/>
-      <c r="E2" s="147" t="s">
+      <c r="E2" s="123" t="s">
         <v>73</v>
       </c>
-      <c r="F2" s="148"/>
-      <c r="G2" s="149"/>
-      <c r="H2" s="148" t="s">
+      <c r="F2" s="124"/>
+      <c r="G2" s="125"/>
+      <c r="H2" s="124" t="s">
         <v>74</v>
       </c>
-      <c r="I2" s="148"/>
-      <c r="J2" s="149"/>
-      <c r="K2" s="148" t="s">
+      <c r="I2" s="124"/>
+      <c r="J2" s="125"/>
+      <c r="K2" s="124" t="s">
         <v>75</v>
       </c>
-      <c r="L2" s="148"/>
-      <c r="M2" s="149"/>
-    </row>
-    <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="136" t="str">
+      <c r="L2" s="124"/>
+      <c r="M2" s="125"/>
+    </row>
+    <row r="3" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="112" t="str">
         <f>Backlog!A11</f>
         <v>As a User, I want to be able to detect Par. in Chemical Diagram, so I can work with polymers</v>
       </c>
-      <c r="B3" s="137"/>
+      <c r="B3" s="113"/>
       <c r="C3" s="87">
         <f>Backlog!C11</f>
         <v>20</v>
       </c>
-      <c r="E3" s="112"/>
-      <c r="F3" s="113"/>
+      <c r="E3" s="126"/>
+      <c r="F3" s="127"/>
       <c r="G3" s="86"/>
-      <c r="H3" s="118" t="str">
+      <c r="H3" s="126"/>
+      <c r="I3" s="127"/>
+      <c r="J3" s="86"/>
+      <c r="K3" s="132" t="str">
         <f>Backlog!A4</f>
         <v>As a Developer, I need an architectural overview of OSRA’s processing, so I can understand the code base.</v>
       </c>
-      <c r="I3" s="119"/>
-      <c r="J3" s="87">
+      <c r="L3" s="133"/>
+      <c r="M3" s="87">
         <f>Backlog!C4</f>
         <v>13</v>
       </c>
-      <c r="K3" s="112"/>
-      <c r="L3" s="113"/>
-      <c r="M3" s="86"/>
-    </row>
-    <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="138"/>
-      <c r="B4" s="139"/>
+    </row>
+    <row r="4" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="114"/>
+      <c r="B4" s="115"/>
       <c r="C4" s="88" t="str">
         <f>Backlog!B11</f>
         <v>M</v>
       </c>
-      <c r="E4" s="114"/>
-      <c r="F4" s="115"/>
+      <c r="E4" s="128"/>
+      <c r="F4" s="129"/>
       <c r="G4" s="84"/>
-      <c r="H4" s="120"/>
-      <c r="I4" s="121"/>
-      <c r="J4" s="88" t="str">
+      <c r="H4" s="128"/>
+      <c r="I4" s="129"/>
+      <c r="J4" s="84"/>
+      <c r="K4" s="134"/>
+      <c r="L4" s="135"/>
+      <c r="M4" s="88" t="str">
         <f>Backlog!B4</f>
         <v>M</v>
       </c>
-      <c r="K4" s="114"/>
-      <c r="L4" s="115"/>
-      <c r="M4" s="84"/>
-    </row>
-    <row r="5" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="140"/>
-      <c r="B5" s="141"/>
+    </row>
+    <row r="5" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="116"/>
+      <c r="B5" s="117"/>
       <c r="C5" s="89"/>
-      <c r="E5" s="116"/>
-      <c r="F5" s="117"/>
+      <c r="E5" s="130"/>
+      <c r="F5" s="131"/>
       <c r="G5" s="85"/>
-      <c r="H5" s="122"/>
-      <c r="I5" s="123"/>
-      <c r="J5" s="89"/>
-      <c r="K5" s="116"/>
-      <c r="L5" s="117"/>
-      <c r="M5" s="85"/>
-    </row>
-    <row r="6" spans="1:13" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="136" t="str">
+      <c r="H5" s="130"/>
+      <c r="I5" s="131"/>
+      <c r="J5" s="85"/>
+      <c r="K5" s="136"/>
+      <c r="L5" s="137"/>
+      <c r="M5" s="89"/>
+    </row>
+    <row r="6" spans="1:13" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="112" t="str">
         <f>Backlog!A12</f>
         <v>As a User, I want to be able to detect Brackets in Chemical Diagrams, so I can work with polymers</v>
       </c>
-      <c r="B6" s="137"/>
+      <c r="B6" s="113"/>
       <c r="C6" s="87">
         <f>Backlog!C12</f>
         <v>20</v>
       </c>
-      <c r="E6" s="112"/>
-      <c r="F6" s="113"/>
+      <c r="E6" s="126"/>
+      <c r="F6" s="127"/>
       <c r="G6" s="86"/>
-      <c r="H6" s="118" t="str">
+      <c r="H6" s="126"/>
+      <c r="I6" s="127"/>
+      <c r="J6" s="86"/>
+      <c r="K6" s="132" t="str">
         <f>Backlog!A5</f>
         <v>As a Developer, I need to review each aspect of OSRA’s architecture, so I can understand the code base.</v>
       </c>
-      <c r="I6" s="119"/>
-      <c r="J6" s="87">
+      <c r="L6" s="133"/>
+      <c r="M6" s="87">
         <f>Backlog!C5</f>
         <v>20</v>
       </c>
-      <c r="K6" s="112"/>
-      <c r="L6" s="113"/>
-      <c r="M6" s="86"/>
-    </row>
-    <row r="7" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="138"/>
-      <c r="B7" s="139"/>
+    </row>
+    <row r="7" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="114"/>
+      <c r="B7" s="115"/>
       <c r="C7" s="88" t="str">
         <f>Backlog!B12</f>
         <v>S</v>
       </c>
-      <c r="E7" s="114"/>
-      <c r="F7" s="115"/>
+      <c r="E7" s="128"/>
+      <c r="F7" s="129"/>
       <c r="G7" s="84"/>
-      <c r="H7" s="120"/>
-      <c r="I7" s="121"/>
-      <c r="J7" s="88" t="str">
+      <c r="H7" s="128"/>
+      <c r="I7" s="129"/>
+      <c r="J7" s="84"/>
+      <c r="K7" s="134"/>
+      <c r="L7" s="135"/>
+      <c r="M7" s="88" t="str">
         <f>Backlog!B5</f>
         <v>M</v>
       </c>
-      <c r="K7" s="114"/>
-      <c r="L7" s="115"/>
-      <c r="M7" s="84"/>
-    </row>
-    <row r="8" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="140"/>
-      <c r="B8" s="141"/>
+    </row>
+    <row r="8" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="116"/>
+      <c r="B8" s="117"/>
       <c r="C8" s="89"/>
-      <c r="E8" s="116"/>
-      <c r="F8" s="117"/>
+      <c r="E8" s="130"/>
+      <c r="F8" s="131"/>
       <c r="G8" s="85"/>
-      <c r="H8" s="122"/>
-      <c r="I8" s="123"/>
-      <c r="J8" s="89"/>
-      <c r="K8" s="116"/>
-      <c r="L8" s="117"/>
-      <c r="M8" s="85"/>
-    </row>
-    <row r="9" spans="1:13" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="136" t="str">
+      <c r="H8" s="130"/>
+      <c r="I8" s="131"/>
+      <c r="J8" s="85"/>
+      <c r="K8" s="136"/>
+      <c r="L8" s="137"/>
+      <c r="M8" s="89"/>
+    </row>
+    <row r="9" spans="1:13" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="112" t="str">
         <f>Backlog!A13</f>
         <v>As a User, I want to be able to detect subscripts for polymer diagrams, so I can work with polymers</v>
       </c>
-      <c r="B9" s="137"/>
+      <c r="B9" s="113"/>
       <c r="C9" s="87">
         <f>Backlog!C13</f>
         <v>13</v>
       </c>
-      <c r="E9" s="112"/>
-      <c r="F9" s="113"/>
+      <c r="E9" s="126"/>
+      <c r="F9" s="127"/>
       <c r="G9" s="86"/>
-      <c r="H9" s="118" t="str">
+      <c r="H9" s="126"/>
+      <c r="I9" s="127"/>
+      <c r="J9" s="86"/>
+      <c r="K9" s="132" t="str">
         <f>Backlog!A6</f>
         <v>As a Developer, I need to get a basic grasp of O-Chem, so I can better understand use cases.</v>
       </c>
-      <c r="I9" s="119"/>
-      <c r="J9" s="87">
+      <c r="L9" s="133"/>
+      <c r="M9" s="87">
         <f>Backlog!C6</f>
         <v>5</v>
       </c>
-      <c r="K9" s="112"/>
-      <c r="L9" s="113"/>
-      <c r="M9" s="86"/>
-    </row>
-    <row r="10" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="138"/>
-      <c r="B10" s="139"/>
+    </row>
+    <row r="10" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="114"/>
+      <c r="B10" s="115"/>
       <c r="C10" s="88" t="str">
         <f>Backlog!B13</f>
         <v>M</v>
       </c>
-      <c r="E10" s="114"/>
-      <c r="F10" s="115"/>
+      <c r="E10" s="128"/>
+      <c r="F10" s="129"/>
       <c r="G10" s="84"/>
-      <c r="H10" s="120"/>
-      <c r="I10" s="121"/>
-      <c r="J10" s="88" t="str">
+      <c r="H10" s="128"/>
+      <c r="I10" s="129"/>
+      <c r="J10" s="84"/>
+      <c r="K10" s="134"/>
+      <c r="L10" s="135"/>
+      <c r="M10" s="88" t="str">
         <f>Backlog!B6</f>
         <v>M</v>
       </c>
-      <c r="K10" s="114"/>
-      <c r="L10" s="115"/>
-      <c r="M10" s="84"/>
-    </row>
-    <row r="11" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="140"/>
-      <c r="B11" s="141"/>
+    </row>
+    <row r="11" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="116"/>
+      <c r="B11" s="117"/>
       <c r="C11" s="89"/>
-      <c r="E11" s="116"/>
-      <c r="F11" s="117"/>
+      <c r="E11" s="130"/>
+      <c r="F11" s="131"/>
       <c r="G11" s="85"/>
-      <c r="H11" s="122"/>
-      <c r="I11" s="123"/>
-      <c r="J11" s="89"/>
-      <c r="K11" s="116"/>
-      <c r="L11" s="117"/>
-      <c r="M11" s="85"/>
-    </row>
-    <row r="12" spans="1:13" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="136" t="str">
+      <c r="H11" s="130"/>
+      <c r="I11" s="131"/>
+      <c r="J11" s="85"/>
+      <c r="K11" s="136"/>
+      <c r="L11" s="137"/>
+      <c r="M11" s="89"/>
+    </row>
+    <row r="12" spans="1:13" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="112" t="str">
         <f>Backlog!A14</f>
         <v>As a User, I want to be able to detect “R-Notation”, so I can work with polymers</v>
       </c>
-      <c r="B12" s="137"/>
+      <c r="B12" s="113"/>
       <c r="C12" s="87" t="str">
         <f>Backlog!C14</f>
         <v>INF</v>
       </c>
-      <c r="E12" s="118" t="str">
+      <c r="E12" s="126"/>
+      <c r="F12" s="127"/>
+      <c r="G12" s="86"/>
+      <c r="H12" s="126"/>
+      <c r="I12" s="127"/>
+      <c r="J12" s="86"/>
+      <c r="K12" s="132" t="str">
         <f>Backlog!A7</f>
         <v>As a Developer, I need workflow and processes for the github repo, so I can collaborate on code</v>
       </c>
-      <c r="F12" s="119"/>
-      <c r="G12" s="87">
+      <c r="L12" s="133"/>
+      <c r="M12" s="87">
         <f>Backlog!C7</f>
         <v>5</v>
       </c>
-      <c r="H12" s="112"/>
-      <c r="I12" s="113"/>
-      <c r="J12" s="86"/>
-      <c r="K12" s="112"/>
-      <c r="L12" s="113"/>
-      <c r="M12" s="86"/>
-    </row>
-    <row r="13" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="138"/>
-      <c r="B13" s="139"/>
+    </row>
+    <row r="13" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="114"/>
+      <c r="B13" s="115"/>
       <c r="C13" s="88" t="str">
         <f>Backlog!B14</f>
         <v>W</v>
       </c>
-      <c r="E13" s="120"/>
-      <c r="F13" s="121"/>
-      <c r="G13" s="88" t="str">
+      <c r="E13" s="128"/>
+      <c r="F13" s="129"/>
+      <c r="G13" s="84"/>
+      <c r="H13" s="128"/>
+      <c r="I13" s="129"/>
+      <c r="J13" s="84"/>
+      <c r="K13" s="134"/>
+      <c r="L13" s="135"/>
+      <c r="M13" s="88" t="str">
         <f>Backlog!B7</f>
         <v>M</v>
       </c>
-      <c r="H13" s="114"/>
-      <c r="I13" s="115"/>
-      <c r="J13" s="84"/>
-      <c r="K13" s="114"/>
-      <c r="L13" s="115"/>
-      <c r="M13" s="84"/>
-    </row>
-    <row r="14" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="142"/>
-      <c r="B14" s="143"/>
+    </row>
+    <row r="14" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="118"/>
+      <c r="B14" s="119"/>
       <c r="C14" s="90"/>
-      <c r="E14" s="122"/>
-      <c r="F14" s="123"/>
-      <c r="G14" s="89"/>
-      <c r="H14" s="116"/>
-      <c r="I14" s="117"/>
+      <c r="E14" s="130"/>
+      <c r="F14" s="131"/>
+      <c r="G14" s="85"/>
+      <c r="H14" s="130"/>
+      <c r="I14" s="131"/>
       <c r="J14" s="85"/>
-      <c r="K14" s="116"/>
-      <c r="L14" s="117"/>
-      <c r="M14" s="85"/>
-    </row>
-    <row r="15" spans="1:13" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="130"/>
-      <c r="B15" s="131"/>
-      <c r="C15" s="87"/>
-      <c r="E15" s="118" t="str">
+      <c r="K14" s="136"/>
+      <c r="L14" s="137"/>
+      <c r="M14" s="89"/>
+    </row>
+    <row r="15" spans="1:13" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="132" t="str">
+        <f>Backlog!A10</f>
+        <v>As a Developer, I need to understand SMILES notation and .SD file structure, so I can desing the smile data structure.</v>
+      </c>
+      <c r="B15" s="133"/>
+      <c r="C15" s="87">
+        <f>Backlog!C10</f>
+        <v>5</v>
+      </c>
+      <c r="E15" s="126"/>
+      <c r="F15" s="127"/>
+      <c r="G15" s="86"/>
+      <c r="H15" s="132" t="str">
         <f>Backlog!A8</f>
         <v>As a Developer, I need a testing enviroment and test documentation, so I can better contribute to the codebase</v>
       </c>
-      <c r="F15" s="119"/>
-      <c r="G15" s="87">
+      <c r="I15" s="133"/>
+      <c r="J15" s="87">
         <f>Backlog!C8</f>
         <v>20</v>
       </c>
-      <c r="H15" s="112"/>
-      <c r="I15" s="113"/>
-      <c r="J15" s="86"/>
-      <c r="K15" s="112"/>
-      <c r="L15" s="113"/>
+      <c r="K15" s="126"/>
+      <c r="L15" s="127"/>
       <c r="M15" s="86"/>
     </row>
-    <row r="16" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="132"/>
-      <c r="B16" s="133"/>
-      <c r="C16" s="88"/>
-      <c r="E16" s="120"/>
-      <c r="F16" s="121"/>
-      <c r="G16" s="88" t="str">
+    <row r="16" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="134"/>
+      <c r="B16" s="135"/>
+      <c r="C16" s="88" t="str">
+        <f>Backlog!B10</f>
+        <v>M</v>
+      </c>
+      <c r="E16" s="128"/>
+      <c r="F16" s="129"/>
+      <c r="G16" s="84"/>
+      <c r="H16" s="134"/>
+      <c r="I16" s="135"/>
+      <c r="J16" s="88" t="str">
         <f>Backlog!B8</f>
         <v>M</v>
       </c>
-      <c r="H16" s="114"/>
-      <c r="I16" s="115"/>
-      <c r="J16" s="84"/>
-      <c r="K16" s="114"/>
-      <c r="L16" s="115"/>
+      <c r="K16" s="128"/>
+      <c r="L16" s="129"/>
       <c r="M16" s="84"/>
     </row>
-    <row r="17" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="134"/>
-      <c r="B17" s="135"/>
+    <row r="17" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="136"/>
+      <c r="B17" s="137"/>
       <c r="C17" s="89"/>
-      <c r="E17" s="122"/>
-      <c r="F17" s="123"/>
-      <c r="G17" s="89"/>
-      <c r="H17" s="116"/>
-      <c r="I17" s="117"/>
-      <c r="J17" s="85"/>
-      <c r="K17" s="116"/>
-      <c r="L17" s="117"/>
+      <c r="E17" s="130"/>
+      <c r="F17" s="131"/>
+      <c r="G17" s="85"/>
+      <c r="H17" s="136"/>
+      <c r="I17" s="137"/>
+      <c r="J17" s="89"/>
+      <c r="K17" s="130"/>
+      <c r="L17" s="131"/>
       <c r="M17" s="85"/>
     </row>
-    <row r="18" spans="1:13" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="130"/>
-      <c r="B18" s="131"/>
-      <c r="C18" s="87"/>
-      <c r="E18" s="118" t="str">
+    <row r="18" spans="1:13" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="132" t="str">
+        <f>Backlog!A15</f>
+        <v>As a User, I want to have a data structure for encoding polymers in “Smile Notation”, so I can work with polymers</v>
+      </c>
+      <c r="B18" s="133"/>
+      <c r="C18" s="87">
+        <f>Backlog!C15</f>
+        <v>13</v>
+      </c>
+      <c r="E18" s="126"/>
+      <c r="F18" s="127"/>
+      <c r="G18" s="86"/>
+      <c r="H18" s="126"/>
+      <c r="I18" s="127"/>
+      <c r="J18" s="86"/>
+      <c r="K18" s="132" t="str">
         <f>Backlog!A9</f>
         <v>As a Developer, I need to have consolidated documentation from other developers, so I can better contribute to the codebase</v>
       </c>
-      <c r="F18" s="119"/>
-      <c r="G18" s="87">
+      <c r="L18" s="133"/>
+      <c r="M18" s="87">
         <f>Backlog!C9</f>
         <v>13</v>
       </c>
-      <c r="H18" s="112"/>
-      <c r="I18" s="113"/>
-      <c r="J18" s="86"/>
-      <c r="K18" s="112"/>
-      <c r="L18" s="113"/>
-      <c r="M18" s="86"/>
-    </row>
-    <row r="19" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="132"/>
-      <c r="B19" s="133"/>
-      <c r="C19" s="88"/>
-      <c r="E19" s="120"/>
-      <c r="F19" s="121"/>
-      <c r="G19" s="88" t="str">
+    </row>
+    <row r="19" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="134"/>
+      <c r="B19" s="135"/>
+      <c r="C19" s="88" t="str">
+        <f>Backlog!B15</f>
+        <v>M</v>
+      </c>
+      <c r="E19" s="128"/>
+      <c r="F19" s="129"/>
+      <c r="G19" s="84"/>
+      <c r="H19" s="128"/>
+      <c r="I19" s="129"/>
+      <c r="J19" s="84"/>
+      <c r="K19" s="134"/>
+      <c r="L19" s="135"/>
+      <c r="M19" s="88" t="str">
         <f>Backlog!B9</f>
         <v>M</v>
       </c>
-      <c r="H19" s="114"/>
-      <c r="I19" s="115"/>
-      <c r="J19" s="84"/>
-      <c r="K19" s="114"/>
-      <c r="L19" s="115"/>
-      <c r="M19" s="84"/>
-    </row>
-    <row r="20" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="134"/>
-      <c r="B20" s="135"/>
+    </row>
+    <row r="20" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="136"/>
+      <c r="B20" s="137"/>
       <c r="C20" s="89"/>
-      <c r="E20" s="122"/>
-      <c r="F20" s="123"/>
-      <c r="G20" s="89"/>
-      <c r="H20" s="116"/>
-      <c r="I20" s="117"/>
+      <c r="E20" s="130"/>
+      <c r="F20" s="131"/>
+      <c r="G20" s="85"/>
+      <c r="H20" s="130"/>
+      <c r="I20" s="131"/>
       <c r="J20" s="85"/>
-      <c r="K20" s="116"/>
-      <c r="L20" s="117"/>
-      <c r="M20" s="85"/>
-    </row>
-    <row r="21" spans="1:13" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="130"/>
-      <c r="B21" s="131"/>
+      <c r="K20" s="136"/>
+      <c r="L20" s="137"/>
+      <c r="M20" s="89"/>
+    </row>
+    <row r="21" spans="1:13" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="144"/>
+      <c r="B21" s="145"/>
       <c r="C21" s="87"/>
-      <c r="E21" s="118" t="str">
-        <f>Backlog!A10</f>
-        <v>As a Developer, I need to understand SMILES notation and .SD file structure, so I can desing the smile data structure.</v>
-      </c>
-      <c r="F21" s="119"/>
-      <c r="G21" s="87">
-        <f>Backlog!C10</f>
-        <v>5</v>
-      </c>
-      <c r="H21" s="112"/>
-      <c r="I21" s="113"/>
+      <c r="E21" s="126"/>
+      <c r="F21" s="127"/>
+      <c r="G21" s="86"/>
+      <c r="H21" s="126"/>
+      <c r="I21" s="127"/>
       <c r="J21" s="86"/>
-      <c r="K21" s="112"/>
-      <c r="L21" s="113"/>
+      <c r="K21" s="126"/>
+      <c r="L21" s="127"/>
       <c r="M21" s="86"/>
     </row>
-    <row r="22" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="132"/>
-      <c r="B22" s="133"/>
+    <row r="22" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="146"/>
+      <c r="B22" s="147"/>
       <c r="C22" s="88"/>
-      <c r="E22" s="120"/>
-      <c r="F22" s="121"/>
-      <c r="G22" s="88" t="str">
-        <f>Backlog!B10</f>
-        <v>M</v>
-      </c>
-      <c r="H22" s="114"/>
-      <c r="I22" s="115"/>
+      <c r="E22" s="128"/>
+      <c r="F22" s="129"/>
+      <c r="G22" s="84"/>
+      <c r="H22" s="128"/>
+      <c r="I22" s="129"/>
       <c r="J22" s="84"/>
-      <c r="K22" s="114"/>
-      <c r="L22" s="115"/>
+      <c r="K22" s="128"/>
+      <c r="L22" s="129"/>
       <c r="M22" s="84"/>
     </row>
-    <row r="23" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="134"/>
-      <c r="B23" s="135"/>
+    <row r="23" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="148"/>
+      <c r="B23" s="149"/>
       <c r="C23" s="89"/>
-      <c r="E23" s="122"/>
-      <c r="F23" s="123"/>
-      <c r="G23" s="89"/>
-      <c r="H23" s="116"/>
-      <c r="I23" s="117"/>
+      <c r="E23" s="130"/>
+      <c r="F23" s="131"/>
+      <c r="G23" s="85"/>
+      <c r="H23" s="130"/>
+      <c r="I23" s="131"/>
       <c r="J23" s="85"/>
-      <c r="K23" s="116"/>
-      <c r="L23" s="117"/>
+      <c r="K23" s="130"/>
+      <c r="L23" s="131"/>
       <c r="M23" s="85"/>
     </row>
-    <row r="24" spans="1:13" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="130"/>
-      <c r="B24" s="131"/>
+    <row r="24" spans="1:13" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="144"/>
+      <c r="B24" s="145"/>
       <c r="C24" s="87"/>
-      <c r="E24" s="118" t="str">
-        <f>Backlog!A15</f>
-        <v>As a User, I want to have a data structure for encoding polymers in “Smile Notation”, so I can work with polymers</v>
-      </c>
-      <c r="F24" s="119"/>
-      <c r="G24" s="87">
-        <f>Backlog!C15</f>
-        <v>13</v>
-      </c>
-      <c r="H24" s="112"/>
-      <c r="I24" s="113"/>
+      <c r="E24" s="126"/>
+      <c r="F24" s="127"/>
+      <c r="G24" s="86"/>
+      <c r="H24" s="126"/>
+      <c r="I24" s="127"/>
       <c r="J24" s="86"/>
-      <c r="K24" s="112"/>
-      <c r="L24" s="113"/>
+      <c r="K24" s="126"/>
+      <c r="L24" s="127"/>
       <c r="M24" s="86"/>
     </row>
-    <row r="25" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="132"/>
-      <c r="B25" s="133"/>
+    <row r="25" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="146"/>
+      <c r="B25" s="147"/>
       <c r="C25" s="88"/>
-      <c r="E25" s="120"/>
-      <c r="F25" s="121"/>
-      <c r="G25" s="88" t="str">
-        <f>Backlog!B15</f>
-        <v>M</v>
-      </c>
-      <c r="H25" s="114"/>
-      <c r="I25" s="115"/>
+      <c r="E25" s="128"/>
+      <c r="F25" s="129"/>
+      <c r="G25" s="84"/>
+      <c r="H25" s="128"/>
+      <c r="I25" s="129"/>
       <c r="J25" s="84"/>
-      <c r="K25" s="114"/>
-      <c r="L25" s="115"/>
+      <c r="K25" s="128"/>
+      <c r="L25" s="129"/>
       <c r="M25" s="84"/>
     </row>
-    <row r="26" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="134"/>
-      <c r="B26" s="135"/>
+    <row r="26" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="148"/>
+      <c r="B26" s="149"/>
       <c r="C26" s="89"/>
-      <c r="E26" s="122"/>
-      <c r="F26" s="123"/>
-      <c r="G26" s="89"/>
-      <c r="H26" s="116"/>
-      <c r="I26" s="117"/>
+      <c r="E26" s="130"/>
+      <c r="F26" s="131"/>
+      <c r="G26" s="85"/>
+      <c r="H26" s="130"/>
+      <c r="I26" s="131"/>
       <c r="J26" s="85"/>
-      <c r="K26" s="116"/>
-      <c r="L26" s="117"/>
+      <c r="K26" s="130"/>
+      <c r="L26" s="131"/>
       <c r="M26" s="85"/>
     </row>
-    <row r="27" spans="1:13" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="130"/>
-      <c r="B27" s="131"/>
+    <row r="27" spans="1:13" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="144"/>
+      <c r="B27" s="145"/>
       <c r="C27" s="87"/>
-      <c r="E27" s="124"/>
-      <c r="F27" s="125"/>
+      <c r="E27" s="138"/>
+      <c r="F27" s="139"/>
       <c r="G27" s="87"/>
-      <c r="H27" s="112"/>
-      <c r="I27" s="113"/>
+      <c r="H27" s="126"/>
+      <c r="I27" s="127"/>
       <c r="J27" s="86"/>
-      <c r="K27" s="112"/>
-      <c r="L27" s="113"/>
+      <c r="K27" s="126"/>
+      <c r="L27" s="127"/>
       <c r="M27" s="86"/>
     </row>
-    <row r="28" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="132"/>
-      <c r="B28" s="133"/>
+    <row r="28" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="146"/>
+      <c r="B28" s="147"/>
       <c r="C28" s="88"/>
-      <c r="E28" s="126"/>
-      <c r="F28" s="127"/>
+      <c r="E28" s="140"/>
+      <c r="F28" s="141"/>
       <c r="G28" s="88"/>
-      <c r="H28" s="114"/>
-      <c r="I28" s="115"/>
+      <c r="H28" s="128"/>
+      <c r="I28" s="129"/>
       <c r="J28" s="84"/>
-      <c r="K28" s="114"/>
-      <c r="L28" s="115"/>
+      <c r="K28" s="128"/>
+      <c r="L28" s="129"/>
       <c r="M28" s="84"/>
     </row>
-    <row r="29" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="134"/>
-      <c r="B29" s="135"/>
+    <row r="29" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="148"/>
+      <c r="B29" s="149"/>
       <c r="C29" s="89"/>
-      <c r="E29" s="128"/>
-      <c r="F29" s="129"/>
+      <c r="E29" s="142"/>
+      <c r="F29" s="143"/>
       <c r="G29" s="89"/>
-      <c r="H29" s="116"/>
-      <c r="I29" s="117"/>
+      <c r="H29" s="130"/>
+      <c r="I29" s="131"/>
       <c r="J29" s="85"/>
-      <c r="K29" s="116"/>
-      <c r="L29" s="117"/>
+      <c r="K29" s="130"/>
+      <c r="L29" s="131"/>
       <c r="M29" s="85"/>
     </row>
-    <row r="30" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="E1:M1"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="K2:M2"/>
-    <mergeCell ref="A1:C2"/>
-    <mergeCell ref="A3:B5"/>
-    <mergeCell ref="A6:B8"/>
-    <mergeCell ref="A9:B11"/>
-    <mergeCell ref="A12:B14"/>
+    <mergeCell ref="H9:I11"/>
+    <mergeCell ref="H18:I20"/>
     <mergeCell ref="A15:B17"/>
-    <mergeCell ref="H3:I5"/>
-    <mergeCell ref="H6:I8"/>
-    <mergeCell ref="H9:I11"/>
-    <mergeCell ref="E12:F14"/>
+    <mergeCell ref="A18:B20"/>
     <mergeCell ref="E15:F17"/>
-    <mergeCell ref="E3:F5"/>
-    <mergeCell ref="E6:F8"/>
-    <mergeCell ref="E9:F11"/>
-    <mergeCell ref="H12:I14"/>
-    <mergeCell ref="H15:I17"/>
     <mergeCell ref="E18:F20"/>
-    <mergeCell ref="E21:F23"/>
-    <mergeCell ref="E24:F26"/>
-    <mergeCell ref="E27:F29"/>
     <mergeCell ref="A21:B23"/>
     <mergeCell ref="A24:B26"/>
     <mergeCell ref="A27:B29"/>
-    <mergeCell ref="A18:B20"/>
-    <mergeCell ref="K3:L5"/>
+    <mergeCell ref="E21:F23"/>
+    <mergeCell ref="E24:F26"/>
     <mergeCell ref="K6:L8"/>
     <mergeCell ref="K9:L11"/>
     <mergeCell ref="K12:L14"/>
+    <mergeCell ref="H15:I17"/>
+    <mergeCell ref="E27:F29"/>
     <mergeCell ref="K15:L17"/>
     <mergeCell ref="K18:L20"/>
     <mergeCell ref="K21:L23"/>
@@ -5426,7 +5484,23 @@
     <mergeCell ref="H21:I23"/>
     <mergeCell ref="H24:I26"/>
     <mergeCell ref="H27:I29"/>
-    <mergeCell ref="H18:I20"/>
+    <mergeCell ref="H6:I8"/>
+    <mergeCell ref="A3:B5"/>
+    <mergeCell ref="A6:B8"/>
+    <mergeCell ref="A9:B11"/>
+    <mergeCell ref="A12:B14"/>
+    <mergeCell ref="E1:M1"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="A1:C2"/>
+    <mergeCell ref="E3:F5"/>
+    <mergeCell ref="E6:F8"/>
+    <mergeCell ref="E9:F11"/>
+    <mergeCell ref="H12:I14"/>
+    <mergeCell ref="E12:F14"/>
+    <mergeCell ref="H3:I5"/>
+    <mergeCell ref="K3:L5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5440,20 +5514,20 @@
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9.109375" style="2"/>
     <col min="2" max="2" width="11" style="2" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26" style="2" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.7109375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="31.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="2"/>
+    <col min="6" max="6" width="20.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.6640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="31.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
         <v>11</v>
@@ -5474,7 +5548,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>22</v>
       </c>
@@ -5499,7 +5573,7 @@
         <v>24.5</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
@@ -5524,7 +5598,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>23</v>
       </c>
@@ -5549,7 +5623,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
         <v>24</v>
       </c>
@@ -5574,7 +5648,7 @@
         <v>24.5</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
         <v>49</v>
       </c>
@@ -5599,7 +5673,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
         <v>25</v>
       </c>
@@ -5624,7 +5698,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
         <v>80</v>
       </c>
@@ -5662,18 +5736,18 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="150">
         <v>41557</v>
       </c>
@@ -5681,7 +5755,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="150"/>
       <c r="B3" t="s">
         <v>20</v>

</xml_diff>